<commit_message>
Results before standard error correction
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E58228-55C6-4394-BC4D-029FAD4E46A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D39096F-81EC-4D32-AA68-A23FD1930012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" firstSheet="9" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -1582,6 +1582,15 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1630,6 +1639,9 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1638,18 +1650,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2252,14 +2252,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2361,14 +2361,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2497,20 +2497,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2825,11 +2825,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2844,13 +2844,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="102"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="10">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2994,11 +2994,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="88" t="s">
+      <c r="G24" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="91"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -3024,13 +3024,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="102"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="11">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -3207,20 +3207,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="102" t="s">
+      <c r="A37" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="102"/>
-      <c r="C37" s="102"/>
-      <c r="D37" s="102"/>
-      <c r="E37" s="102"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="88" t="s">
+      <c r="G38" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3512,20 +3512,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="102" t="s">
+      <c r="A51" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="102"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="102"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="88" t="s">
+      <c r="G52" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="88"/>
-      <c r="I52" s="88"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3849,15 +3849,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
   <dimension ref="A2:S73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="Q60" sqref="Q60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57:F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3959,52 +3961,52 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="108" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="K9" s="105" t="s">
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="K9" s="109" t="s">
         <v>308</v>
       </c>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="K11" s="103" t="s">
+      <c r="B11" s="106"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
+      <c r="K11" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="103"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="106"/>
+      <c r="N11" s="106"/>
+      <c r="O11" s="106"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
     </row>
     <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4228,28 +4230,28 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="K21" s="103" t="s">
+      <c r="B21" s="106"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="106"/>
+      <c r="K21" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="L21" s="103"/>
-      <c r="M21" s="103"/>
-      <c r="N21" s="103"/>
-      <c r="O21" s="103"/>
-      <c r="P21" s="103"/>
-      <c r="Q21" s="103"/>
-      <c r="R21" s="103"/>
-      <c r="S21" s="103"/>
+      <c r="L21" s="106"/>
+      <c r="M21" s="106"/>
+      <c r="N21" s="106"/>
+      <c r="O21" s="106"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="106"/>
+      <c r="R21" s="106"/>
+      <c r="S21" s="106"/>
     </row>
     <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4472,32 +4474,32 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A31" s="103" t="s">
+    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="K31" s="103" t="s">
+      <c r="B31" s="106"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="106"/>
+      <c r="K31" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L31" s="106"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="106"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="106"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="10" t="s">
         <v>8</v>
       </c>
@@ -4529,7 +4531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>93</v>
       </c>
@@ -4561,7 +4563,7 @@
         <v>3.93416384989266E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="D35" s="73" t="str">
         <f>+IF(M37=0,"",M37)</f>
         <v/>
@@ -4595,7 +4597,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>9</v>
       </c>
@@ -4627,7 +4629,7 @@
         <v>1.7184485249948499E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
       <c r="F37" s="73"/>
@@ -4649,7 +4651,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>10</v>
       </c>
@@ -4681,7 +4683,7 @@
         <v>1.8797507235916999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="19"/>
       <c r="D39" s="74" t="str">
         <f>+IF(M39=0,"",M39)</f>
@@ -4717,29 +4719,30 @@
         <v/>
       </c>
     </row>
+    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="42" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="B42" s="103"/>
-      <c r="C42" s="103"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="103"/>
-      <c r="H42" s="103"/>
-      <c r="I42" s="103"/>
-      <c r="K42" s="103" t="s">
+      <c r="B42" s="106"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="106"/>
+      <c r="E42" s="106"/>
+      <c r="F42" s="106"/>
+      <c r="G42" s="106"/>
+      <c r="H42" s="106"/>
+      <c r="I42" s="106"/>
+      <c r="K42" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="L42" s="103"/>
-      <c r="M42" s="103"/>
-      <c r="N42" s="103"/>
-      <c r="O42" s="103"/>
-      <c r="P42" s="103"/>
-      <c r="Q42" s="103"/>
-      <c r="R42" s="103"/>
-      <c r="S42" s="103"/>
+      <c r="L42" s="106"/>
+      <c r="M42" s="106"/>
+      <c r="N42" s="106"/>
+      <c r="O42" s="106"/>
+      <c r="P42" s="106"/>
+      <c r="Q42" s="106"/>
+      <c r="R42" s="106"/>
+      <c r="S42" s="106"/>
     </row>
     <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4778,65 +4781,53 @@
       <c r="C45" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="72">
-        <v>0.248864529029136</v>
-      </c>
-      <c r="E45" s="72">
-        <v>0.32228532721911801</v>
-      </c>
-      <c r="F45" s="72">
-        <v>0.97851029268032497</v>
-      </c>
-      <c r="G45" s="72">
-        <v>2.3466172100891899E-2</v>
+      <c r="D45" s="88">
+        <v>0.31018306322082201</v>
+      </c>
+      <c r="E45" s="88">
+        <v>0.35740478053101099</v>
+      </c>
+      <c r="F45" s="88">
+        <v>0.68349910741717101</v>
+      </c>
+      <c r="G45" s="88">
+        <v>0.30750371060827297</v>
       </c>
       <c r="M45" t="s">
         <v>93</v>
       </c>
       <c r="N45" s="72">
-        <v>0.248864529029136</v>
+        <v>0.26365085003831501</v>
       </c>
       <c r="O45" s="72">
-        <v>0.32228532721911801</v>
+        <v>0.35840187547189101</v>
       </c>
       <c r="P45" s="72">
-        <v>0.97851029268032497</v>
+        <v>0.91009860384202801</v>
       </c>
       <c r="Q45" s="72">
-        <v>2.3466172100891899E-2</v>
+        <v>4.5583593355867702E-2</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D46" s="73" t="str">
-        <f>+IF(M48=0,"",M48)</f>
-        <v/>
-      </c>
-      <c r="E46" s="73" t="str">
-        <f t="shared" ref="E46" si="35">+IF(N48=0,"",N48)</f>
-        <v/>
-      </c>
-      <c r="F46" s="73" t="str">
-        <f t="shared" ref="F46" si="36">+IF(O48=0,"",O48)</f>
-        <v/>
-      </c>
-      <c r="G46" s="73" t="str">
-        <f t="shared" ref="G46" si="37">+IF(P48=0,"",P48)</f>
-        <v/>
-      </c>
+      <c r="D46" s="73"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
       <c r="N46" s="73" t="str">
         <f>+IF(W48=0,"",W48)</f>
         <v/>
       </c>
       <c r="O46" s="73" t="str">
-        <f t="shared" ref="O46" si="38">+IF(X48=0,"",X48)</f>
+        <f t="shared" ref="O46" si="35">+IF(X48=0,"",X48)</f>
         <v/>
       </c>
       <c r="P46" s="73" t="str">
-        <f t="shared" ref="P46" si="39">+IF(Y48=0,"",Y48)</f>
+        <f t="shared" ref="P46" si="36">+IF(Y48=0,"",Y48)</f>
         <v/>
       </c>
       <c r="Q46" s="73" t="str">
-        <f t="shared" ref="Q46" si="40">+IF(Z48=0,"",Z48)</f>
+        <f t="shared" ref="Q46" si="37">+IF(Z48=0,"",Z48)</f>
         <v/>
       </c>
     </row>
@@ -4844,39 +4835,39 @@
       <c r="C47" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="72">
-        <v>0.248864529029136</v>
-      </c>
-      <c r="E47" s="72">
-        <v>0.39624966997320399</v>
-      </c>
-      <c r="F47" s="72">
-        <v>0.57629676926180995</v>
-      </c>
-      <c r="G47" s="72">
-        <v>0.36210216060626799</v>
+      <c r="D47" s="89">
+        <v>0.31018306322082201</v>
+      </c>
+      <c r="E47" s="89">
+        <v>0.65682449572895196</v>
+      </c>
+      <c r="F47" s="89">
+        <v>0.49183973592229402</v>
+      </c>
+      <c r="G47" s="89">
+        <v>0.130974449674474</v>
       </c>
       <c r="M47" t="s">
         <v>9</v>
       </c>
       <c r="N47" s="72">
-        <v>0.248864529029136</v>
+        <v>0.26365085003831501</v>
       </c>
       <c r="O47" s="72">
-        <v>0.39624966997320399</v>
+        <v>0.58197736367224095</v>
       </c>
       <c r="P47" s="72">
-        <v>0.57629676926180995</v>
+        <v>0.68182507979061102</v>
       </c>
       <c r="Q47" s="72">
-        <v>0.36210216060626799</v>
+        <v>2.22521472100402E-2</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="73"/>
+      <c r="D48" s="89"/>
+      <c r="E48" s="89"/>
+      <c r="F48" s="89"/>
+      <c r="G48" s="89"/>
       <c r="N48" s="73"/>
       <c r="O48" s="73"/>
       <c r="P48" s="73"/>
@@ -4886,50 +4877,50 @@
       <c r="C49" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="72">
-        <v>0.248864529029136</v>
-      </c>
-      <c r="E49" s="72">
-        <v>1.0367633249888799</v>
-      </c>
-      <c r="F49" s="72">
-        <v>0.18895009228718701</v>
-      </c>
-      <c r="G49" s="72">
-        <v>2.1497210541473601E-2</v>
+      <c r="D49" s="89">
+        <v>0.31018306322082201</v>
+      </c>
+      <c r="E49" s="89">
+        <v>0.63946528642015499</v>
+      </c>
+      <c r="F49" s="89">
+        <v>0.35108000833060798</v>
+      </c>
+      <c r="G49" s="89">
+        <v>0.28430945844107902</v>
       </c>
       <c r="M49" t="s">
         <v>10</v>
       </c>
       <c r="N49" s="72">
-        <v>0.248864529029136</v>
+        <v>0.26365085003831501</v>
       </c>
       <c r="O49" s="72">
-        <v>1.0367633249888799</v>
+        <v>0.76446346549597</v>
       </c>
       <c r="P49" s="72">
-        <v>0.18895009228718701</v>
+        <v>0.45459858775955098</v>
       </c>
       <c r="Q49" s="72">
-        <v>2.1497210541473601E-2</v>
+        <v>2.5977753128474598E-2</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="19"/>
-      <c r="D50" s="74" t="str">
+      <c r="D50" s="90" t="str">
         <f>+IF(M50=0,"",M50)</f>
         <v/>
       </c>
-      <c r="E50" s="74" t="str">
-        <f t="shared" ref="E50" si="41">+IF(N50=0,"",N50)</f>
+      <c r="E50" s="90" t="str">
+        <f t="shared" ref="E50" si="38">+IF(N50=0,"",N50)</f>
         <v/>
       </c>
-      <c r="F50" s="74" t="str">
-        <f t="shared" ref="F50" si="42">+IF(O50=0,"",O50)</f>
+      <c r="F50" s="90" t="str">
+        <f t="shared" ref="F50" si="39">+IF(O50=0,"",O50)</f>
         <v/>
       </c>
-      <c r="G50" s="74" t="str">
-        <f t="shared" ref="G50" si="43">+IF(P50=0,"",P50)</f>
+      <c r="G50" s="90" t="str">
+        <f t="shared" ref="G50" si="40">+IF(P50=0,"",P50)</f>
         <v/>
       </c>
       <c r="M50" s="19"/>
@@ -4938,15 +4929,15 @@
         <v/>
       </c>
       <c r="O50" s="74" t="str">
-        <f t="shared" ref="O50" si="44">+IF(X50=0,"",X50)</f>
+        <f t="shared" ref="O50" si="41">+IF(X50=0,"",X50)</f>
         <v/>
       </c>
       <c r="P50" s="74" t="str">
-        <f t="shared" ref="P50" si="45">+IF(Y50=0,"",Y50)</f>
+        <f t="shared" ref="P50" si="42">+IF(Y50=0,"",Y50)</f>
         <v/>
       </c>
       <c r="Q50" s="74" t="str">
-        <f t="shared" ref="Q50" si="46">+IF(Z50=0,"",Z50)</f>
+        <f t="shared" ref="Q50" si="43">+IF(Z50=0,"",Z50)</f>
         <v/>
       </c>
     </row>
@@ -4974,28 +4965,28 @@
       <c r="S53" s="107"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A55" s="103" t="s">
+      <c r="A55" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="B55" s="103"/>
-      <c r="C55" s="103"/>
-      <c r="D55" s="103"/>
-      <c r="E55" s="103"/>
-      <c r="F55" s="103"/>
-      <c r="G55" s="103"/>
-      <c r="H55" s="103"/>
-      <c r="I55" s="103"/>
-      <c r="K55" s="103" t="s">
+      <c r="B55" s="106"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="106"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="106"/>
+      <c r="I55" s="106"/>
+      <c r="K55" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="L55" s="103"/>
-      <c r="M55" s="103"/>
-      <c r="N55" s="103"/>
-      <c r="O55" s="103"/>
-      <c r="P55" s="103"/>
-      <c r="Q55" s="103"/>
-      <c r="R55" s="103"/>
-      <c r="S55" s="103"/>
+      <c r="L55" s="106"/>
+      <c r="M55" s="106"/>
+      <c r="N55" s="106"/>
+      <c r="O55" s="106"/>
+      <c r="P55" s="106"/>
+      <c r="Q55" s="106"/>
+      <c r="R55" s="106"/>
+      <c r="S55" s="106"/>
     </row>
     <row r="56" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5011,7 +5002,7 @@
       <c r="F57" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="108"/>
+      <c r="G57" s="54"/>
       <c r="M57" s="10" t="s">
         <v>8</v>
       </c>
@@ -5024,75 +5015,111 @@
       <c r="P57" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="Q57" s="108"/>
+      <c r="Q57" s="54"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="72"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
-      <c r="G58" s="109"/>
+      <c r="D58" s="72">
+        <v>0.30019250319507501</v>
+      </c>
+      <c r="E58" s="72">
+        <v>0.314020637070486</v>
+      </c>
+      <c r="F58" s="72">
+        <v>0.81723706035450705</v>
+      </c>
+      <c r="G58" s="72"/>
       <c r="M58" t="s">
         <v>93</v>
       </c>
-      <c r="N58" s="72"/>
-      <c r="O58" s="72"/>
-      <c r="P58" s="72"/>
-      <c r="Q58" s="109"/>
+      <c r="N58" s="72">
+        <v>0.25982265214567601</v>
+      </c>
+      <c r="O58" s="72">
+        <v>0.44355437941932302</v>
+      </c>
+      <c r="P58" s="72">
+        <v>0.86019078842469998</v>
+      </c>
+      <c r="Q58" s="72"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D59" s="73"/>
       <c r="E59" s="73"/>
       <c r="F59" s="73"/>
-      <c r="G59" s="110"/>
+      <c r="G59" s="73"/>
       <c r="N59" s="73"/>
       <c r="O59" s="73"/>
       <c r="P59" s="73"/>
-      <c r="Q59" s="110"/>
+      <c r="Q59" s="73"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="72"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
-      <c r="G60" s="109"/>
+      <c r="D60" s="72">
+        <v>0.30019250319507501</v>
+      </c>
+      <c r="E60" s="72">
+        <v>0.68025733523300802</v>
+      </c>
+      <c r="F60" s="72">
+        <v>0.50537378426994894</v>
+      </c>
+      <c r="G60" s="72"/>
       <c r="M60" t="s">
         <v>9</v>
       </c>
-      <c r="N60" s="72"/>
-      <c r="O60" s="72"/>
-      <c r="P60" s="72"/>
-      <c r="Q60" s="109"/>
+      <c r="N60" s="72">
+        <v>0.25982265214567601</v>
+      </c>
+      <c r="O60" s="72">
+        <v>0.59428100860744704</v>
+      </c>
+      <c r="P60" s="72">
+        <v>0.68938812324867804</v>
+      </c>
+      <c r="Q60" s="72"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D61" s="73"/>
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
-      <c r="G61" s="110"/>
+      <c r="G61" s="73"/>
       <c r="N61" s="73"/>
       <c r="O61" s="73"/>
       <c r="P61" s="73"/>
-      <c r="Q61" s="110"/>
+      <c r="Q61" s="73"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="72"/>
-      <c r="E62" s="72"/>
-      <c r="F62" s="72"/>
-      <c r="G62" s="109"/>
+      <c r="D62" s="72">
+        <v>0.30019250319507501</v>
+      </c>
+      <c r="E62" s="72">
+        <v>0.854752473086689</v>
+      </c>
+      <c r="F62" s="72">
+        <v>0.30630121932812399</v>
+      </c>
+      <c r="G62" s="72"/>
       <c r="M62" t="s">
         <v>10</v>
       </c>
-      <c r="N62" s="72"/>
-      <c r="O62" s="72"/>
-      <c r="P62" s="72"/>
-      <c r="Q62" s="109"/>
+      <c r="N62" s="72">
+        <v>0.25982265214567601</v>
+      </c>
+      <c r="O62" s="72">
+        <v>0.71413163907242005</v>
+      </c>
+      <c r="P62" s="72">
+        <v>0.530642372299581</v>
+      </c>
+      <c r="Q62" s="72"/>
     </row>
     <row r="63" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="19"/>
@@ -5101,15 +5128,15 @@
         <v/>
       </c>
       <c r="E63" s="74" t="str">
-        <f t="shared" ref="E63" si="47">+IF(N63=0,"",N63)</f>
+        <f t="shared" ref="E63" si="44">+IF(N63=0,"",N63)</f>
         <v/>
       </c>
       <c r="F63" s="74" t="str">
-        <f t="shared" ref="F63" si="48">+IF(O63=0,"",O63)</f>
+        <f t="shared" ref="F63" si="45">+IF(O63=0,"",O63)</f>
         <v/>
       </c>
-      <c r="G63" s="110" t="str">
-        <f t="shared" ref="G63" si="49">+IF(P63=0,"",P63)</f>
+      <c r="G63" s="73" t="str">
+        <f t="shared" ref="G63" si="46">+IF(P63=0,"",P63)</f>
         <v/>
       </c>
       <c r="M63" s="19"/>
@@ -5118,38 +5145,38 @@
         <v/>
       </c>
       <c r="O63" s="74" t="str">
-        <f t="shared" ref="O63" si="50">+IF(X63=0,"",X63)</f>
+        <f t="shared" ref="O63" si="47">+IF(X63=0,"",X63)</f>
         <v/>
       </c>
       <c r="P63" s="74" t="str">
-        <f t="shared" ref="P63" si="51">+IF(Y63=0,"",Y63)</f>
+        <f t="shared" ref="P63" si="48">+IF(Y63=0,"",Y63)</f>
         <v/>
       </c>
-      <c r="Q63" s="110"/>
+      <c r="Q63" s="73"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A65" s="103" t="s">
+      <c r="A65" s="106" t="s">
         <v>315</v>
       </c>
-      <c r="B65" s="103"/>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="103"/>
-      <c r="F65" s="103"/>
-      <c r="G65" s="103"/>
-      <c r="H65" s="103"/>
-      <c r="I65" s="103"/>
-      <c r="K65" s="103" t="s">
+      <c r="B65" s="106"/>
+      <c r="C65" s="106"/>
+      <c r="D65" s="106"/>
+      <c r="E65" s="106"/>
+      <c r="F65" s="106"/>
+      <c r="G65" s="106"/>
+      <c r="H65" s="106"/>
+      <c r="I65" s="106"/>
+      <c r="K65" s="106" t="s">
         <v>315</v>
       </c>
-      <c r="L65" s="103"/>
-      <c r="M65" s="103"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="103"/>
-      <c r="P65" s="103"/>
-      <c r="Q65" s="103"/>
-      <c r="R65" s="103"/>
-      <c r="S65" s="103"/>
+      <c r="L65" s="106"/>
+      <c r="M65" s="106"/>
+      <c r="N65" s="106"/>
+      <c r="O65" s="106"/>
+      <c r="P65" s="106"/>
+      <c r="Q65" s="106"/>
+      <c r="R65" s="106"/>
+      <c r="S65" s="106"/>
     </row>
     <row r="66" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5165,7 +5192,7 @@
       <c r="F67" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G67" s="108"/>
+      <c r="G67" s="54"/>
       <c r="M67" s="10" t="s">
         <v>8</v>
       </c>
@@ -5176,77 +5203,113 @@
         <v>4</v>
       </c>
       <c r="P67" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q67" s="108"/>
+        <v>6</v>
+      </c>
+      <c r="Q67" s="54"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C68" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="72"/>
-      <c r="E68" s="72"/>
-      <c r="F68" s="72"/>
-      <c r="G68" s="109"/>
+      <c r="D68" s="72">
+        <v>0.35282665388944701</v>
+      </c>
+      <c r="E68" s="72">
+        <v>1.0265099595049401</v>
+      </c>
+      <c r="F68" s="72">
+        <v>1.8237993964939098E-2</v>
+      </c>
+      <c r="G68" s="72"/>
       <c r="M68" t="s">
         <v>93</v>
       </c>
-      <c r="N68" s="72"/>
-      <c r="O68" s="72"/>
-      <c r="P68" s="72"/>
-      <c r="Q68" s="109"/>
+      <c r="N68" s="72">
+        <v>0.33588666548609197</v>
+      </c>
+      <c r="O68" s="72">
+        <v>0.96897252741872897</v>
+      </c>
+      <c r="P68" s="72">
+        <v>0.31851032815477898</v>
+      </c>
+      <c r="Q68" s="72"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D69" s="73"/>
       <c r="E69" s="73"/>
       <c r="F69" s="73"/>
-      <c r="G69" s="110"/>
+      <c r="G69" s="73"/>
       <c r="N69" s="73"/>
       <c r="O69" s="73"/>
       <c r="P69" s="73"/>
-      <c r="Q69" s="110"/>
+      <c r="Q69" s="73"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C70" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="72"/>
-      <c r="E70" s="72"/>
-      <c r="F70" s="72"/>
-      <c r="G70" s="109"/>
+      <c r="D70" s="72">
+        <v>0.35282665388944701</v>
+      </c>
+      <c r="E70" s="72">
+        <v>1.0726708688684199</v>
+      </c>
+      <c r="F70" s="72">
+        <v>0.140178425773164</v>
+      </c>
+      <c r="G70" s="72"/>
       <c r="M70" t="s">
         <v>9</v>
       </c>
-      <c r="N70" s="72"/>
-      <c r="O70" s="72"/>
-      <c r="P70" s="72"/>
-      <c r="Q70" s="109"/>
+      <c r="N70" s="72">
+        <v>0.33588666548609197</v>
+      </c>
+      <c r="O70" s="72">
+        <v>1.12449589196761</v>
+      </c>
+      <c r="P70" s="72">
+        <v>0.110727984920165</v>
+      </c>
+      <c r="Q70" s="72"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.35">
       <c r="D71" s="73"/>
       <c r="E71" s="73"/>
       <c r="F71" s="73"/>
-      <c r="G71" s="110"/>
+      <c r="G71" s="73"/>
       <c r="N71" s="73"/>
       <c r="O71" s="73"/>
       <c r="P71" s="73"/>
-      <c r="Q71" s="110"/>
+      <c r="Q71" s="73"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.35">
       <c r="C72" t="s">
         <v>10</v>
       </c>
-      <c r="D72" s="72"/>
-      <c r="E72" s="72"/>
-      <c r="F72" s="72"/>
-      <c r="G72" s="109"/>
+      <c r="D72" s="72">
+        <v>0.35282665388944701</v>
+      </c>
+      <c r="E72" s="72">
+        <v>0.91491379472894196</v>
+      </c>
+      <c r="F72" s="72">
+        <v>0.249567365316156</v>
+      </c>
+      <c r="G72" s="72"/>
       <c r="M72" t="s">
         <v>10</v>
       </c>
-      <c r="N72" s="72"/>
-      <c r="O72" s="72"/>
-      <c r="P72" s="72"/>
-      <c r="Q72" s="109"/>
+      <c r="N72" s="72">
+        <v>0.33588666548609197</v>
+      </c>
+      <c r="O72" s="72">
+        <v>1.0725714298648099</v>
+      </c>
+      <c r="P72" s="72">
+        <v>0.125346807934135</v>
+      </c>
+      <c r="Q72" s="72"/>
     </row>
     <row r="73" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C73" s="19"/>
@@ -5255,15 +5318,15 @@
         <v/>
       </c>
       <c r="E73" s="74" t="str">
-        <f t="shared" ref="E73" si="52">+IF(N73=0,"",N73)</f>
+        <f t="shared" ref="E73" si="49">+IF(N73=0,"",N73)</f>
         <v/>
       </c>
       <c r="F73" s="74" t="str">
-        <f t="shared" ref="F73" si="53">+IF(O73=0,"",O73)</f>
+        <f t="shared" ref="F73" si="50">+IF(O73=0,"",O73)</f>
         <v/>
       </c>
-      <c r="G73" s="110" t="str">
-        <f t="shared" ref="G73" si="54">+IF(P73=0,"",P73)</f>
+      <c r="G73" s="73" t="str">
+        <f t="shared" ref="G73" si="51">+IF(P73=0,"",P73)</f>
         <v/>
       </c>
       <c r="M73" s="19"/>
@@ -5272,24 +5335,17 @@
         <v/>
       </c>
       <c r="O73" s="74" t="str">
-        <f t="shared" ref="O73" si="55">+IF(X73=0,"",X73)</f>
+        <f t="shared" ref="O73" si="52">+IF(X73=0,"",X73)</f>
         <v/>
       </c>
       <c r="P73" s="74" t="str">
-        <f t="shared" ref="P73" si="56">+IF(Y73=0,"",Y73)</f>
+        <f t="shared" ref="P73" si="53">+IF(Y73=0,"",Y73)</f>
         <v/>
       </c>
-      <c r="Q73" s="110"/>
+      <c r="Q73" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K65:S65"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="K42:S42"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="K55:S55"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="K31:S31"/>
     <mergeCell ref="A9:I9"/>
@@ -5298,6 +5354,13 @@
     <mergeCell ref="K11:S11"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="K21:S21"/>
+    <mergeCell ref="K65:S65"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="K42:S42"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K55:S55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5330,20 +5393,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -5664,10 +5727,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="H10" s="106" t="s">
+      <c r="H10" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="I10" s="106"/>
+      <c r="I10" s="110"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5678,8 +5741,8 @@
       <c r="F11" s="28">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
       <c r="L11" s="35"/>
       <c r="N11" s="35"/>
     </row>
@@ -5696,8 +5759,8 @@
       <c r="F12" s="28">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="106"/>
-      <c r="I12" s="106"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5713,8 +5776,8 @@
       <c r="F13" s="49">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="106"/>
-      <c r="I13" s="106"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
       <c r="L13" s="35"/>
       <c r="N13" s="35"/>
     </row>
@@ -5882,8 +5945,8 @@
       <c r="E33" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="92"/>
-      <c r="I33" s="92"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="95"/>
       <c r="L33" s="35"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5891,10 +5954,10 @@
         <v>290</v>
       </c>
       <c r="O34" s="79"/>
-      <c r="P34" s="92" t="s">
+      <c r="P34" s="95" t="s">
         <v>280</v>
       </c>
-      <c r="Q34" s="92"/>
+      <c r="Q34" s="95"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
@@ -6024,10 +6087,10 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="F40" s="28"/>
-      <c r="H40" s="106" t="s">
+      <c r="H40" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="I40" s="106"/>
+      <c r="I40" s="110"/>
       <c r="K40" t="s">
         <v>288</v>
       </c>
@@ -6045,8 +6108,8 @@
       <c r="F41" s="28">
         <v>1.365048</v>
       </c>
-      <c r="H41" s="106"/>
-      <c r="I41" s="106"/>
+      <c r="H41" s="110"/>
+      <c r="I41" s="110"/>
       <c r="K41" t="s">
         <v>289</v>
       </c>
@@ -6059,8 +6122,8 @@
       <c r="F42" s="28">
         <v>-0.3439432</v>
       </c>
-      <c r="H42" s="106"/>
-      <c r="I42" s="106"/>
+      <c r="H42" s="110"/>
+      <c r="I42" s="110"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="35">
@@ -6075,8 +6138,8 @@
       <c r="F43" s="49">
         <v>13.51919</v>
       </c>
-      <c r="H43" s="106"/>
-      <c r="I43" s="106"/>
+      <c r="H43" s="110"/>
+      <c r="I43" s="110"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44" s="35">
@@ -7495,12 +7558,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -8064,66 +8127,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="92" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="N1" s="89" t="s">
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="T1" s="89" t="s">
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="T1" s="92" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="N2" s="90" t="s">
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="N2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="T2" s="90" t="s">
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="T2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="91"/>
-      <c r="V2" s="91"/>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -9158,10 +9221,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="92"/>
+      <c r="C2" s="95"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -9696,13 +9759,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9816,12 +9879,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -10120,12 +10183,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -10459,13 +10522,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -10703,13 +10766,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="96" t="s">
+      <c r="A21" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="96"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -10737,13 +10800,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="95" t="s">
+      <c r="A25" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -11005,13 +11068,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="96"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="99"/>
+      <c r="E43" s="99"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -11379,36 +11442,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -11927,35 +11990,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101" t="s">
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="98" t="s">
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99" t="s">
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Corrected standard errors two equation model
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B136050B-BAF2-416E-9042-833EAEBF769F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483539F5-DF25-4370-BBBD-12BCE5DE4CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" firstSheet="9" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -1417,7 +1417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1641,6 +1641,16 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2477,8 +2487,8 @@
   </sheetPr>
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3838,10 +3848,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
-  <dimension ref="A2:S73"/>
+  <dimension ref="A2:W73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44:Q50"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S50" sqref="S50:V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3853,7 +3863,7 @@
     <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="87" t="s">
         <v>306</v>
       </c>
@@ -3866,7 +3876,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="86">
         <v>0</v>
       </c>
@@ -3895,7 +3905,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="86">
         <v>1</v>
       </c>
@@ -3918,7 +3928,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="86">
         <v>2</v>
       </c>
@@ -3935,7 +3945,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="86">
         <v>3</v>
       </c>
@@ -3949,7 +3959,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="104" t="s">
         <v>307</v>
       </c>
@@ -3973,7 +3983,7 @@
       <c r="R9" s="105"/>
       <c r="S9" s="105"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="103" t="s">
         <v>309</v>
       </c>
@@ -3997,8 +4007,8 @@
       <c r="R11" s="103"/>
       <c r="S11" s="103"/>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="10" t="s">
         <v>8</v>
       </c>
@@ -4030,7 +4040,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>93</v>
       </c>
@@ -4062,41 +4072,53 @@
         <v>5.6152933972934901E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D15" s="73" t="str">
         <f>+IF(M17=0,"",M17)</f>
         <v/>
       </c>
-      <c r="E15" s="73" t="str">
+      <c r="E15" s="73">
         <f t="shared" ref="E15:G15" si="0">+IF(N17=0,"",N17)</f>
-        <v/>
-      </c>
-      <c r="F15" s="73" t="str">
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="F15" s="73">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G15" s="73" t="str">
+        <v>-7.3981842197322401E-2</v>
+      </c>
+      <c r="G15" s="73">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N15" s="73" t="str">
-        <f>+IF(W17=0,"",W17)</f>
-        <v/>
-      </c>
-      <c r="O15" s="73" t="str">
-        <f t="shared" ref="O15:Q15" si="1">+IF(X17=0,"",X17)</f>
-        <v/>
-      </c>
-      <c r="P15" s="73" t="str">
+        <v>-7.6118564642824793E-2</v>
+      </c>
+      <c r="N15" s="73">
+        <f>-S15</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O15" s="73">
+        <f t="shared" ref="O15:Q15" si="1">-T15</f>
+        <v>-6.2921396769632695E-2</v>
+      </c>
+      <c r="P15" s="73">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q15" s="73" t="str">
+        <v>-6.4583503348773899E-2</v>
+      </c>
+      <c r="Q15" s="73">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-7.67475876248436E-2</v>
+      </c>
+      <c r="S15">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T15">
+        <v>6.2921396769632695E-2</v>
+      </c>
+      <c r="U15">
+        <v>6.4583503348773899E-2</v>
+      </c>
+      <c r="V15">
+        <v>7.67475876248436E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -4128,29 +4150,41 @@
         <v>2.7066505491686099E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D17" s="73"/>
       <c r="E17" s="73"/>
       <c r="F17" s="73"/>
       <c r="G17" s="73"/>
-      <c r="N17" s="73" t="str">
-        <f>+IF(W18=0,"",W18)</f>
-        <v/>
-      </c>
-      <c r="O17" s="73" t="str">
-        <f t="shared" ref="O17:Q17" si="2">+IF(X18=0,"",X18)</f>
-        <v/>
-      </c>
-      <c r="P17" s="73" t="str">
+      <c r="N17" s="73">
+        <f>-S17</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O17" s="73">
+        <f t="shared" ref="O17:Q17" si="2">-T17</f>
+        <v>-7.3981842197322401E-2</v>
+      </c>
+      <c r="P17" s="73">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q17" s="73" t="str">
+        <v>-7.6118564642824793E-2</v>
+      </c>
+      <c r="Q17" s="73">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-7.8421126834552699E-2</v>
+      </c>
+      <c r="S17">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T17">
+        <v>7.3981842197322401E-2</v>
+      </c>
+      <c r="U17">
+        <v>7.6118564642824793E-2</v>
+      </c>
+      <c r="V17">
+        <v>7.8421126834552699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>10</v>
       </c>
@@ -4182,43 +4216,55 @@
         <v>3.1046085155378701E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="19"/>
       <c r="D19" s="74" t="str">
         <f>+IF(M19=0,"",M19)</f>
         <v/>
       </c>
-      <c r="E19" s="74" t="str">
+      <c r="E19" s="74">
         <f t="shared" ref="E19:G19" si="3">+IF(N19=0,"",N19)</f>
-        <v/>
-      </c>
-      <c r="F19" s="74" t="str">
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="F19" s="74">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G19" s="74" t="str">
+        <v>-6.4554005463114295E-2</v>
+      </c>
+      <c r="G19" s="74">
         <f t="shared" si="3"/>
-        <v/>
+        <v>-6.6745927637415006E-2</v>
       </c>
       <c r="M19" s="19"/>
-      <c r="N19" s="74" t="str">
-        <f>+IF(W19=0,"",W19)</f>
-        <v/>
-      </c>
-      <c r="O19" s="74" t="str">
-        <f t="shared" ref="O19:Q19" si="4">+IF(X19=0,"",X19)</f>
-        <v/>
-      </c>
-      <c r="P19" s="74" t="str">
+      <c r="N19" s="74">
+        <f>-S19</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O19" s="74">
+        <f t="shared" ref="O19:Q19" si="4">-T19</f>
+        <v>-6.4554005463114295E-2</v>
+      </c>
+      <c r="P19" s="74">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q19" s="74" t="str">
+        <v>-6.6745927637415006E-2</v>
+      </c>
+      <c r="Q19" s="74">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-5.3873187988552002E-3</v>
+      </c>
+      <c r="S19">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T19">
+        <v>6.4554005463114295E-2</v>
+      </c>
+      <c r="U19">
+        <v>6.6745927637415006E-2</v>
+      </c>
+      <c r="V19">
+        <v>5.3873187988552002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="103" t="s">
         <v>310</v>
       </c>
@@ -4242,8 +4288,8 @@
       <c r="R21" s="103"/>
       <c r="S21" s="103"/>
     </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="10" t="s">
         <v>8</v>
       </c>
@@ -4275,7 +4321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>93</v>
       </c>
@@ -4307,41 +4353,53 @@
         <v>4.5710077252419302E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D25" s="73" t="str">
         <f>+IF(M27=0,"",M27)</f>
         <v/>
       </c>
-      <c r="E25" s="73" t="str">
+      <c r="E25" s="73">
         <f t="shared" ref="E25" si="5">+IF(N27=0,"",N27)</f>
-        <v/>
-      </c>
-      <c r="F25" s="73" t="str">
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="F25" s="73">
         <f t="shared" ref="F25" si="6">+IF(O27=0,"",O27)</f>
-        <v/>
-      </c>
-      <c r="G25" s="73" t="str">
+        <v>-7.4363070184416902E-2</v>
+      </c>
+      <c r="G25" s="73">
         <f t="shared" ref="G25" si="7">+IF(P27=0,"",P27)</f>
-        <v/>
-      </c>
-      <c r="N25" s="73" t="str">
-        <f>+IF(W27=0,"",W27)</f>
-        <v/>
-      </c>
-      <c r="O25" s="73" t="str">
-        <f t="shared" ref="O25" si="8">+IF(X27=0,"",X27)</f>
-        <v/>
-      </c>
-      <c r="P25" s="73" t="str">
-        <f t="shared" ref="P25" si="9">+IF(Y27=0,"",Y27)</f>
-        <v/>
-      </c>
-      <c r="Q25" s="73" t="str">
-        <f t="shared" ref="Q25" si="10">+IF(Z27=0,"",Z27)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-7.3014723185476305E-2</v>
+      </c>
+      <c r="N25" s="73">
+        <f>-S25</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O25" s="73">
+        <f t="shared" ref="O25:Q25" si="8">-T25</f>
+        <v>-6.2705340586680203E-2</v>
+      </c>
+      <c r="P25" s="73">
+        <f t="shared" si="8"/>
+        <v>-6.0532147295976703E-2</v>
+      </c>
+      <c r="Q25" s="73">
+        <f t="shared" si="8"/>
+        <v>-6.79552860893851E-2</v>
+      </c>
+      <c r="S25">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T25">
+        <v>6.2705340586680203E-2</v>
+      </c>
+      <c r="U25">
+        <v>6.0532147295976703E-2</v>
+      </c>
+      <c r="V25">
+        <v>6.79552860893851E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>9</v>
       </c>
@@ -4373,29 +4431,41 @@
         <v>2.2043508532012299E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="D27" s="73"/>
       <c r="E27" s="73"/>
       <c r="F27" s="73"/>
       <c r="G27" s="73"/>
-      <c r="N27" s="73" t="str">
-        <f>+IF(W28=0,"",W28)</f>
-        <v/>
-      </c>
-      <c r="O27" s="73" t="str">
-        <f t="shared" ref="O27" si="11">+IF(X28=0,"",X28)</f>
-        <v/>
-      </c>
-      <c r="P27" s="73" t="str">
-        <f t="shared" ref="P27" si="12">+IF(Y28=0,"",Y28)</f>
-        <v/>
-      </c>
-      <c r="Q27" s="73" t="str">
-        <f t="shared" ref="Q27" si="13">+IF(Z28=0,"",Z28)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N27" s="73">
+        <f>-S27</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O27" s="73">
+        <f t="shared" ref="O27:Q27" si="9">-T27</f>
+        <v>-7.4363070184416902E-2</v>
+      </c>
+      <c r="P27" s="73">
+        <f t="shared" si="9"/>
+        <v>-7.3014723185476305E-2</v>
+      </c>
+      <c r="Q27" s="73">
+        <f t="shared" si="9"/>
+        <v>-7.1882201893921804E-2</v>
+      </c>
+      <c r="S27">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T27">
+        <v>7.4363070184416902E-2</v>
+      </c>
+      <c r="U27">
+        <v>7.3014723185476305E-2</v>
+      </c>
+      <c r="V27">
+        <v>7.1882201893921804E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>10</v>
       </c>
@@ -4427,43 +4497,55 @@
         <v>2.6102828154984499E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="19"/>
       <c r="D29" s="74" t="str">
         <f>+IF(M29=0,"",M29)</f>
         <v/>
       </c>
-      <c r="E29" s="74" t="str">
-        <f t="shared" ref="E29" si="14">+IF(N29=0,"",N29)</f>
-        <v/>
-      </c>
-      <c r="F29" s="74" t="str">
-        <f t="shared" ref="F29" si="15">+IF(O29=0,"",O29)</f>
-        <v/>
-      </c>
-      <c r="G29" s="74" t="str">
-        <f t="shared" ref="G29" si="16">+IF(P29=0,"",P29)</f>
-        <v/>
+      <c r="E29" s="74">
+        <f t="shared" ref="E29" si="10">+IF(N29=0,"",N29)</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="F29" s="74">
+        <f t="shared" ref="F29" si="11">+IF(O29=0,"",O29)</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="G29" s="74">
+        <f t="shared" ref="G29" si="12">+IF(P29=0,"",P29)</f>
+        <v>-6.6984637221420507E-2</v>
       </c>
       <c r="M29" s="19"/>
-      <c r="N29" s="74" t="str">
-        <f>+IF(W29=0,"",W29)</f>
-        <v/>
-      </c>
-      <c r="O29" s="74" t="str">
-        <f t="shared" ref="O29" si="17">+IF(X29=0,"",X29)</f>
-        <v/>
-      </c>
-      <c r="P29" s="74" t="str">
-        <f t="shared" ref="P29" si="18">+IF(Y29=0,"",Y29)</f>
-        <v/>
-      </c>
-      <c r="Q29" s="74" t="str">
-        <f t="shared" ref="Q29" si="19">+IF(Z29=0,"",Z29)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N29" s="74">
+        <f>-S29</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O29" s="74">
+        <f t="shared" ref="O29:Q29" si="13">-T29</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="P29" s="74">
+        <f t="shared" si="13"/>
+        <v>-6.6984637221420507E-2</v>
+      </c>
+      <c r="Q29" s="74">
+        <f t="shared" si="13"/>
+        <v>-5.8788297464031098E-3</v>
+      </c>
+      <c r="S29">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T29">
+        <v>6.4688998413530194E-2</v>
+      </c>
+      <c r="U29">
+        <v>6.6984637221420507E-2</v>
+      </c>
+      <c r="V29">
+        <v>5.8788297464031098E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="103" t="s">
         <v>311</v>
       </c>
@@ -4487,8 +4569,8 @@
       <c r="R31" s="103"/>
       <c r="S31" s="103"/>
     </row>
-    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="33" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="10" t="s">
         <v>8</v>
       </c>
@@ -4520,7 +4602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>93</v>
       </c>
@@ -4552,41 +4634,53 @@
         <v>3.93416384989266E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D35" s="73" t="str">
         <f>+IF(M37=0,"",M37)</f>
         <v/>
       </c>
-      <c r="E35" s="73" t="str">
-        <f t="shared" ref="E35" si="20">+IF(N37=0,"",N37)</f>
-        <v/>
-      </c>
-      <c r="F35" s="73" t="str">
-        <f t="shared" ref="F35" si="21">+IF(O37=0,"",O37)</f>
-        <v/>
-      </c>
-      <c r="G35" s="73" t="str">
-        <f t="shared" ref="G35" si="22">+IF(P37=0,"",P37)</f>
-        <v/>
-      </c>
-      <c r="N35" s="73" t="str">
-        <f>+IF(W37=0,"",W37)</f>
-        <v/>
-      </c>
-      <c r="O35" s="73" t="str">
-        <f t="shared" ref="O35" si="23">+IF(X37=0,"",X37)</f>
-        <v/>
-      </c>
-      <c r="P35" s="73" t="str">
-        <f t="shared" ref="P35" si="24">+IF(Y37=0,"",Y37)</f>
-        <v/>
-      </c>
-      <c r="Q35" s="73" t="str">
-        <f t="shared" ref="Q35" si="25">+IF(Z37=0,"",Z37)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="E35" s="73">
+        <f t="shared" ref="E35" si="14">+IF(N37=0,"",N37)</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" ref="F35" si="15">+IF(O37=0,"",O37)</f>
+        <v>-7.7697154041311306E-2</v>
+      </c>
+      <c r="G35" s="73">
+        <f t="shared" ref="G35" si="16">+IF(P37=0,"",P37)</f>
+        <v>-7.0698211707042102E-2</v>
+      </c>
+      <c r="N35" s="73">
+        <f>-S35</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O35" s="73">
+        <f t="shared" ref="O35:P35" si="17">-T35</f>
+        <v>-6.6121303110595497E-2</v>
+      </c>
+      <c r="P35" s="73">
+        <f t="shared" si="17"/>
+        <v>-5.7998508062290899E-2</v>
+      </c>
+      <c r="Q35" s="73">
+        <f>-V35</f>
+        <v>-6.5015545691961399E-2</v>
+      </c>
+      <c r="S35">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T35">
+        <v>6.6121303110595497E-2</v>
+      </c>
+      <c r="U35">
+        <v>5.7998508062290899E-2</v>
+      </c>
+      <c r="V35">
+        <v>6.5015545691961399E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>9</v>
       </c>
@@ -4618,29 +4712,41 @@
         <v>1.7184485249948499E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D37" s="73"/>
       <c r="E37" s="73"/>
       <c r="F37" s="73"/>
       <c r="G37" s="73"/>
-      <c r="N37" s="73" t="str">
-        <f>+IF(W38=0,"",W38)</f>
-        <v/>
-      </c>
-      <c r="O37" s="73" t="str">
-        <f t="shared" ref="O37" si="26">+IF(X38=0,"",X38)</f>
-        <v/>
-      </c>
-      <c r="P37" s="73" t="str">
-        <f t="shared" ref="P37" si="27">+IF(Y38=0,"",Y38)</f>
-        <v/>
-      </c>
-      <c r="Q37" s="73" t="str">
-        <f t="shared" ref="Q37" si="28">+IF(Z38=0,"",Z38)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N37" s="73">
+        <f>-S37</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O37" s="73">
+        <f t="shared" ref="O37:Q37" si="18">-T37</f>
+        <v>-7.7697154041311306E-2</v>
+      </c>
+      <c r="P37" s="73">
+        <f t="shared" si="18"/>
+        <v>-7.0698211707042102E-2</v>
+      </c>
+      <c r="Q37" s="73">
+        <f t="shared" si="18"/>
+        <v>-7.1608927235836894E-2</v>
+      </c>
+      <c r="S37">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T37">
+        <v>7.7697154041311306E-2</v>
+      </c>
+      <c r="U37">
+        <v>7.0698211707042102E-2</v>
+      </c>
+      <c r="V37">
+        <v>7.1608927235836894E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>10</v>
       </c>
@@ -4672,43 +4778,55 @@
         <v>1.8797507235916999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="19"/>
       <c r="D39" s="74" t="str">
         <f>+IF(M39=0,"",M39)</f>
         <v/>
       </c>
-      <c r="E39" s="74" t="str">
-        <f t="shared" ref="E39" si="29">+IF(N39=0,"",N39)</f>
-        <v/>
-      </c>
-      <c r="F39" s="74" t="str">
-        <f t="shared" ref="F39" si="30">+IF(O39=0,"",O39)</f>
-        <v/>
-      </c>
-      <c r="G39" s="74" t="str">
-        <f t="shared" ref="G39" si="31">+IF(P39=0,"",P39)</f>
-        <v/>
+      <c r="E39" s="74">
+        <f t="shared" ref="E39" si="19">+IF(N39=0,"",N39)</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="F39" s="74">
+        <f t="shared" ref="F39" si="20">+IF(O39=0,"",O39)</f>
+        <v>-6.4659214976102206E-2</v>
+      </c>
+      <c r="G39" s="74">
+        <f t="shared" ref="G39" si="21">+IF(P39=0,"",P39)</f>
+        <v>-6.7086317193334202E-2</v>
       </c>
       <c r="M39" s="19"/>
-      <c r="N39" s="74" t="str">
-        <f>+IF(W39=0,"",W39)</f>
-        <v/>
-      </c>
-      <c r="O39" s="74" t="str">
-        <f t="shared" ref="O39" si="32">+IF(X39=0,"",X39)</f>
-        <v/>
-      </c>
-      <c r="P39" s="74" t="str">
-        <f t="shared" ref="P39" si="33">+IF(Y39=0,"",Y39)</f>
-        <v/>
-      </c>
-      <c r="Q39" s="74" t="str">
-        <f t="shared" ref="Q39" si="34">+IF(Z39=0,"",Z39)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N39" s="74">
+        <f>-S39</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O39" s="74">
+        <f t="shared" ref="O39:Q39" si="22">-T39</f>
+        <v>-6.4659214976102206E-2</v>
+      </c>
+      <c r="P39" s="74">
+        <f t="shared" si="22"/>
+        <v>-6.7086317193334202E-2</v>
+      </c>
+      <c r="Q39" s="74">
+        <f t="shared" si="22"/>
+        <v>-6.7079383018708201E-3</v>
+      </c>
+      <c r="S39">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T39">
+        <v>6.4659214976102206E-2</v>
+      </c>
+      <c r="U39">
+        <v>6.7086317193334202E-2</v>
+      </c>
+      <c r="V39">
+        <v>6.7079383018708201E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="103" t="s">
         <v>312</v>
       </c>
@@ -4732,8 +4850,8 @@
       <c r="R42" s="103"/>
       <c r="S42" s="103"/>
     </row>
-    <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C44" s="10" t="s">
         <v>8</v>
       </c>
@@ -4765,7 +4883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>93</v>
       </c>
@@ -4788,30 +4906,50 @@
       <c r="Q45" s="72">
         <v>4.5583593355867702E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R45" s="110"/>
+      <c r="S45" s="110"/>
+      <c r="T45" s="110"/>
+      <c r="U45" s="110"/>
+      <c r="V45" s="110"/>
+      <c r="W45" s="110"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
       <c r="F46" s="73"/>
       <c r="G46" s="73"/>
-      <c r="N46" s="73" t="str">
-        <f>+IF(W48=0,"",W48)</f>
-        <v/>
-      </c>
-      <c r="O46" s="73" t="str">
-        <f t="shared" ref="O46" si="35">+IF(X48=0,"",X48)</f>
-        <v/>
-      </c>
-      <c r="P46" s="73" t="str">
-        <f t="shared" ref="P46" si="36">+IF(Y48=0,"",Y48)</f>
-        <v/>
-      </c>
-      <c r="Q46" s="73" t="str">
-        <f t="shared" ref="Q46" si="37">+IF(Z48=0,"",Z48)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N46" s="108">
+        <f>-S46</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O46" s="108">
+        <f t="shared" ref="O46:Q46" si="23">-T46</f>
+        <v>-6.2705340586680203E-2</v>
+      </c>
+      <c r="P46" s="108">
+        <f t="shared" si="23"/>
+        <v>-6.0532147295976703E-2</v>
+      </c>
+      <c r="Q46" s="108">
+        <f t="shared" si="23"/>
+        <v>-6.79552860893851E-2</v>
+      </c>
+      <c r="R46" s="110"/>
+      <c r="S46" s="108">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T46" s="108">
+        <v>6.2705340586680203E-2</v>
+      </c>
+      <c r="U46" s="108">
+        <v>6.0532147295976703E-2</v>
+      </c>
+      <c r="V46" s="108">
+        <v>6.79552860893851E-2</v>
+      </c>
+      <c r="W46" s="110"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>9</v>
       </c>
@@ -4834,18 +4972,50 @@
       <c r="Q47" s="72">
         <v>2.22521472100402E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R47" s="110"/>
+      <c r="S47" s="110"/>
+      <c r="T47" s="110"/>
+      <c r="U47" s="110"/>
+      <c r="V47" s="110"/>
+      <c r="W47" s="110"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D48" s="73"/>
       <c r="E48" s="73"/>
       <c r="F48" s="73"/>
       <c r="G48" s="73"/>
-      <c r="N48" s="73"/>
-      <c r="O48" s="73"/>
-      <c r="P48" s="73"/>
-      <c r="Q48" s="73"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N48" s="108">
+        <f>-S48</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O48" s="108">
+        <f t="shared" ref="O48:Q48" si="24">-T48</f>
+        <v>-7.4363070184416902E-2</v>
+      </c>
+      <c r="P48" s="108">
+        <f t="shared" si="24"/>
+        <v>-7.3014723185476305E-2</v>
+      </c>
+      <c r="Q48" s="108">
+        <f t="shared" si="24"/>
+        <v>-7.1882201893921804E-2</v>
+      </c>
+      <c r="R48" s="110"/>
+      <c r="S48" s="108">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T48" s="108">
+        <v>7.4363070184416902E-2</v>
+      </c>
+      <c r="U48" s="108">
+        <v>7.3014723185476305E-2</v>
+      </c>
+      <c r="V48" s="108">
+        <v>7.1882201893921804E-2</v>
+      </c>
+      <c r="W48" s="110"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
         <v>10</v>
       </c>
@@ -4868,44 +5038,64 @@
       <c r="Q49" s="72">
         <v>2.5977753128474598E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R49" s="110"/>
+      <c r="S49" s="110"/>
+      <c r="T49" s="110"/>
+      <c r="U49" s="110"/>
+      <c r="V49" s="110"/>
+      <c r="W49" s="110"/>
+    </row>
+    <row r="50" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="19"/>
       <c r="D50" s="74" t="str">
         <f>+IF(M50=0,"",M50)</f>
         <v/>
       </c>
-      <c r="E50" s="74" t="str">
-        <f t="shared" ref="E50" si="38">+IF(N50=0,"",N50)</f>
-        <v/>
-      </c>
-      <c r="F50" s="74" t="str">
-        <f t="shared" ref="F50" si="39">+IF(O50=0,"",O50)</f>
-        <v/>
-      </c>
-      <c r="G50" s="74" t="str">
-        <f t="shared" ref="G50" si="40">+IF(P50=0,"",P50)</f>
-        <v/>
+      <c r="E50" s="74">
+        <f t="shared" ref="E50" si="25">+IF(N50=0,"",N50)</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="F50" s="74">
+        <f t="shared" ref="F50" si="26">+IF(O50=0,"",O50)</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="G50" s="74">
+        <f t="shared" ref="G50" si="27">+IF(P50=0,"",P50)</f>
+        <v>-6.6984637221420507E-2</v>
       </c>
       <c r="M50" s="19"/>
-      <c r="N50" s="74" t="str">
-        <f>+IF(W50=0,"",W50)</f>
-        <v/>
-      </c>
-      <c r="O50" s="74" t="str">
-        <f t="shared" ref="O50" si="41">+IF(X50=0,"",X50)</f>
-        <v/>
-      </c>
-      <c r="P50" s="74" t="str">
-        <f t="shared" ref="P50" si="42">+IF(Y50=0,"",Y50)</f>
-        <v/>
-      </c>
-      <c r="Q50" s="74" t="str">
-        <f t="shared" ref="Q50" si="43">+IF(Z50=0,"",Z50)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N50" s="109">
+        <f>-S50</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O50" s="109">
+        <f t="shared" ref="O50:Q50" si="28">-T50</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="P50" s="109">
+        <f t="shared" si="28"/>
+        <v>-6.6984637221420507E-2</v>
+      </c>
+      <c r="Q50" s="109">
+        <f t="shared" si="28"/>
+        <v>-5.8788297464031098E-3</v>
+      </c>
+      <c r="R50" s="110"/>
+      <c r="S50" s="111">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T50" s="111">
+        <v>6.4688998413530194E-2</v>
+      </c>
+      <c r="U50" s="111">
+        <v>6.6984637221420507E-2</v>
+      </c>
+      <c r="V50" s="111">
+        <v>5.8788297464031098E-3</v>
+      </c>
+      <c r="W50" s="110"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="106" t="s">
         <v>313</v>
       </c>
@@ -4928,7 +5118,7 @@
       <c r="R53" s="106"/>
       <c r="S53" s="106"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="103" t="s">
         <v>314</v>
       </c>
@@ -4952,8 +5142,8 @@
       <c r="R55" s="103"/>
       <c r="S55" s="103"/>
     </row>
-    <row r="56" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="10" t="s">
         <v>8</v>
       </c>
@@ -4981,7 +5171,7 @@
       </c>
       <c r="Q57" s="54"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>93</v>
       </c>
@@ -5003,7 +5193,7 @@
       </c>
       <c r="Q58" s="72"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D59" s="73"/>
       <c r="E59" s="73"/>
       <c r="F59" s="73"/>
@@ -5013,7 +5203,7 @@
       <c r="P59" s="73"/>
       <c r="Q59" s="73"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>9</v>
       </c>
@@ -5035,7 +5225,7 @@
       </c>
       <c r="Q60" s="72"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D61" s="73"/>
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
@@ -5045,7 +5235,7 @@
       <c r="P61" s="73"/>
       <c r="Q61" s="73"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
         <v>10</v>
       </c>
@@ -5067,22 +5257,22 @@
       </c>
       <c r="Q62" s="72"/>
     </row>
-    <row r="63" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="19"/>
       <c r="D63" s="74" t="str">
         <f>+IF(M63=0,"",M63)</f>
         <v/>
       </c>
       <c r="E63" s="74" t="str">
-        <f t="shared" ref="E63" si="44">+IF(N63=0,"",N63)</f>
+        <f t="shared" ref="E63" si="29">+IF(N63=0,"",N63)</f>
         <v/>
       </c>
       <c r="F63" s="74" t="str">
-        <f t="shared" ref="F63" si="45">+IF(O63=0,"",O63)</f>
+        <f t="shared" ref="F63" si="30">+IF(O63=0,"",O63)</f>
         <v/>
       </c>
       <c r="G63" s="73" t="str">
-        <f t="shared" ref="G63" si="46">+IF(P63=0,"",P63)</f>
+        <f t="shared" ref="G63" si="31">+IF(P63=0,"",P63)</f>
         <v/>
       </c>
       <c r="M63" s="19"/>
@@ -5091,11 +5281,11 @@
         <v/>
       </c>
       <c r="O63" s="74" t="str">
-        <f t="shared" ref="O63" si="47">+IF(X63=0,"",X63)</f>
+        <f t="shared" ref="O63" si="32">+IF(X63=0,"",X63)</f>
         <v/>
       </c>
       <c r="P63" s="74" t="str">
-        <f t="shared" ref="P63" si="48">+IF(Y63=0,"",Y63)</f>
+        <f t="shared" ref="P63" si="33">+IF(Y63=0,"",Y63)</f>
         <v/>
       </c>
       <c r="Q63" s="73"/>
@@ -5246,15 +5436,15 @@
         <v/>
       </c>
       <c r="E73" s="74" t="str">
-        <f t="shared" ref="E73" si="49">+IF(N73=0,"",N73)</f>
+        <f t="shared" ref="E73" si="34">+IF(N73=0,"",N73)</f>
         <v/>
       </c>
       <c r="F73" s="74" t="str">
-        <f t="shared" ref="F73" si="50">+IF(O73=0,"",O73)</f>
+        <f t="shared" ref="F73" si="35">+IF(O73=0,"",O73)</f>
         <v/>
       </c>
       <c r="G73" s="73" t="str">
-        <f t="shared" ref="G73" si="51">+IF(P73=0,"",P73)</f>
+        <f t="shared" ref="G73" si="36">+IF(P73=0,"",P73)</f>
         <v/>
       </c>
       <c r="M73" s="19"/>
@@ -5263,11 +5453,11 @@
         <v/>
       </c>
       <c r="O73" s="74" t="str">
-        <f t="shared" ref="O73" si="52">+IF(X73=0,"",X73)</f>
+        <f t="shared" ref="O73" si="37">+IF(X73=0,"",X73)</f>
         <v/>
       </c>
       <c r="P73" s="74" t="str">
-        <f t="shared" ref="P73" si="53">+IF(Y73=0,"",Y73)</f>
+        <f t="shared" ref="P73" si="38">+IF(Y73=0,"",Y73)</f>
         <v/>
       </c>
       <c r="Q73" s="73"/>
@@ -7690,7 +7880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Computed corrected standard errors
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D39096F-81EC-4D32-AA68-A23FD1930012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C04228-FA08-4B5E-AE29-D8B2DE2852FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="656" firstSheet="9" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -1582,15 +1582,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2487,7 +2485,7 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3847,24 +3845,22 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
-  <dimension ref="A2:S73"/>
+  <dimension ref="A2:W73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A50" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57:F63"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="87" t="s">
         <v>306</v>
       </c>
@@ -3877,7 +3873,7 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="86">
         <v>0</v>
       </c>
@@ -3906,7 +3902,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A4" s="86">
         <v>1</v>
       </c>
@@ -3929,7 +3925,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" s="86">
         <v>2</v>
       </c>
@@ -3946,7 +3942,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" s="86">
         <v>3</v>
       </c>
@@ -3960,7 +3956,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="108" t="s">
         <v>307</v>
       </c>
@@ -3984,7 +3980,7 @@
       <c r="R9" s="109"/>
       <c r="S9" s="109"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="106" t="s">
         <v>309</v>
       </c>
@@ -4008,8 +4004,8 @@
       <c r="R11" s="106"/>
       <c r="S11" s="106"/>
     </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="10" t="s">
         <v>8</v>
       </c>
@@ -4041,7 +4037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>93</v>
       </c>
@@ -4073,41 +4069,65 @@
         <v>5.6152933972934901E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D15" s="73" t="str">
-        <f>+IF(M17=0,"",M17)</f>
-        <v/>
-      </c>
-      <c r="E15" s="73" t="str">
-        <f t="shared" ref="E15:G15" si="0">+IF(N17=0,"",N17)</f>
-        <v/>
-      </c>
-      <c r="F15" s="73" t="str">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D15" s="73">
+        <f>-H15</f>
+        <v>-1.9824513343154201E-2</v>
+      </c>
+      <c r="E15" s="73">
+        <f t="shared" ref="E15:G15" si="0">-I15</f>
+        <v>-7.3337925396310899E-2</v>
+      </c>
+      <c r="F15" s="73">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G15" s="73" t="str">
+        <v>-8.4175794644333599E-2</v>
+      </c>
+      <c r="G15" s="73">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="N15" s="73" t="str">
-        <f>+IF(W17=0,"",W17)</f>
-        <v/>
-      </c>
-      <c r="O15" s="73" t="str">
-        <f t="shared" ref="O15:Q15" si="1">+IF(X17=0,"",X17)</f>
-        <v/>
-      </c>
-      <c r="P15" s="73" t="str">
+        <v>-7.0869425551512197E-2</v>
+      </c>
+      <c r="H15">
+        <v>1.9824513343154201E-2</v>
+      </c>
+      <c r="I15">
+        <v>7.3337925396310899E-2</v>
+      </c>
+      <c r="J15">
+        <v>8.4175794644333599E-2</v>
+      </c>
+      <c r="K15">
+        <v>7.0869425551512197E-2</v>
+      </c>
+      <c r="N15" s="73">
+        <f>-S15</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O15" s="73">
+        <f t="shared" ref="O15:Q15" si="1">-T15</f>
+        <v>-6.2921396769632695E-2</v>
+      </c>
+      <c r="P15" s="73">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="Q15" s="73" t="str">
+        <v>-6.4583503348773899E-2</v>
+      </c>
+      <c r="Q15" s="73">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-7.67475876248436E-2</v>
+      </c>
+      <c r="S15">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T15">
+        <v>6.2921396769632695E-2</v>
+      </c>
+      <c r="U15">
+        <v>6.4583503348773899E-2</v>
+      </c>
+      <c r="V15">
+        <v>7.67475876248436E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>9</v>
       </c>
@@ -4139,29 +4159,65 @@
         <v>2.7066505491686099E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D17" s="73"/>
-      <c r="E17" s="73"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="N17" s="73" t="str">
-        <f>+IF(W18=0,"",W18)</f>
-        <v/>
-      </c>
-      <c r="O17" s="73" t="str">
-        <f t="shared" ref="O17:Q17" si="2">+IF(X18=0,"",X18)</f>
-        <v/>
-      </c>
-      <c r="P17" s="73" t="str">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D17" s="73">
+        <f>-H17</f>
+        <v>-1.9824513343154201E-2</v>
+      </c>
+      <c r="E17" s="73">
+        <f t="shared" ref="E17:G17" si="2">-I17</f>
+        <v>-6.8502347913652506E-2</v>
+      </c>
+      <c r="F17" s="73">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="Q17" s="73" t="str">
+        <v>-8.4504659408050506E-2</v>
+      </c>
+      <c r="G17" s="73">
         <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+        <v>-8.3651740784867104E-2</v>
+      </c>
+      <c r="H17">
+        <v>1.9824513343154201E-2</v>
+      </c>
+      <c r="I17">
+        <v>6.8502347913652506E-2</v>
+      </c>
+      <c r="J17">
+        <v>8.4504659408050506E-2</v>
+      </c>
+      <c r="K17">
+        <v>8.3651740784867104E-2</v>
+      </c>
+      <c r="N17" s="73">
+        <f>-S17</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O17" s="73">
+        <f t="shared" ref="O17:Q17" si="3">-T17</f>
+        <v>-7.3981842197322401E-2</v>
+      </c>
+      <c r="P17" s="73">
+        <f t="shared" si="3"/>
+        <v>-7.6118564642824793E-2</v>
+      </c>
+      <c r="Q17" s="73">
+        <f t="shared" si="3"/>
+        <v>-7.8421126834552699E-2</v>
+      </c>
+      <c r="S17">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T17">
+        <v>7.3981842197322401E-2</v>
+      </c>
+      <c r="U17">
+        <v>7.6118564642824793E-2</v>
+      </c>
+      <c r="V17">
+        <v>7.8421126834552699E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>10</v>
       </c>
@@ -4193,43 +4249,67 @@
         <v>3.1046085155378701E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="19"/>
-      <c r="D19" s="74" t="str">
-        <f>+IF(M19=0,"",M19)</f>
-        <v/>
-      </c>
-      <c r="E19" s="74" t="str">
-        <f t="shared" ref="E19:G19" si="3">+IF(N19=0,"",N19)</f>
-        <v/>
-      </c>
-      <c r="F19" s="74" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="G19" s="74" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="D19" s="74">
+        <f>-H19</f>
+        <v>-1.9824513343154201E-2</v>
+      </c>
+      <c r="E19" s="74">
+        <f t="shared" ref="E19:G19" si="4">-I19</f>
+        <v>-7.8151917060514706E-2</v>
+      </c>
+      <c r="F19" s="74">
+        <f t="shared" si="4"/>
+        <v>-8.1556156708327401E-2</v>
+      </c>
+      <c r="G19" s="74">
+        <f t="shared" si="4"/>
+        <v>-4.9714630821618101E-3</v>
+      </c>
+      <c r="H19">
+        <v>1.9824513343154201E-2</v>
+      </c>
+      <c r="I19">
+        <v>7.8151917060514706E-2</v>
+      </c>
+      <c r="J19">
+        <v>8.1556156708327401E-2</v>
+      </c>
+      <c r="K19">
+        <v>4.9714630821618101E-3</v>
       </c>
       <c r="M19" s="19"/>
-      <c r="N19" s="74" t="str">
-        <f>+IF(W19=0,"",W19)</f>
-        <v/>
-      </c>
-      <c r="O19" s="74" t="str">
-        <f t="shared" ref="O19:Q19" si="4">+IF(X19=0,"",X19)</f>
-        <v/>
-      </c>
-      <c r="P19" s="74" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="Q19" s="74" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N19" s="74">
+        <f>-S19</f>
+        <v>-1.80163841799885E-2</v>
+      </c>
+      <c r="O19" s="74">
+        <f t="shared" ref="O19:Q19" si="5">-T19</f>
+        <v>-6.4554005463114295E-2</v>
+      </c>
+      <c r="P19" s="74">
+        <f t="shared" si="5"/>
+        <v>-6.6745927637415006E-2</v>
+      </c>
+      <c r="Q19" s="74">
+        <f t="shared" si="5"/>
+        <v>-5.3873187988552002E-3</v>
+      </c>
+      <c r="S19">
+        <v>1.80163841799885E-2</v>
+      </c>
+      <c r="T19">
+        <v>6.4554005463114295E-2</v>
+      </c>
+      <c r="U19">
+        <v>6.6745927637415006E-2</v>
+      </c>
+      <c r="V19">
+        <v>5.3873187988552002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" s="106" t="s">
         <v>310</v>
       </c>
@@ -4253,8 +4333,8 @@
       <c r="R21" s="106"/>
       <c r="S21" s="106"/>
     </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C23" s="10" t="s">
         <v>8</v>
       </c>
@@ -4286,7 +4366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>93</v>
       </c>
@@ -4318,41 +4398,65 @@
         <v>4.5710077252419302E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D25" s="73" t="str">
-        <f>+IF(M27=0,"",M27)</f>
-        <v/>
-      </c>
-      <c r="E25" s="73" t="str">
-        <f t="shared" ref="E25" si="5">+IF(N27=0,"",N27)</f>
-        <v/>
-      </c>
-      <c r="F25" s="73" t="str">
-        <f t="shared" ref="F25" si="6">+IF(O27=0,"",O27)</f>
-        <v/>
-      </c>
-      <c r="G25" s="73" t="str">
-        <f t="shared" ref="G25" si="7">+IF(P27=0,"",P27)</f>
-        <v/>
-      </c>
-      <c r="N25" s="73" t="str">
-        <f>+IF(W27=0,"",W27)</f>
-        <v/>
-      </c>
-      <c r="O25" s="73" t="str">
-        <f t="shared" ref="O25" si="8">+IF(X27=0,"",X27)</f>
-        <v/>
-      </c>
-      <c r="P25" s="73" t="str">
-        <f t="shared" ref="P25" si="9">+IF(Y27=0,"",Y27)</f>
-        <v/>
-      </c>
-      <c r="Q25" s="73" t="str">
-        <f t="shared" ref="Q25" si="10">+IF(Z27=0,"",Z27)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D25" s="73">
+        <f>-H25</f>
+        <v>-2.00128377538078E-2</v>
+      </c>
+      <c r="E25" s="73">
+        <f t="shared" ref="E25:G25" si="6">-I25</f>
+        <v>-7.3925691515197997E-2</v>
+      </c>
+      <c r="F25" s="73">
+        <f t="shared" si="6"/>
+        <v>-8.1053378650391694E-2</v>
+      </c>
+      <c r="G25" s="73">
+        <f t="shared" si="6"/>
+        <v>-6.6767345006274001E-2</v>
+      </c>
+      <c r="H25">
+        <v>2.00128377538078E-2</v>
+      </c>
+      <c r="I25">
+        <v>7.3925691515197997E-2</v>
+      </c>
+      <c r="J25">
+        <v>8.1053378650391694E-2</v>
+      </c>
+      <c r="K25">
+        <v>6.6767345006274001E-2</v>
+      </c>
+      <c r="N25" s="73">
+        <f>-S25</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O25" s="73">
+        <f t="shared" ref="O25:Q25" si="7">-T25</f>
+        <v>-6.2705340586680203E-2</v>
+      </c>
+      <c r="P25" s="73">
+        <f t="shared" si="7"/>
+        <v>-6.0532147295976703E-2</v>
+      </c>
+      <c r="Q25" s="73">
+        <f t="shared" si="7"/>
+        <v>-6.79552860893851E-2</v>
+      </c>
+      <c r="S25">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T25">
+        <v>6.2705340586680203E-2</v>
+      </c>
+      <c r="U25">
+        <v>6.0532147295976703E-2</v>
+      </c>
+      <c r="V25">
+        <v>6.79552860893851E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>9</v>
       </c>
@@ -4384,29 +4488,65 @@
         <v>2.2043508532012299E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D27" s="73"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
-      <c r="N27" s="73" t="str">
-        <f>+IF(W28=0,"",W28)</f>
-        <v/>
-      </c>
-      <c r="O27" s="73" t="str">
-        <f t="shared" ref="O27" si="11">+IF(X28=0,"",X28)</f>
-        <v/>
-      </c>
-      <c r="P27" s="73" t="str">
-        <f t="shared" ref="P27" si="12">+IF(Y28=0,"",Y28)</f>
-        <v/>
-      </c>
-      <c r="Q27" s="73" t="str">
-        <f t="shared" ref="Q27" si="13">+IF(Z28=0,"",Z28)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="D27" s="73">
+        <f>-H27</f>
+        <v>-2.00128377538078E-2</v>
+      </c>
+      <c r="E27" s="73">
+        <f t="shared" ref="E27:G27" si="8">-I27</f>
+        <v>-6.8455439714427802E-2</v>
+      </c>
+      <c r="F27" s="73">
+        <f t="shared" si="8"/>
+        <v>-8.1332811762689305E-2</v>
+      </c>
+      <c r="G27" s="73">
+        <f t="shared" si="8"/>
+        <v>-8.05281988916981E-2</v>
+      </c>
+      <c r="H27">
+        <v>2.00128377538078E-2</v>
+      </c>
+      <c r="I27">
+        <v>6.8455439714427802E-2</v>
+      </c>
+      <c r="J27">
+        <v>8.1332811762689305E-2</v>
+      </c>
+      <c r="K27">
+        <v>8.05281988916981E-2</v>
+      </c>
+      <c r="N27" s="73">
+        <f>-S27</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O27" s="73">
+        <f t="shared" ref="O27:Q27" si="9">-T27</f>
+        <v>-7.4363070184416902E-2</v>
+      </c>
+      <c r="P27" s="73">
+        <f t="shared" si="9"/>
+        <v>-7.3014723185476305E-2</v>
+      </c>
+      <c r="Q27" s="73">
+        <f t="shared" si="9"/>
+        <v>-7.1882201893921804E-2</v>
+      </c>
+      <c r="S27">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T27">
+        <v>7.4363070184416902E-2</v>
+      </c>
+      <c r="U27">
+        <v>7.3014723185476305E-2</v>
+      </c>
+      <c r="V27">
+        <v>7.1882201893921804E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="C28" t="s">
         <v>10</v>
       </c>
@@ -4438,43 +4578,67 @@
         <v>2.6102828154984499E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="19"/>
-      <c r="D29" s="74" t="str">
-        <f>+IF(M29=0,"",M29)</f>
-        <v/>
-      </c>
-      <c r="E29" s="74" t="str">
-        <f t="shared" ref="E29" si="14">+IF(N29=0,"",N29)</f>
-        <v/>
-      </c>
-      <c r="F29" s="74" t="str">
-        <f t="shared" ref="F29" si="15">+IF(O29=0,"",O29)</f>
-        <v/>
-      </c>
-      <c r="G29" s="74" t="str">
-        <f t="shared" ref="G29" si="16">+IF(P29=0,"",P29)</f>
-        <v/>
+      <c r="D29" s="74">
+        <f>-H29</f>
+        <v>-2.00128377538078E-2</v>
+      </c>
+      <c r="E29" s="74">
+        <f t="shared" ref="E29:G29" si="10">-I29</f>
+        <v>-7.8311238676915501E-2</v>
+      </c>
+      <c r="F29" s="74">
+        <f t="shared" si="10"/>
+        <v>-8.1763058847982101E-2</v>
+      </c>
+      <c r="G29" s="74">
+        <f t="shared" si="10"/>
+        <v>-5.35045409069495E-3</v>
+      </c>
+      <c r="H29">
+        <v>2.00128377538078E-2</v>
+      </c>
+      <c r="I29">
+        <v>7.8311238676915501E-2</v>
+      </c>
+      <c r="J29">
+        <v>8.1763058847982101E-2</v>
+      </c>
+      <c r="K29">
+        <v>5.35045409069495E-3</v>
       </c>
       <c r="M29" s="19"/>
-      <c r="N29" s="74" t="str">
-        <f>+IF(W29=0,"",W29)</f>
-        <v/>
-      </c>
-      <c r="O29" s="74" t="str">
-        <f t="shared" ref="O29" si="17">+IF(X29=0,"",X29)</f>
-        <v/>
-      </c>
-      <c r="P29" s="74" t="str">
-        <f t="shared" ref="P29" si="18">+IF(Y29=0,"",Y29)</f>
-        <v/>
-      </c>
-      <c r="Q29" s="74" t="str">
-        <f t="shared" ref="Q29" si="19">+IF(Z29=0,"",Z29)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+      <c r="N29" s="74">
+        <f>-S29</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O29" s="74">
+        <f t="shared" ref="O29:Q29" si="11">-T29</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="P29" s="74">
+        <f t="shared" si="11"/>
+        <v>-6.6984637221420507E-2</v>
+      </c>
+      <c r="Q29" s="74">
+        <f t="shared" si="11"/>
+        <v>-5.8788297464031098E-3</v>
+      </c>
+      <c r="S29">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T29">
+        <v>6.4688998413530194E-2</v>
+      </c>
+      <c r="U29">
+        <v>6.6984637221420507E-2</v>
+      </c>
+      <c r="V29">
+        <v>5.8788297464031098E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" s="106" t="s">
         <v>311</v>
       </c>
@@ -4498,8 +4662,8 @@
       <c r="R31" s="106"/>
       <c r="S31" s="106"/>
     </row>
-    <row r="32" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="33" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="10" t="s">
         <v>8</v>
       </c>
@@ -4531,7 +4695,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C34" t="s">
         <v>93</v>
       </c>
@@ -4563,41 +4727,65 @@
         <v>3.93416384989266E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
-      <c r="D35" s="73" t="str">
-        <f>+IF(M37=0,"",M37)</f>
-        <v/>
-      </c>
-      <c r="E35" s="73" t="str">
-        <f t="shared" ref="E35" si="20">+IF(N37=0,"",N37)</f>
-        <v/>
-      </c>
-      <c r="F35" s="73" t="str">
-        <f t="shared" ref="F35" si="21">+IF(O37=0,"",O37)</f>
-        <v/>
-      </c>
-      <c r="G35" s="73" t="str">
-        <f t="shared" ref="G35" si="22">+IF(P37=0,"",P37)</f>
-        <v/>
-      </c>
-      <c r="N35" s="73" t="str">
-        <f>+IF(W37=0,"",W37)</f>
-        <v/>
-      </c>
-      <c r="O35" s="73" t="str">
-        <f t="shared" ref="O35" si="23">+IF(X37=0,"",X37)</f>
-        <v/>
-      </c>
-      <c r="P35" s="73" t="str">
-        <f t="shared" ref="P35" si="24">+IF(Y37=0,"",Y37)</f>
-        <v/>
-      </c>
-      <c r="Q35" s="73" t="str">
-        <f t="shared" ref="Q35" si="25">+IF(Z37=0,"",Z37)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="D35" s="73">
+        <f>-H35</f>
+        <v>-2.0235567234909199E-2</v>
+      </c>
+      <c r="E35" s="73">
+        <f t="shared" ref="E35:G35" si="12">-I35</f>
+        <v>-7.5552651728106296E-2</v>
+      </c>
+      <c r="F35" s="73">
+        <f t="shared" si="12"/>
+        <v>-7.8481015659589495E-2</v>
+      </c>
+      <c r="G35" s="73">
+        <f t="shared" si="12"/>
+        <v>-6.1029708840424898E-2</v>
+      </c>
+      <c r="H35">
+        <v>2.0235567234909199E-2</v>
+      </c>
+      <c r="I35">
+        <v>7.5552651728106296E-2</v>
+      </c>
+      <c r="J35">
+        <v>7.8481015659589495E-2</v>
+      </c>
+      <c r="K35">
+        <v>6.1029708840424898E-2</v>
+      </c>
+      <c r="N35" s="73">
+        <f>-S35</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O35" s="73">
+        <f t="shared" ref="O35:P35" si="13">-T35</f>
+        <v>-6.6121303110595497E-2</v>
+      </c>
+      <c r="P35" s="73">
+        <f t="shared" si="13"/>
+        <v>-5.7998508062290899E-2</v>
+      </c>
+      <c r="Q35" s="73">
+        <f>-V35</f>
+        <v>-6.5015545691961399E-2</v>
+      </c>
+      <c r="S35">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T35">
+        <v>6.6121303110595497E-2</v>
+      </c>
+      <c r="U35">
+        <v>5.7998508062290899E-2</v>
+      </c>
+      <c r="V35">
+        <v>6.5015545691961399E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C36" t="s">
         <v>9</v>
       </c>
@@ -4629,29 +4817,65 @@
         <v>1.7184485249948499E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
-      <c r="D37" s="73"/>
-      <c r="E37" s="73"/>
-      <c r="F37" s="73"/>
-      <c r="G37" s="73"/>
-      <c r="N37" s="73" t="str">
-        <f>+IF(W38=0,"",W38)</f>
-        <v/>
-      </c>
-      <c r="O37" s="73" t="str">
-        <f t="shared" ref="O37" si="26">+IF(X38=0,"",X38)</f>
-        <v/>
-      </c>
-      <c r="P37" s="73" t="str">
-        <f t="shared" ref="P37" si="27">+IF(Y38=0,"",Y38)</f>
-        <v/>
-      </c>
-      <c r="Q37" s="73" t="str">
-        <f t="shared" ref="Q37" si="28">+IF(Z38=0,"",Z38)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="D37" s="73">
+        <f>-H37</f>
+        <v>-2.0235567234909199E-2</v>
+      </c>
+      <c r="E37" s="73">
+        <f t="shared" ref="E37:G37" si="14">-I37</f>
+        <v>-6.9992651510969103E-2</v>
+      </c>
+      <c r="F37" s="73">
+        <f t="shared" si="14"/>
+        <v>-7.7099892551743293E-2</v>
+      </c>
+      <c r="G37" s="73">
+        <f t="shared" si="14"/>
+        <v>-7.8626651379215096E-2</v>
+      </c>
+      <c r="H37">
+        <v>2.0235567234909199E-2</v>
+      </c>
+      <c r="I37">
+        <v>6.9992651510969103E-2</v>
+      </c>
+      <c r="J37">
+        <v>7.7099892551743293E-2</v>
+      </c>
+      <c r="K37">
+        <v>7.8626651379215096E-2</v>
+      </c>
+      <c r="N37" s="73">
+        <f>-S37</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O37" s="73">
+        <f t="shared" ref="O37:Q37" si="15">-T37</f>
+        <v>-7.7697154041311306E-2</v>
+      </c>
+      <c r="P37" s="73">
+        <f t="shared" si="15"/>
+        <v>-7.0698211707042102E-2</v>
+      </c>
+      <c r="Q37" s="73">
+        <f t="shared" si="15"/>
+        <v>-7.1608927235836894E-2</v>
+      </c>
+      <c r="S37">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T37">
+        <v>7.7697154041311306E-2</v>
+      </c>
+      <c r="U37">
+        <v>7.0698211707042102E-2</v>
+      </c>
+      <c r="V37">
+        <v>7.1608927235836894E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C38" t="s">
         <v>10</v>
       </c>
@@ -4683,44 +4907,67 @@
         <v>1.8797507235916999E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="19"/>
-      <c r="D39" s="74" t="str">
-        <f>+IF(M39=0,"",M39)</f>
-        <v/>
-      </c>
-      <c r="E39" s="74" t="str">
-        <f t="shared" ref="E39" si="29">+IF(N39=0,"",N39)</f>
-        <v/>
-      </c>
-      <c r="F39" s="74" t="str">
-        <f t="shared" ref="F39" si="30">+IF(O39=0,"",O39)</f>
-        <v/>
-      </c>
-      <c r="G39" s="74" t="str">
-        <f t="shared" ref="G39" si="31">+IF(P39=0,"",P39)</f>
-        <v/>
+      <c r="D39" s="74">
+        <f>-H39</f>
+        <v>-2.0235567234909199E-2</v>
+      </c>
+      <c r="E39" s="74">
+        <f t="shared" ref="E39:G39" si="16">-I39</f>
+        <v>-7.8220484531113396E-2</v>
+      </c>
+      <c r="F39" s="74">
+        <f t="shared" si="16"/>
+        <v>-8.15621610602935E-2</v>
+      </c>
+      <c r="G39" s="74">
+        <f t="shared" si="16"/>
+        <v>-5.86398043718569E-3</v>
+      </c>
+      <c r="H39">
+        <v>2.0235567234909199E-2</v>
+      </c>
+      <c r="I39">
+        <v>7.8220484531113396E-2</v>
+      </c>
+      <c r="J39">
+        <v>8.15621610602935E-2</v>
+      </c>
+      <c r="K39">
+        <v>5.86398043718569E-3</v>
       </c>
       <c r="M39" s="19"/>
-      <c r="N39" s="74" t="str">
-        <f>+IF(W39=0,"",W39)</f>
-        <v/>
-      </c>
-      <c r="O39" s="74" t="str">
-        <f t="shared" ref="O39" si="32">+IF(X39=0,"",X39)</f>
-        <v/>
-      </c>
-      <c r="P39" s="74" t="str">
-        <f t="shared" ref="P39" si="33">+IF(Y39=0,"",Y39)</f>
-        <v/>
-      </c>
-      <c r="Q39" s="74" t="str">
-        <f t="shared" ref="Q39" si="34">+IF(Z39=0,"",Z39)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N39" s="74">
+        <f>-S39</f>
+        <v>-1.8593580225319199E-2</v>
+      </c>
+      <c r="O39" s="74">
+        <f t="shared" ref="O39:Q39" si="17">-T39</f>
+        <v>-6.4659214976102206E-2</v>
+      </c>
+      <c r="P39" s="74">
+        <f t="shared" si="17"/>
+        <v>-6.7086317193334202E-2</v>
+      </c>
+      <c r="Q39" s="74">
+        <f t="shared" si="17"/>
+        <v>-6.7079383018708201E-3</v>
+      </c>
+      <c r="S39">
+        <v>1.8593580225319199E-2</v>
+      </c>
+      <c r="T39">
+        <v>6.4659214976102206E-2</v>
+      </c>
+      <c r="U39">
+        <v>6.7086317193334202E-2</v>
+      </c>
+      <c r="V39">
+        <v>6.7079383018708201E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="106" t="s">
         <v>312</v>
       </c>
@@ -4744,8 +4991,8 @@
       <c r="R42" s="106"/>
       <c r="S42" s="106"/>
     </row>
-    <row r="43" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="44" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C44" s="10" t="s">
         <v>8</v>
       </c>
@@ -4777,22 +5024,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C45" t="s">
         <v>93</v>
       </c>
-      <c r="D45" s="88">
-        <v>0.31018306322082201</v>
-      </c>
-      <c r="E45" s="88">
-        <v>0.35740478053101099</v>
-      </c>
-      <c r="F45" s="88">
-        <v>0.68349910741717101</v>
-      </c>
-      <c r="G45" s="88">
-        <v>0.30750371060827297</v>
-      </c>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
       <c r="M45" t="s">
         <v>93</v>
       </c>
@@ -4808,45 +5047,57 @@
       <c r="Q45" s="72">
         <v>4.5583593355867702E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R45" s="90"/>
+      <c r="S45" s="90"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
       <c r="F46" s="73"/>
       <c r="G46" s="73"/>
-      <c r="N46" s="73" t="str">
-        <f>+IF(W48=0,"",W48)</f>
-        <v/>
-      </c>
-      <c r="O46" s="73" t="str">
-        <f t="shared" ref="O46" si="35">+IF(X48=0,"",X48)</f>
-        <v/>
-      </c>
-      <c r="P46" s="73" t="str">
-        <f t="shared" ref="P46" si="36">+IF(Y48=0,"",Y48)</f>
-        <v/>
-      </c>
-      <c r="Q46" s="73" t="str">
-        <f t="shared" ref="Q46" si="37">+IF(Z48=0,"",Z48)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N46" s="88">
+        <f>-S46</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O46" s="88">
+        <f t="shared" ref="O46:Q46" si="18">-T46</f>
+        <v>-6.2705340586680203E-2</v>
+      </c>
+      <c r="P46" s="88">
+        <f t="shared" si="18"/>
+        <v>-6.0532147295976703E-2</v>
+      </c>
+      <c r="Q46" s="88">
+        <f t="shared" si="18"/>
+        <v>-6.79552860893851E-2</v>
+      </c>
+      <c r="R46" s="90"/>
+      <c r="S46" s="88">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T46" s="88">
+        <v>6.2705340586680203E-2</v>
+      </c>
+      <c r="U46" s="88">
+        <v>6.0532147295976703E-2</v>
+      </c>
+      <c r="V46" s="88">
+        <v>6.79552860893851E-2</v>
+      </c>
+      <c r="W46" s="90"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="89">
-        <v>0.31018306322082201</v>
-      </c>
-      <c r="E47" s="89">
-        <v>0.65682449572895196</v>
-      </c>
-      <c r="F47" s="89">
-        <v>0.49183973592229402</v>
-      </c>
-      <c r="G47" s="89">
-        <v>0.130974449674474</v>
-      </c>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
+      <c r="F47" s="72"/>
+      <c r="G47" s="72"/>
       <c r="M47" t="s">
         <v>9</v>
       </c>
@@ -4862,33 +5113,57 @@
       <c r="Q47" s="72">
         <v>2.22521472100402E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="D48" s="89"/>
-      <c r="E48" s="89"/>
-      <c r="F48" s="89"/>
-      <c r="G48" s="89"/>
-      <c r="N48" s="73"/>
-      <c r="O48" s="73"/>
-      <c r="P48" s="73"/>
-      <c r="Q48" s="73"/>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R47" s="90"/>
+      <c r="S47" s="90"/>
+      <c r="T47" s="90"/>
+      <c r="U47" s="90"/>
+      <c r="V47" s="90"/>
+      <c r="W47" s="90"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="73"/>
+      <c r="N48" s="88">
+        <f>-S48</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O48" s="88">
+        <f t="shared" ref="O48:Q48" si="19">-T48</f>
+        <v>-7.4363070184416902E-2</v>
+      </c>
+      <c r="P48" s="88">
+        <f t="shared" si="19"/>
+        <v>-7.3014723185476305E-2</v>
+      </c>
+      <c r="Q48" s="88">
+        <f t="shared" si="19"/>
+        <v>-7.1882201893921804E-2</v>
+      </c>
+      <c r="R48" s="90"/>
+      <c r="S48" s="88">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T48" s="88">
+        <v>7.4363070184416902E-2</v>
+      </c>
+      <c r="U48" s="88">
+        <v>7.3014723185476305E-2</v>
+      </c>
+      <c r="V48" s="88">
+        <v>7.1882201893921804E-2</v>
+      </c>
+      <c r="W48" s="90"/>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="89">
-        <v>0.31018306322082201</v>
-      </c>
-      <c r="E49" s="89">
-        <v>0.63946528642015499</v>
-      </c>
-      <c r="F49" s="89">
-        <v>0.35108000833060798</v>
-      </c>
-      <c r="G49" s="89">
-        <v>0.28430945844107902</v>
-      </c>
+      <c r="D49" s="72"/>
+      <c r="E49" s="72"/>
+      <c r="F49" s="72"/>
+      <c r="G49" s="72"/>
       <c r="M49" t="s">
         <v>10</v>
       </c>
@@ -4904,44 +5179,55 @@
       <c r="Q49" s="72">
         <v>2.5977753128474598E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="R49" s="90"/>
+      <c r="S49" s="90"/>
+      <c r="T49" s="90"/>
+      <c r="U49" s="90"/>
+      <c r="V49" s="90"/>
+      <c r="W49" s="90"/>
+    </row>
+    <row r="50" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="19"/>
-      <c r="D50" s="90" t="str">
+      <c r="D50" s="74" t="str">
         <f>+IF(M50=0,"",M50)</f>
         <v/>
       </c>
-      <c r="E50" s="90" t="str">
-        <f t="shared" ref="E50" si="38">+IF(N50=0,"",N50)</f>
-        <v/>
-      </c>
-      <c r="F50" s="90" t="str">
-        <f t="shared" ref="F50" si="39">+IF(O50=0,"",O50)</f>
-        <v/>
-      </c>
-      <c r="G50" s="90" t="str">
-        <f t="shared" ref="G50" si="40">+IF(P50=0,"",P50)</f>
-        <v/>
-      </c>
+      <c r="E50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
       <c r="M50" s="19"/>
-      <c r="N50" s="74" t="str">
-        <f>+IF(W50=0,"",W50)</f>
-        <v/>
-      </c>
-      <c r="O50" s="74" t="str">
-        <f t="shared" ref="O50" si="41">+IF(X50=0,"",X50)</f>
-        <v/>
-      </c>
-      <c r="P50" s="74" t="str">
-        <f t="shared" ref="P50" si="42">+IF(Y50=0,"",Y50)</f>
-        <v/>
-      </c>
-      <c r="Q50" s="74" t="str">
-        <f t="shared" ref="Q50" si="43">+IF(Z50=0,"",Z50)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="N50" s="89">
+        <f>-S50</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="O50" s="89">
+        <f t="shared" ref="O50:Q50" si="20">-T50</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="P50" s="89">
+        <f t="shared" si="20"/>
+        <v>-6.6984637221420507E-2</v>
+      </c>
+      <c r="Q50" s="89">
+        <f t="shared" si="20"/>
+        <v>-5.8788297464031098E-3</v>
+      </c>
+      <c r="R50" s="90"/>
+      <c r="S50" s="88">
+        <v>1.8232139167409501E-2</v>
+      </c>
+      <c r="T50" s="88">
+        <v>6.4688998413530194E-2</v>
+      </c>
+      <c r="U50" s="88">
+        <v>6.6984637221420507E-2</v>
+      </c>
+      <c r="V50" s="88">
+        <v>5.8788297464031098E-3</v>
+      </c>
+      <c r="W50" s="90"/>
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A53" s="107" t="s">
         <v>313</v>
       </c>
@@ -4964,7 +5250,7 @@
       <c r="R53" s="107"/>
       <c r="S53" s="107"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A55" s="106" t="s">
         <v>314</v>
       </c>
@@ -4988,8 +5274,8 @@
       <c r="R55" s="106"/>
       <c r="S55" s="106"/>
     </row>
-    <row r="56" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="57" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C57" s="10" t="s">
         <v>8</v>
       </c>
@@ -5017,19 +5303,13 @@
       </c>
       <c r="Q57" s="54"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C58" t="s">
         <v>93</v>
       </c>
-      <c r="D58" s="72">
-        <v>0.30019250319507501</v>
-      </c>
-      <c r="E58" s="72">
-        <v>0.314020637070486</v>
-      </c>
-      <c r="F58" s="72">
-        <v>0.81723706035450705</v>
-      </c>
+      <c r="D58" s="72"/>
+      <c r="E58" s="72"/>
+      <c r="F58" s="72"/>
       <c r="G58" s="72"/>
       <c r="M58" t="s">
         <v>93</v>
@@ -5045,7 +5325,7 @@
       </c>
       <c r="Q58" s="72"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D59" s="73"/>
       <c r="E59" s="73"/>
       <c r="F59" s="73"/>
@@ -5055,19 +5335,13 @@
       <c r="P59" s="73"/>
       <c r="Q59" s="73"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C60" t="s">
         <v>9</v>
       </c>
-      <c r="D60" s="72">
-        <v>0.30019250319507501</v>
-      </c>
-      <c r="E60" s="72">
-        <v>0.68025733523300802</v>
-      </c>
-      <c r="F60" s="72">
-        <v>0.50537378426994894</v>
-      </c>
+      <c r="D60" s="72"/>
+      <c r="E60" s="72"/>
+      <c r="F60" s="72"/>
       <c r="G60" s="72"/>
       <c r="M60" t="s">
         <v>9</v>
@@ -5083,7 +5357,7 @@
       </c>
       <c r="Q60" s="72"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D61" s="73"/>
       <c r="E61" s="73"/>
       <c r="F61" s="73"/>
@@ -5093,19 +5367,13 @@
       <c r="P61" s="73"/>
       <c r="Q61" s="73"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C62" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="72">
-        <v>0.30019250319507501</v>
-      </c>
-      <c r="E62" s="72">
-        <v>0.854752473086689</v>
-      </c>
-      <c r="F62" s="72">
-        <v>0.30630121932812399</v>
-      </c>
+      <c r="D62" s="72"/>
+      <c r="E62" s="72"/>
+      <c r="F62" s="72"/>
       <c r="G62" s="72"/>
       <c r="M62" t="s">
         <v>10</v>
@@ -5121,22 +5389,22 @@
       </c>
       <c r="Q62" s="72"/>
     </row>
-    <row r="63" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C63" s="19"/>
       <c r="D63" s="74" t="str">
         <f>+IF(M63=0,"",M63)</f>
         <v/>
       </c>
       <c r="E63" s="74" t="str">
-        <f t="shared" ref="E63" si="44">+IF(N63=0,"",N63)</f>
+        <f t="shared" ref="E63" si="21">+IF(N63=0,"",N63)</f>
         <v/>
       </c>
       <c r="F63" s="74" t="str">
-        <f t="shared" ref="F63" si="45">+IF(O63=0,"",O63)</f>
+        <f t="shared" ref="F63" si="22">+IF(O63=0,"",O63)</f>
         <v/>
       </c>
       <c r="G63" s="73" t="str">
-        <f t="shared" ref="G63" si="46">+IF(P63=0,"",P63)</f>
+        <f t="shared" ref="G63" si="23">+IF(P63=0,"",P63)</f>
         <v/>
       </c>
       <c r="M63" s="19"/>
@@ -5145,11 +5413,11 @@
         <v/>
       </c>
       <c r="O63" s="74" t="str">
-        <f t="shared" ref="O63" si="47">+IF(X63=0,"",X63)</f>
+        <f t="shared" ref="O63" si="24">+IF(X63=0,"",X63)</f>
         <v/>
       </c>
       <c r="P63" s="74" t="str">
-        <f t="shared" ref="P63" si="48">+IF(Y63=0,"",Y63)</f>
+        <f t="shared" ref="P63" si="25">+IF(Y63=0,"",Y63)</f>
         <v/>
       </c>
       <c r="Q63" s="73"/>
@@ -5211,15 +5479,9 @@
       <c r="C68" t="s">
         <v>93</v>
       </c>
-      <c r="D68" s="72">
-        <v>0.35282665388944701</v>
-      </c>
-      <c r="E68" s="72">
-        <v>1.0265099595049401</v>
-      </c>
-      <c r="F68" s="72">
-        <v>1.8237993964939098E-2</v>
-      </c>
+      <c r="D68" s="72"/>
+      <c r="E68" s="72"/>
+      <c r="F68" s="72"/>
       <c r="G68" s="72"/>
       <c r="M68" t="s">
         <v>93</v>
@@ -5249,15 +5511,9 @@
       <c r="C70" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="72">
-        <v>0.35282665388944701</v>
-      </c>
-      <c r="E70" s="72">
-        <v>1.0726708688684199</v>
-      </c>
-      <c r="F70" s="72">
-        <v>0.140178425773164</v>
-      </c>
+      <c r="D70" s="72"/>
+      <c r="E70" s="72"/>
+      <c r="F70" s="72"/>
       <c r="G70" s="72"/>
       <c r="M70" t="s">
         <v>9</v>
@@ -5287,15 +5543,9 @@
       <c r="C72" t="s">
         <v>10</v>
       </c>
-      <c r="D72" s="72">
-        <v>0.35282665388944701</v>
-      </c>
-      <c r="E72" s="72">
-        <v>0.91491379472894196</v>
-      </c>
-      <c r="F72" s="72">
-        <v>0.249567365316156</v>
-      </c>
+      <c r="D72" s="72"/>
+      <c r="E72" s="72"/>
+      <c r="F72" s="72"/>
       <c r="G72" s="72"/>
       <c r="M72" t="s">
         <v>10</v>
@@ -5318,15 +5568,15 @@
         <v/>
       </c>
       <c r="E73" s="74" t="str">
-        <f t="shared" ref="E73" si="49">+IF(N73=0,"",N73)</f>
+        <f t="shared" ref="E73" si="26">+IF(N73=0,"",N73)</f>
         <v/>
       </c>
       <c r="F73" s="74" t="str">
-        <f t="shared" ref="F73" si="50">+IF(O73=0,"",O73)</f>
+        <f t="shared" ref="F73" si="27">+IF(O73=0,"",O73)</f>
         <v/>
       </c>
       <c r="G73" s="73" t="str">
-        <f t="shared" ref="G73" si="51">+IF(P73=0,"",P73)</f>
+        <f t="shared" ref="G73" si="28">+IF(P73=0,"",P73)</f>
         <v/>
       </c>
       <c r="M73" s="19"/>
@@ -5335,11 +5585,11 @@
         <v/>
       </c>
       <c r="O73" s="74" t="str">
-        <f t="shared" ref="O73" si="52">+IF(X73=0,"",X73)</f>
+        <f t="shared" ref="O73" si="29">+IF(X73=0,"",X73)</f>
         <v/>
       </c>
       <c r="P73" s="74" t="str">
-        <f t="shared" ref="P73" si="53">+IF(Y73=0,"",Y73)</f>
+        <f t="shared" ref="P73" si="30">+IF(Y73=0,"",Y73)</f>
         <v/>
       </c>
       <c r="Q73" s="73"/>
@@ -7762,7 +8012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commiting changes in the excel
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483539F5-DF25-4370-BBBD-12BCE5DE4CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840BC064-4BB9-413E-A0C9-E49E799A6DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="12" activeTab="15" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="320">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1107,6 +1107,18 @@
   </si>
   <si>
     <t>No routine, definition 2</t>
+  </si>
+  <si>
+    <t>A. Manual</t>
+  </si>
+  <si>
+    <t>B. Social</t>
+  </si>
+  <si>
+    <t>C. Adaptability</t>
+  </si>
+  <si>
+    <t>D. Abstract</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1242,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1312,6 +1324,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1582,6 +1600,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1630,26 +1655,19 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2253,14 +2271,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2362,14 +2380,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="91" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
+      <c r="B9" s="91"/>
+      <c r="C9" s="91"/>
+      <c r="D9" s="91"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="91"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2487,8 +2505,8 @@
   </sheetPr>
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2498,20 +2516,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="105"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2826,11 +2844,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="91"/>
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2845,13 +2863,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="102" t="s">
+      <c r="A15" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="102"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="102"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="10">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2995,11 +3013,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="88" t="s">
+      <c r="G24" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="88"/>
-      <c r="I24" s="88"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="91"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -3025,13 +3043,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="102" t="s">
+      <c r="A26" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="102"/>
-      <c r="C26" s="102"/>
-      <c r="D26" s="102"/>
-      <c r="E26" s="102"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
+      <c r="E26" s="105"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="11">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -3208,20 +3226,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="102" t="s">
+      <c r="A37" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="102"/>
-      <c r="C37" s="102"/>
-      <c r="D37" s="102"/>
-      <c r="E37" s="102"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="105"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="105"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="88" t="s">
+      <c r="G38" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="88"/>
-      <c r="I38" s="88"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="91"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3513,20 +3531,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="102" t="s">
+      <c r="A51" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="102"/>
-      <c r="C51" s="102"/>
-      <c r="D51" s="102"/>
-      <c r="E51" s="102"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="88" t="s">
+      <c r="G52" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="88"/>
-      <c r="I52" s="88"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3850,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
   <dimension ref="A2:W73"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S50" sqref="S50:V50"/>
+    <sheetView showGridLines="0" topLeftCell="E26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3960,52 +3978,52 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="104" t="s">
+      <c r="A9" s="108" t="s">
         <v>307</v>
       </c>
-      <c r="B9" s="104"/>
-      <c r="C9" s="104"/>
-      <c r="D9" s="104"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="K9" s="105" t="s">
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="108"/>
+      <c r="E9" s="108"/>
+      <c r="F9" s="108"/>
+      <c r="G9" s="108"/>
+      <c r="H9" s="108"/>
+      <c r="I9" s="108"/>
+      <c r="K9" s="109" t="s">
         <v>308</v>
       </c>
-      <c r="L9" s="105"/>
-      <c r="M9" s="105"/>
-      <c r="N9" s="105"/>
-      <c r="O9" s="105"/>
-      <c r="P9" s="105"/>
-      <c r="Q9" s="105"/>
-      <c r="R9" s="105"/>
-      <c r="S9" s="105"/>
+      <c r="L9" s="109"/>
+      <c r="M9" s="109"/>
+      <c r="N9" s="109"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="109"/>
+      <c r="Q9" s="109"/>
+      <c r="R9" s="109"/>
+      <c r="S9" s="109"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="B11" s="103"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="K11" s="103" t="s">
+      <c r="B11" s="106"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="106"/>
+      <c r="F11" s="106"/>
+      <c r="G11" s="106"/>
+      <c r="H11" s="106"/>
+      <c r="I11" s="106"/>
+      <c r="K11" s="106" t="s">
         <v>309</v>
       </c>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="103"/>
-      <c r="R11" s="103"/>
-      <c r="S11" s="103"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="106"/>
+      <c r="N11" s="106"/>
+      <c r="O11" s="106"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="106"/>
+      <c r="R11" s="106"/>
+      <c r="S11" s="106"/>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4265,28 +4283,28 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="103" t="s">
+      <c r="A21" s="106" t="s">
         <v>310</v>
       </c>
-      <c r="B21" s="103"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
-      <c r="H21" s="103"/>
-      <c r="I21" s="103"/>
-      <c r="K21" s="103" t="s">
+      <c r="B21" s="106"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
+      <c r="I21" s="106"/>
+      <c r="K21" s="111" t="s">
         <v>310</v>
       </c>
-      <c r="L21" s="103"/>
-      <c r="M21" s="103"/>
-      <c r="N21" s="103"/>
-      <c r="O21" s="103"/>
-      <c r="P21" s="103"/>
-      <c r="Q21" s="103"/>
-      <c r="R21" s="103"/>
-      <c r="S21" s="103"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
     </row>
     <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4546,28 +4564,28 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A31" s="103" t="s">
+      <c r="A31" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="K31" s="103" t="s">
+      <c r="B31" s="106"/>
+      <c r="C31" s="106"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="106"/>
+      <c r="F31" s="106"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="106"/>
+      <c r="I31" s="106"/>
+      <c r="K31" s="106" t="s">
         <v>311</v>
       </c>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
+      <c r="L31" s="106"/>
+      <c r="M31" s="106"/>
+      <c r="N31" s="106"/>
+      <c r="O31" s="106"/>
+      <c r="P31" s="106"/>
+      <c r="Q31" s="106"/>
+      <c r="R31" s="106"/>
+      <c r="S31" s="106"/>
     </row>
     <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4827,28 +4845,28 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A42" s="103" t="s">
+      <c r="A42" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="B42" s="103"/>
-      <c r="C42" s="103"/>
-      <c r="D42" s="103"/>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="103"/>
-      <c r="H42" s="103"/>
-      <c r="I42" s="103"/>
-      <c r="K42" s="103" t="s">
+      <c r="B42" s="106"/>
+      <c r="C42" s="106"/>
+      <c r="D42" s="106"/>
+      <c r="E42" s="106"/>
+      <c r="F42" s="106"/>
+      <c r="G42" s="106"/>
+      <c r="H42" s="106"/>
+      <c r="I42" s="106"/>
+      <c r="K42" s="106" t="s">
         <v>312</v>
       </c>
-      <c r="L42" s="103"/>
-      <c r="M42" s="103"/>
-      <c r="N42" s="103"/>
-      <c r="O42" s="103"/>
-      <c r="P42" s="103"/>
-      <c r="Q42" s="103"/>
-      <c r="R42" s="103"/>
-      <c r="S42" s="103"/>
+      <c r="L42" s="106"/>
+      <c r="M42" s="106"/>
+      <c r="N42" s="106"/>
+      <c r="O42" s="106"/>
+      <c r="P42" s="106"/>
+      <c r="Q42" s="106"/>
+      <c r="R42" s="106"/>
+      <c r="S42" s="106"/>
     </row>
     <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4906,48 +4924,48 @@
       <c r="Q45" s="72">
         <v>4.5583593355867702E-2</v>
       </c>
-      <c r="R45" s="110"/>
-      <c r="S45" s="110"/>
-      <c r="T45" s="110"/>
-      <c r="U45" s="110"/>
-      <c r="V45" s="110"/>
-      <c r="W45" s="110"/>
+      <c r="R45" s="90"/>
+      <c r="S45" s="90"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D46" s="73"/>
       <c r="E46" s="73"/>
       <c r="F46" s="73"/>
       <c r="G46" s="73"/>
-      <c r="N46" s="108">
+      <c r="N46" s="88">
         <f>-S46</f>
         <v>-1.8232139167409501E-2</v>
       </c>
-      <c r="O46" s="108">
+      <c r="O46" s="88">
         <f t="shared" ref="O46:Q46" si="23">-T46</f>
         <v>-6.2705340586680203E-2</v>
       </c>
-      <c r="P46" s="108">
+      <c r="P46" s="88">
         <f t="shared" si="23"/>
         <v>-6.0532147295976703E-2</v>
       </c>
-      <c r="Q46" s="108">
+      <c r="Q46" s="88">
         <f t="shared" si="23"/>
         <v>-6.79552860893851E-2</v>
       </c>
-      <c r="R46" s="110"/>
-      <c r="S46" s="108">
+      <c r="R46" s="90"/>
+      <c r="S46" s="88">
         <v>1.8232139167409501E-2</v>
       </c>
-      <c r="T46" s="108">
+      <c r="T46" s="88">
         <v>6.2705340586680203E-2</v>
       </c>
-      <c r="U46" s="108">
+      <c r="U46" s="88">
         <v>6.0532147295976703E-2</v>
       </c>
-      <c r="V46" s="108">
+      <c r="V46" s="88">
         <v>6.79552860893851E-2</v>
       </c>
-      <c r="W46" s="110"/>
+      <c r="W46" s="90"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C47" t="s">
@@ -4972,48 +4990,48 @@
       <c r="Q47" s="72">
         <v>2.22521472100402E-2</v>
       </c>
-      <c r="R47" s="110"/>
-      <c r="S47" s="110"/>
-      <c r="T47" s="110"/>
-      <c r="U47" s="110"/>
-      <c r="V47" s="110"/>
-      <c r="W47" s="110"/>
+      <c r="R47" s="90"/>
+      <c r="S47" s="90"/>
+      <c r="T47" s="90"/>
+      <c r="U47" s="90"/>
+      <c r="V47" s="90"/>
+      <c r="W47" s="90"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="D48" s="73"/>
       <c r="E48" s="73"/>
       <c r="F48" s="73"/>
       <c r="G48" s="73"/>
-      <c r="N48" s="108">
+      <c r="N48" s="88">
         <f>-S48</f>
         <v>-1.8232139167409501E-2</v>
       </c>
-      <c r="O48" s="108">
+      <c r="O48" s="88">
         <f t="shared" ref="O48:Q48" si="24">-T48</f>
         <v>-7.4363070184416902E-2</v>
       </c>
-      <c r="P48" s="108">
+      <c r="P48" s="88">
         <f t="shared" si="24"/>
         <v>-7.3014723185476305E-2</v>
       </c>
-      <c r="Q48" s="108">
+      <c r="Q48" s="88">
         <f t="shared" si="24"/>
         <v>-7.1882201893921804E-2</v>
       </c>
-      <c r="R48" s="110"/>
-      <c r="S48" s="108">
+      <c r="R48" s="90"/>
+      <c r="S48" s="88">
         <v>1.8232139167409501E-2</v>
       </c>
-      <c r="T48" s="108">
+      <c r="T48" s="88">
         <v>7.4363070184416902E-2</v>
       </c>
-      <c r="U48" s="108">
+      <c r="U48" s="88">
         <v>7.3014723185476305E-2</v>
       </c>
-      <c r="V48" s="108">
+      <c r="V48" s="88">
         <v>7.1882201893921804E-2</v>
       </c>
-      <c r="W48" s="110"/>
+      <c r="W48" s="90"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.35">
       <c r="C49" t="s">
@@ -5038,12 +5056,12 @@
       <c r="Q49" s="72">
         <v>2.5977753128474598E-2</v>
       </c>
-      <c r="R49" s="110"/>
-      <c r="S49" s="110"/>
-      <c r="T49" s="110"/>
-      <c r="U49" s="110"/>
-      <c r="V49" s="110"/>
-      <c r="W49" s="110"/>
+      <c r="R49" s="90"/>
+      <c r="S49" s="90"/>
+      <c r="T49" s="90"/>
+      <c r="U49" s="90"/>
+      <c r="V49" s="90"/>
+      <c r="W49" s="90"/>
     </row>
     <row r="50" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C50" s="19"/>
@@ -5064,83 +5082,83 @@
         <v>-6.6984637221420507E-2</v>
       </c>
       <c r="M50" s="19"/>
-      <c r="N50" s="109">
+      <c r="N50" s="89">
         <f>-S50</f>
         <v>-1.8232139167409501E-2</v>
       </c>
-      <c r="O50" s="109">
+      <c r="O50" s="89">
         <f t="shared" ref="O50:Q50" si="28">-T50</f>
         <v>-6.4688998413530194E-2</v>
       </c>
-      <c r="P50" s="109">
+      <c r="P50" s="89">
         <f t="shared" si="28"/>
         <v>-6.6984637221420507E-2</v>
       </c>
-      <c r="Q50" s="109">
+      <c r="Q50" s="89">
         <f t="shared" si="28"/>
         <v>-5.8788297464031098E-3</v>
       </c>
-      <c r="R50" s="110"/>
-      <c r="S50" s="111">
+      <c r="R50" s="90"/>
+      <c r="S50" s="88">
         <v>1.8232139167409501E-2</v>
       </c>
-      <c r="T50" s="111">
+      <c r="T50" s="88">
         <v>6.4688998413530194E-2</v>
       </c>
-      <c r="U50" s="111">
+      <c r="U50" s="88">
         <v>6.6984637221420507E-2</v>
       </c>
-      <c r="V50" s="111">
+      <c r="V50" s="88">
         <v>5.8788297464031098E-3</v>
       </c>
-      <c r="W50" s="110"/>
+      <c r="W50" s="90"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A53" s="106" t="s">
+      <c r="A53" s="107" t="s">
         <v>313</v>
       </c>
-      <c r="B53" s="106"/>
-      <c r="C53" s="106"/>
-      <c r="D53" s="106"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="106"/>
-      <c r="G53" s="106"/>
-      <c r="H53" s="106"/>
-      <c r="I53" s="106"/>
-      <c r="J53" s="106"/>
-      <c r="K53" s="106"/>
-      <c r="L53" s="106"/>
-      <c r="M53" s="106"/>
-      <c r="N53" s="106"/>
-      <c r="O53" s="106"/>
-      <c r="P53" s="106"/>
-      <c r="Q53" s="106"/>
-      <c r="R53" s="106"/>
-      <c r="S53" s="106"/>
+      <c r="B53" s="107"/>
+      <c r="C53" s="107"/>
+      <c r="D53" s="107"/>
+      <c r="E53" s="107"/>
+      <c r="F53" s="107"/>
+      <c r="G53" s="107"/>
+      <c r="H53" s="107"/>
+      <c r="I53" s="107"/>
+      <c r="J53" s="107"/>
+      <c r="K53" s="107"/>
+      <c r="L53" s="107"/>
+      <c r="M53" s="107"/>
+      <c r="N53" s="107"/>
+      <c r="O53" s="107"/>
+      <c r="P53" s="107"/>
+      <c r="Q53" s="107"/>
+      <c r="R53" s="107"/>
+      <c r="S53" s="107"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A55" s="103" t="s">
+      <c r="A55" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="B55" s="103"/>
-      <c r="C55" s="103"/>
-      <c r="D55" s="103"/>
-      <c r="E55" s="103"/>
-      <c r="F55" s="103"/>
-      <c r="G55" s="103"/>
-      <c r="H55" s="103"/>
-      <c r="I55" s="103"/>
-      <c r="K55" s="103" t="s">
+      <c r="B55" s="106"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="106"/>
+      <c r="E55" s="106"/>
+      <c r="F55" s="106"/>
+      <c r="G55" s="106"/>
+      <c r="H55" s="106"/>
+      <c r="I55" s="106"/>
+      <c r="K55" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="L55" s="103"/>
-      <c r="M55" s="103"/>
-      <c r="N55" s="103"/>
-      <c r="O55" s="103"/>
-      <c r="P55" s="103"/>
-      <c r="Q55" s="103"/>
-      <c r="R55" s="103"/>
-      <c r="S55" s="103"/>
+      <c r="L55" s="106"/>
+      <c r="M55" s="106"/>
+      <c r="N55" s="106"/>
+      <c r="O55" s="106"/>
+      <c r="P55" s="106"/>
+      <c r="Q55" s="106"/>
+      <c r="R55" s="106"/>
+      <c r="S55" s="106"/>
     </row>
     <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5291,28 +5309,28 @@
       <c r="Q63" s="73"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A65" s="103" t="s">
+      <c r="A65" s="106" t="s">
         <v>315</v>
       </c>
-      <c r="B65" s="103"/>
-      <c r="C65" s="103"/>
-      <c r="D65" s="103"/>
-      <c r="E65" s="103"/>
-      <c r="F65" s="103"/>
-      <c r="G65" s="103"/>
-      <c r="H65" s="103"/>
-      <c r="I65" s="103"/>
-      <c r="K65" s="103" t="s">
+      <c r="B65" s="106"/>
+      <c r="C65" s="106"/>
+      <c r="D65" s="106"/>
+      <c r="E65" s="106"/>
+      <c r="F65" s="106"/>
+      <c r="G65" s="106"/>
+      <c r="H65" s="106"/>
+      <c r="I65" s="106"/>
+      <c r="K65" s="106" t="s">
         <v>315</v>
       </c>
-      <c r="L65" s="103"/>
-      <c r="M65" s="103"/>
-      <c r="N65" s="103"/>
-      <c r="O65" s="103"/>
-      <c r="P65" s="103"/>
-      <c r="Q65" s="103"/>
-      <c r="R65" s="103"/>
-      <c r="S65" s="103"/>
+      <c r="L65" s="106"/>
+      <c r="M65" s="106"/>
+      <c r="N65" s="106"/>
+      <c r="O65" s="106"/>
+      <c r="P65" s="106"/>
+      <c r="Q65" s="106"/>
+      <c r="R65" s="106"/>
+      <c r="S65" s="106"/>
     </row>
     <row r="66" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5464,13 +5482,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K65:S65"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="K42:S42"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="K55:S55"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="K31:S31"/>
     <mergeCell ref="A9:I9"/>
@@ -5479,6 +5490,13 @@
     <mergeCell ref="K11:S11"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="K21:S21"/>
+    <mergeCell ref="K65:S65"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="K42:S42"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K55:S55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5511,20 +5529,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="102" t="s">
+      <c r="A3" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="102"/>
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="105"/>
+      <c r="E3" s="105"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -5704,8 +5722,8 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5845,10 +5863,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="H10" s="107" t="s">
+      <c r="H10" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="I10" s="107"/>
+      <c r="I10" s="110"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5859,8 +5877,8 @@
       <c r="F11" s="28">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="110"/>
       <c r="L11" s="35"/>
       <c r="N11" s="35"/>
     </row>
@@ -5877,8 +5895,8 @@
       <c r="F12" s="28">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
+      <c r="H12" s="110"/>
+      <c r="I12" s="110"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5894,8 +5912,8 @@
       <c r="F13" s="49">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
       <c r="L13" s="35"/>
       <c r="N13" s="35"/>
     </row>
@@ -6063,8 +6081,8 @@
       <c r="E33" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="92"/>
-      <c r="I33" s="92"/>
+      <c r="H33" s="95"/>
+      <c r="I33" s="95"/>
       <c r="L33" s="35"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6072,10 +6090,10 @@
         <v>290</v>
       </c>
       <c r="O34" s="79"/>
-      <c r="P34" s="92" t="s">
+      <c r="P34" s="95" t="s">
         <v>280</v>
       </c>
-      <c r="Q34" s="92"/>
+      <c r="Q34" s="95"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
@@ -6205,10 +6223,10 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="F40" s="28"/>
-      <c r="H40" s="107" t="s">
+      <c r="H40" s="110" t="s">
         <v>293</v>
       </c>
-      <c r="I40" s="107"/>
+      <c r="I40" s="110"/>
       <c r="K40" t="s">
         <v>288</v>
       </c>
@@ -6226,8 +6244,8 @@
       <c r="F41" s="28">
         <v>1.365048</v>
       </c>
-      <c r="H41" s="107"/>
-      <c r="I41" s="107"/>
+      <c r="H41" s="110"/>
+      <c r="I41" s="110"/>
       <c r="K41" t="s">
         <v>289</v>
       </c>
@@ -6240,8 +6258,8 @@
       <c r="F42" s="28">
         <v>-0.3439432</v>
       </c>
-      <c r="H42" s="107"/>
-      <c r="I42" s="107"/>
+      <c r="H42" s="110"/>
+      <c r="I42" s="110"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="35">
@@ -6256,8 +6274,8 @@
       <c r="F43" s="49">
         <v>13.51919</v>
       </c>
-      <c r="H43" s="107"/>
-      <c r="I43" s="107"/>
+      <c r="H43" s="110"/>
+      <c r="I43" s="110"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44" s="35">
@@ -6694,10 +6712,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:I33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6709,6 +6727,14 @@
     <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>140</v>
@@ -6747,69 +6773,51 @@
       <c r="B6" s="35">
         <v>0.01</v>
       </c>
-      <c r="C6" s="9">
-        <v>-1.357559</v>
-      </c>
+      <c r="C6" s="9"/>
       <c r="E6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="47">
-        <v>744</v>
-      </c>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="35">
         <v>0.05</v>
       </c>
-      <c r="C7" s="9">
-        <v>-0.38607930000000001</v>
-      </c>
+      <c r="C7" s="9"/>
       <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="48">
-        <v>744</v>
-      </c>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="35">
         <v>0.1</v>
       </c>
-      <c r="C8" s="9">
-        <v>-0.26557120000000001</v>
-      </c>
+      <c r="C8" s="9"/>
       <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35">
         <v>0.25</v>
       </c>
-      <c r="C9" s="9">
-        <v>-8.2062300000000005E-2</v>
-      </c>
+      <c r="C9" s="9"/>
       <c r="E9" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="28">
-        <v>0.22691549999999999</v>
-      </c>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="28">
-        <v>1.390266</v>
-      </c>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="35">
         <v>0.5</v>
       </c>
-      <c r="C11" s="9">
-        <v>7.4287500000000006E-2</v>
-      </c>
+      <c r="C11" s="9"/>
       <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -6817,53 +6825,39 @@
       <c r="E12" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="28">
-        <v>1.932839</v>
-      </c>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="35">
         <v>0.75</v>
       </c>
-      <c r="C13" s="9">
-        <v>0.23517479999999999</v>
-      </c>
+      <c r="C13" s="9"/>
       <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="28">
-        <v>8.7551120000000004</v>
-      </c>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="35">
         <v>0.9</v>
       </c>
-      <c r="C14" s="9">
-        <v>0.57731120000000002</v>
-      </c>
+      <c r="C14" s="9"/>
       <c r="E14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="49">
-        <v>102.45529999999999</v>
-      </c>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="35">
         <v>0.95</v>
       </c>
-      <c r="C15" s="9">
-        <v>1.1694340000000001</v>
-      </c>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="45">
         <v>0.99</v>
       </c>
-      <c r="C16" s="46">
-        <v>5.8520029999999998</v>
-      </c>
+      <c r="C16" s="46"/>
     </row>
     <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -6904,38 +6898,28 @@
       <c r="B22" s="35">
         <v>0.01</v>
       </c>
-      <c r="C22" s="9">
-        <v>-2.9382799999999998</v>
-      </c>
+      <c r="C22" s="9"/>
       <c r="E22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="47">
-        <v>912</v>
-      </c>
+      <c r="F22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="35">
         <v>0.05</v>
       </c>
-      <c r="C23" s="9">
-        <v>-1.2431639999999999</v>
-      </c>
+      <c r="C23" s="9"/>
       <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="48">
-        <v>912</v>
-      </c>
+      <c r="F23" s="48"/>
       <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="35">
         <v>0.1</v>
       </c>
-      <c r="C24" s="9">
-        <v>-0.64895800000000003</v>
-      </c>
+      <c r="C24" s="9"/>
       <c r="F24" s="28"/>
       <c r="I24" s="35"/>
     </row>
@@ -6943,15 +6927,11 @@
       <c r="B25" s="35">
         <v>0.25</v>
       </c>
-      <c r="C25" s="9">
-        <v>-9.5295599999999994E-2</v>
-      </c>
+      <c r="C25" s="9"/>
       <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="28">
-        <v>0.3211851</v>
-      </c>
+      <c r="F25" s="28"/>
       <c r="I25" s="35"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -6959,18 +6939,14 @@
       <c r="E26" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="28">
-        <v>1.20275</v>
-      </c>
+      <c r="F26" s="28"/>
       <c r="I26" s="35"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="35">
         <v>0.5</v>
       </c>
-      <c r="C27" s="9">
-        <v>0.1865655</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -6978,62 +6954,51 @@
       <c r="E28" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="28">
-        <v>1.446607</v>
-      </c>
+      <c r="F28" s="28"/>
       <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
         <v>0.75</v>
       </c>
-      <c r="C29" s="9">
-        <v>0.57733040000000002</v>
-      </c>
+      <c r="C29" s="9"/>
       <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="28">
-        <v>1.274227</v>
-      </c>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="35">
         <v>0.9</v>
       </c>
-      <c r="C30" s="9">
-        <v>1.4211590000000001</v>
-      </c>
+      <c r="C30" s="9"/>
       <c r="E30" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="49">
-        <v>9.5781530000000004</v>
-      </c>
+      <c r="F30" s="49"/>
       <c r="I30" s="35"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="35">
         <v>0.95</v>
       </c>
-      <c r="C31" s="9">
-        <v>2.3540019999999999</v>
-      </c>
+      <c r="C31" s="9"/>
       <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="45">
         <v>0.99</v>
       </c>
-      <c r="C32" s="46">
-        <v>5.2469239999999999</v>
-      </c>
+      <c r="C32" s="46"/>
       <c r="I32" s="35"/>
     </row>
     <row r="33" spans="9:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I33" s="35"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7647,10 +7612,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:D19"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7666,7 +7631,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -7676,26 +7641,20 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="96"/>
+      <c r="D4" s="96"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
-        <v>3</v>
+        <v>316</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>6</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -7705,12 +7664,6 @@
       <c r="B7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
@@ -7719,12 +7672,6 @@
       <c r="B8" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
@@ -7733,12 +7680,6 @@
       <c r="B9" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
@@ -7747,12 +7688,6 @@
       <c r="B10" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
@@ -7761,12 +7696,6 @@
       <c r="B11" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
@@ -7775,12 +7704,6 @@
       <c r="B12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
@@ -7789,12 +7712,6 @@
       <c r="B13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
@@ -7803,12 +7720,6 @@
       <c r="B14" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -7817,12 +7728,6 @@
       <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
@@ -7831,42 +7736,128 @@
       <c r="B16" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>170</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="C18" s="22" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D18" s="22" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
@@ -7880,7 +7871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -8245,66 +8236,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="89" t="s">
+      <c r="B1" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="92" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="N1" s="89" t="s">
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="N1" s="92" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="T1" s="89" t="s">
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="T1" s="92" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="90"/>
-      <c r="L2" s="90"/>
-      <c r="N2" s="90" t="s">
+      <c r="I2" s="93"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93"/>
+      <c r="N2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="90"/>
-      <c r="T2" s="90" t="s">
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="T2" s="93" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="91"/>
-      <c r="V2" s="91"/>
-      <c r="W2" s="91"/>
-      <c r="X2" s="91"/>
+      <c r="U2" s="94"/>
+      <c r="V2" s="94"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -9339,10 +9330,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="92" t="s">
+      <c r="B2" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="92"/>
+      <c r="C2" s="95"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -9877,13 +9868,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -9997,12 +9988,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="94" t="s">
+      <c r="A10" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -10301,12 +10292,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="97" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="94"/>
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -10640,13 +10631,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -10884,13 +10875,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="96" t="s">
+      <c r="A21" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="96"/>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -10918,13 +10909,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="95" t="s">
+      <c r="A25" s="98" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="95"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
-      <c r="E25" s="95"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="98"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -11186,13 +11177,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="96" t="s">
+      <c r="A43" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="96"/>
-      <c r="C43" s="96"/>
-      <c r="D43" s="96"/>
-      <c r="E43" s="96"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="99"/>
+      <c r="E43" s="99"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -11560,36 +11551,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="97"/>
-      <c r="C3" s="97"/>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="100"/>
+      <c r="R3" s="100"/>
+      <c r="S3" s="100"/>
+      <c r="T3" s="100"/>
+      <c r="U3" s="100"/>
+      <c r="V3" s="100"/>
+      <c r="W3" s="100"/>
+      <c r="X3" s="100"/>
+      <c r="Y3" s="100"/>
+      <c r="Z3" s="100"/>
+      <c r="AA3" s="100"/>
+      <c r="AB3" s="100"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -12108,35 +12099,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="101" t="s">
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="101"/>
-      <c r="G4" s="101"/>
-      <c r="H4" s="101"/>
-      <c r="I4" s="101"/>
-      <c r="J4" s="101"/>
-      <c r="K4" s="98" t="s">
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="101" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="99" t="s">
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="99"/>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="99"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="102"/>
+      <c r="R4" s="102"/>
+      <c r="S4" s="102"/>
+      <c r="T4" s="102"/>
+      <c r="U4" s="102"/>
+      <c r="V4" s="102"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>

<commit_message>
Updated main results to reflect a2 definition
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C04228-FA08-4B5E-AE29-D8B2DE2852FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840BC064-4BB9-413E-A0C9-E49E799A6DF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="10" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="12" activeTab="15" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="320">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1107,6 +1107,18 @@
   </si>
   <si>
     <t>No routine, definition 2</t>
+  </si>
+  <si>
+    <t>A. Manual</t>
+  </si>
+  <si>
+    <t>B. Social</t>
+  </si>
+  <si>
+    <t>C. Adaptability</t>
+  </si>
+  <si>
+    <t>D. Abstract</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1242,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1312,6 +1324,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1417,7 +1435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1648,6 +1666,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2484,8 +2505,8 @@
   </sheetPr>
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3847,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
   <dimension ref="A2:W73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" topLeftCell="E26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4070,33 +4091,21 @@
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="D15" s="73">
-        <f>-H15</f>
-        <v>-1.9824513343154201E-2</v>
+      <c r="D15" s="73" t="str">
+        <f>+IF(M17=0,"",M17)</f>
+        <v/>
       </c>
       <c r="E15" s="73">
-        <f t="shared" ref="E15:G15" si="0">-I15</f>
-        <v>-7.3337925396310899E-2</v>
+        <f t="shared" ref="E15:G15" si="0">+IF(N17=0,"",N17)</f>
+        <v>-1.80163841799885E-2</v>
       </c>
       <c r="F15" s="73">
         <f t="shared" si="0"/>
-        <v>-8.4175794644333599E-2</v>
+        <v>-7.3981842197322401E-2</v>
       </c>
       <c r="G15" s="73">
         <f t="shared" si="0"/>
-        <v>-7.0869425551512197E-2</v>
-      </c>
-      <c r="H15">
-        <v>1.9824513343154201E-2</v>
-      </c>
-      <c r="I15">
-        <v>7.3337925396310899E-2</v>
-      </c>
-      <c r="J15">
-        <v>8.4175794644333599E-2</v>
-      </c>
-      <c r="K15">
-        <v>7.0869425551512197E-2</v>
+        <v>-7.6118564642824793E-2</v>
       </c>
       <c r="N15" s="73">
         <f>-S15</f>
@@ -4160,48 +4169,24 @@
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="D17" s="73">
-        <f>-H17</f>
-        <v>-1.9824513343154201E-2</v>
-      </c>
-      <c r="E17" s="73">
-        <f t="shared" ref="E17:G17" si="2">-I17</f>
-        <v>-6.8502347913652506E-2</v>
-      </c>
-      <c r="F17" s="73">
-        <f t="shared" si="2"/>
-        <v>-8.4504659408050506E-2</v>
-      </c>
-      <c r="G17" s="73">
-        <f t="shared" si="2"/>
-        <v>-8.3651740784867104E-2</v>
-      </c>
-      <c r="H17">
-        <v>1.9824513343154201E-2</v>
-      </c>
-      <c r="I17">
-        <v>6.8502347913652506E-2</v>
-      </c>
-      <c r="J17">
-        <v>8.4504659408050506E-2</v>
-      </c>
-      <c r="K17">
-        <v>8.3651740784867104E-2</v>
-      </c>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
       <c r="N17" s="73">
         <f>-S17</f>
         <v>-1.80163841799885E-2</v>
       </c>
       <c r="O17" s="73">
-        <f t="shared" ref="O17:Q17" si="3">-T17</f>
+        <f t="shared" ref="O17:Q17" si="2">-T17</f>
         <v>-7.3981842197322401E-2</v>
       </c>
       <c r="P17" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-7.6118564642824793E-2</v>
       </c>
       <c r="Q17" s="73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-7.8421126834552699E-2</v>
       </c>
       <c r="S17">
@@ -4251,33 +4236,21 @@
     </row>
     <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="19"/>
-      <c r="D19" s="74">
-        <f>-H19</f>
-        <v>-1.9824513343154201E-2</v>
+      <c r="D19" s="74" t="str">
+        <f>+IF(M19=0,"",M19)</f>
+        <v/>
       </c>
       <c r="E19" s="74">
-        <f t="shared" ref="E19:G19" si="4">-I19</f>
-        <v>-7.8151917060514706E-2</v>
+        <f t="shared" ref="E19:G19" si="3">+IF(N19=0,"",N19)</f>
+        <v>-1.80163841799885E-2</v>
       </c>
       <c r="F19" s="74">
-        <f t="shared" si="4"/>
-        <v>-8.1556156708327401E-2</v>
+        <f t="shared" si="3"/>
+        <v>-6.4554005463114295E-2</v>
       </c>
       <c r="G19" s="74">
-        <f t="shared" si="4"/>
-        <v>-4.9714630821618101E-3</v>
-      </c>
-      <c r="H19">
-        <v>1.9824513343154201E-2</v>
-      </c>
-      <c r="I19">
-        <v>7.8151917060514706E-2</v>
-      </c>
-      <c r="J19">
-        <v>8.1556156708327401E-2</v>
-      </c>
-      <c r="K19">
-        <v>4.9714630821618101E-3</v>
+        <f t="shared" si="3"/>
+        <v>-6.6745927637415006E-2</v>
       </c>
       <c r="M19" s="19"/>
       <c r="N19" s="74">
@@ -4285,15 +4258,15 @@
         <v>-1.80163841799885E-2</v>
       </c>
       <c r="O19" s="74">
-        <f t="shared" ref="O19:Q19" si="5">-T19</f>
+        <f t="shared" ref="O19:Q19" si="4">-T19</f>
         <v>-6.4554005463114295E-2</v>
       </c>
       <c r="P19" s="74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-6.6745927637415006E-2</v>
       </c>
       <c r="Q19" s="74">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-5.3873187988552002E-3</v>
       </c>
       <c r="S19">
@@ -4321,17 +4294,17 @@
       <c r="G21" s="106"/>
       <c r="H21" s="106"/>
       <c r="I21" s="106"/>
-      <c r="K21" s="106" t="s">
+      <c r="K21" s="111" t="s">
         <v>310</v>
       </c>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="106"/>
-      <c r="O21" s="106"/>
-      <c r="P21" s="106"/>
-      <c r="Q21" s="106"/>
-      <c r="R21" s="106"/>
-      <c r="S21" s="106"/>
+      <c r="L21" s="111"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+      <c r="R21" s="111"/>
+      <c r="S21" s="111"/>
     </row>
     <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4399,48 +4372,36 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="D25" s="73">
-        <f>-H25</f>
-        <v>-2.00128377538078E-2</v>
+      <c r="D25" s="73" t="str">
+        <f>+IF(M27=0,"",M27)</f>
+        <v/>
       </c>
       <c r="E25" s="73">
-        <f t="shared" ref="E25:G25" si="6">-I25</f>
-        <v>-7.3925691515197997E-2</v>
+        <f t="shared" ref="E25" si="5">+IF(N27=0,"",N27)</f>
+        <v>-1.8232139167409501E-2</v>
       </c>
       <c r="F25" s="73">
-        <f t="shared" si="6"/>
-        <v>-8.1053378650391694E-2</v>
+        <f t="shared" ref="F25" si="6">+IF(O27=0,"",O27)</f>
+        <v>-7.4363070184416902E-2</v>
       </c>
       <c r="G25" s="73">
-        <f t="shared" si="6"/>
-        <v>-6.6767345006274001E-2</v>
-      </c>
-      <c r="H25">
-        <v>2.00128377538078E-2</v>
-      </c>
-      <c r="I25">
-        <v>7.3925691515197997E-2</v>
-      </c>
-      <c r="J25">
-        <v>8.1053378650391694E-2</v>
-      </c>
-      <c r="K25">
-        <v>6.6767345006274001E-2</v>
+        <f t="shared" ref="G25" si="7">+IF(P27=0,"",P27)</f>
+        <v>-7.3014723185476305E-2</v>
       </c>
       <c r="N25" s="73">
         <f>-S25</f>
         <v>-1.8232139167409501E-2</v>
       </c>
       <c r="O25" s="73">
-        <f t="shared" ref="O25:Q25" si="7">-T25</f>
+        <f t="shared" ref="O25:Q25" si="8">-T25</f>
         <v>-6.2705340586680203E-2</v>
       </c>
       <c r="P25" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-6.0532147295976703E-2</v>
       </c>
       <c r="Q25" s="73">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>-6.79552860893851E-2</v>
       </c>
       <c r="S25">
@@ -4489,34 +4450,10 @@
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="D27" s="73">
-        <f>-H27</f>
-        <v>-2.00128377538078E-2</v>
-      </c>
-      <c r="E27" s="73">
-        <f t="shared" ref="E27:G27" si="8">-I27</f>
-        <v>-6.8455439714427802E-2</v>
-      </c>
-      <c r="F27" s="73">
-        <f t="shared" si="8"/>
-        <v>-8.1332811762689305E-2</v>
-      </c>
-      <c r="G27" s="73">
-        <f t="shared" si="8"/>
-        <v>-8.05281988916981E-2</v>
-      </c>
-      <c r="H27">
-        <v>2.00128377538078E-2</v>
-      </c>
-      <c r="I27">
-        <v>6.8455439714427802E-2</v>
-      </c>
-      <c r="J27">
-        <v>8.1332811762689305E-2</v>
-      </c>
-      <c r="K27">
-        <v>8.05281988916981E-2</v>
-      </c>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="N27" s="73">
         <f>-S27</f>
         <v>-1.8232139167409501E-2</v>
@@ -4580,33 +4517,21 @@
     </row>
     <row r="29" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="19"/>
-      <c r="D29" s="74">
-        <f>-H29</f>
-        <v>-2.00128377538078E-2</v>
+      <c r="D29" s="74" t="str">
+        <f>+IF(M29=0,"",M29)</f>
+        <v/>
       </c>
       <c r="E29" s="74">
-        <f t="shared" ref="E29:G29" si="10">-I29</f>
-        <v>-7.8311238676915501E-2</v>
+        <f t="shared" ref="E29" si="10">+IF(N29=0,"",N29)</f>
+        <v>-1.8232139167409501E-2</v>
       </c>
       <c r="F29" s="74">
-        <f t="shared" si="10"/>
-        <v>-8.1763058847982101E-2</v>
+        <f t="shared" ref="F29" si="11">+IF(O29=0,"",O29)</f>
+        <v>-6.4688998413530194E-2</v>
       </c>
       <c r="G29" s="74">
-        <f t="shared" si="10"/>
-        <v>-5.35045409069495E-3</v>
-      </c>
-      <c r="H29">
-        <v>2.00128377538078E-2</v>
-      </c>
-      <c r="I29">
-        <v>7.8311238676915501E-2</v>
-      </c>
-      <c r="J29">
-        <v>8.1763058847982101E-2</v>
-      </c>
-      <c r="K29">
-        <v>5.35045409069495E-3</v>
+        <f t="shared" ref="G29" si="12">+IF(P29=0,"",P29)</f>
+        <v>-6.6984637221420507E-2</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="74">
@@ -4614,15 +4539,15 @@
         <v>-1.8232139167409501E-2</v>
       </c>
       <c r="O29" s="74">
-        <f t="shared" ref="O29:Q29" si="11">-T29</f>
+        <f t="shared" ref="O29:Q29" si="13">-T29</f>
         <v>-6.4688998413530194E-2</v>
       </c>
       <c r="P29" s="74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-6.6984637221420507E-2</v>
       </c>
       <c r="Q29" s="74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-5.8788297464031098E-3</v>
       </c>
       <c r="S29">
@@ -4728,44 +4653,32 @@
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D35" s="73">
-        <f>-H35</f>
-        <v>-2.0235567234909199E-2</v>
+      <c r="D35" s="73" t="str">
+        <f>+IF(M37=0,"",M37)</f>
+        <v/>
       </c>
       <c r="E35" s="73">
-        <f t="shared" ref="E35:G35" si="12">-I35</f>
-        <v>-7.5552651728106296E-2</v>
+        <f t="shared" ref="E35" si="14">+IF(N37=0,"",N37)</f>
+        <v>-1.8593580225319199E-2</v>
       </c>
       <c r="F35" s="73">
-        <f t="shared" si="12"/>
-        <v>-7.8481015659589495E-2</v>
+        <f t="shared" ref="F35" si="15">+IF(O37=0,"",O37)</f>
+        <v>-7.7697154041311306E-2</v>
       </c>
       <c r="G35" s="73">
-        <f t="shared" si="12"/>
-        <v>-6.1029708840424898E-2</v>
-      </c>
-      <c r="H35">
-        <v>2.0235567234909199E-2</v>
-      </c>
-      <c r="I35">
-        <v>7.5552651728106296E-2</v>
-      </c>
-      <c r="J35">
-        <v>7.8481015659589495E-2</v>
-      </c>
-      <c r="K35">
-        <v>6.1029708840424898E-2</v>
+        <f t="shared" ref="G35" si="16">+IF(P37=0,"",P37)</f>
+        <v>-7.0698211707042102E-2</v>
       </c>
       <c r="N35" s="73">
         <f>-S35</f>
         <v>-1.8593580225319199E-2</v>
       </c>
       <c r="O35" s="73">
-        <f t="shared" ref="O35:P35" si="13">-T35</f>
+        <f t="shared" ref="O35:P35" si="17">-T35</f>
         <v>-6.6121303110595497E-2</v>
       </c>
       <c r="P35" s="73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-5.7998508062290899E-2</v>
       </c>
       <c r="Q35" s="73">
@@ -4818,48 +4731,24 @@
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="D37" s="73">
-        <f>-H37</f>
-        <v>-2.0235567234909199E-2</v>
-      </c>
-      <c r="E37" s="73">
-        <f t="shared" ref="E37:G37" si="14">-I37</f>
-        <v>-6.9992651510969103E-2</v>
-      </c>
-      <c r="F37" s="73">
-        <f t="shared" si="14"/>
-        <v>-7.7099892551743293E-2</v>
-      </c>
-      <c r="G37" s="73">
-        <f t="shared" si="14"/>
-        <v>-7.8626651379215096E-2</v>
-      </c>
-      <c r="H37">
-        <v>2.0235567234909199E-2</v>
-      </c>
-      <c r="I37">
-        <v>6.9992651510969103E-2</v>
-      </c>
-      <c r="J37">
-        <v>7.7099892551743293E-2</v>
-      </c>
-      <c r="K37">
-        <v>7.8626651379215096E-2</v>
-      </c>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
       <c r="N37" s="73">
         <f>-S37</f>
         <v>-1.8593580225319199E-2</v>
       </c>
       <c r="O37" s="73">
-        <f t="shared" ref="O37:Q37" si="15">-T37</f>
+        <f t="shared" ref="O37:Q37" si="18">-T37</f>
         <v>-7.7697154041311306E-2</v>
       </c>
       <c r="P37" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-7.0698211707042102E-2</v>
       </c>
       <c r="Q37" s="73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>-7.1608927235836894E-2</v>
       </c>
       <c r="S37">
@@ -4909,33 +4798,21 @@
     </row>
     <row r="39" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C39" s="19"/>
-      <c r="D39" s="74">
-        <f>-H39</f>
-        <v>-2.0235567234909199E-2</v>
+      <c r="D39" s="74" t="str">
+        <f>+IF(M39=0,"",M39)</f>
+        <v/>
       </c>
       <c r="E39" s="74">
-        <f t="shared" ref="E39:G39" si="16">-I39</f>
-        <v>-7.8220484531113396E-2</v>
+        <f t="shared" ref="E39" si="19">+IF(N39=0,"",N39)</f>
+        <v>-1.8593580225319199E-2</v>
       </c>
       <c r="F39" s="74">
-        <f t="shared" si="16"/>
-        <v>-8.15621610602935E-2</v>
+        <f t="shared" ref="F39" si="20">+IF(O39=0,"",O39)</f>
+        <v>-6.4659214976102206E-2</v>
       </c>
       <c r="G39" s="74">
-        <f t="shared" si="16"/>
-        <v>-5.86398043718569E-3</v>
-      </c>
-      <c r="H39">
-        <v>2.0235567234909199E-2</v>
-      </c>
-      <c r="I39">
-        <v>7.8220484531113396E-2</v>
-      </c>
-      <c r="J39">
-        <v>8.15621610602935E-2</v>
-      </c>
-      <c r="K39">
-        <v>5.86398043718569E-3</v>
+        <f t="shared" ref="G39" si="21">+IF(P39=0,"",P39)</f>
+        <v>-6.7086317193334202E-2</v>
       </c>
       <c r="M39" s="19"/>
       <c r="N39" s="74">
@@ -4943,15 +4820,15 @@
         <v>-1.8593580225319199E-2</v>
       </c>
       <c r="O39" s="74">
-        <f t="shared" ref="O39:Q39" si="17">-T39</f>
+        <f t="shared" ref="O39:Q39" si="22">-T39</f>
         <v>-6.4659214976102206E-2</v>
       </c>
       <c r="P39" s="74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-6.7086317193334202E-2</v>
       </c>
       <c r="Q39" s="74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>-6.7079383018708201E-3</v>
       </c>
       <c r="S39">
@@ -5064,15 +4941,15 @@
         <v>-1.8232139167409501E-2</v>
       </c>
       <c r="O46" s="88">
-        <f t="shared" ref="O46:Q46" si="18">-T46</f>
+        <f t="shared" ref="O46:Q46" si="23">-T46</f>
         <v>-6.2705340586680203E-2</v>
       </c>
       <c r="P46" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>-6.0532147295976703E-2</v>
       </c>
       <c r="Q46" s="88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>-6.79552860893851E-2</v>
       </c>
       <c r="R46" s="90"/>
@@ -5130,15 +5007,15 @@
         <v>-1.8232139167409501E-2</v>
       </c>
       <c r="O48" s="88">
-        <f t="shared" ref="O48:Q48" si="19">-T48</f>
+        <f t="shared" ref="O48:Q48" si="24">-T48</f>
         <v>-7.4363070184416902E-2</v>
       </c>
       <c r="P48" s="88">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>-7.3014723185476305E-2</v>
       </c>
       <c r="Q48" s="88">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>-7.1882201893921804E-2</v>
       </c>
       <c r="R48" s="90"/>
@@ -5192,24 +5069,33 @@
         <f>+IF(M50=0,"",M50)</f>
         <v/>
       </c>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
+      <c r="E50" s="74">
+        <f t="shared" ref="E50" si="25">+IF(N50=0,"",N50)</f>
+        <v>-1.8232139167409501E-2</v>
+      </c>
+      <c r="F50" s="74">
+        <f t="shared" ref="F50" si="26">+IF(O50=0,"",O50)</f>
+        <v>-6.4688998413530194E-2</v>
+      </c>
+      <c r="G50" s="74">
+        <f t="shared" ref="G50" si="27">+IF(P50=0,"",P50)</f>
+        <v>-6.6984637221420507E-2</v>
+      </c>
       <c r="M50" s="19"/>
       <c r="N50" s="89">
         <f>-S50</f>
         <v>-1.8232139167409501E-2</v>
       </c>
       <c r="O50" s="89">
-        <f t="shared" ref="O50:Q50" si="20">-T50</f>
+        <f t="shared" ref="O50:Q50" si="28">-T50</f>
         <v>-6.4688998413530194E-2</v>
       </c>
       <c r="P50" s="89">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>-6.6984637221420507E-2</v>
       </c>
       <c r="Q50" s="89">
-        <f t="shared" si="20"/>
+        <f t="shared" si="28"/>
         <v>-5.8788297464031098E-3</v>
       </c>
       <c r="R50" s="90"/>
@@ -5396,15 +5282,15 @@
         <v/>
       </c>
       <c r="E63" s="74" t="str">
-        <f t="shared" ref="E63" si="21">+IF(N63=0,"",N63)</f>
+        <f t="shared" ref="E63" si="29">+IF(N63=0,"",N63)</f>
         <v/>
       </c>
       <c r="F63" s="74" t="str">
-        <f t="shared" ref="F63" si="22">+IF(O63=0,"",O63)</f>
+        <f t="shared" ref="F63" si="30">+IF(O63=0,"",O63)</f>
         <v/>
       </c>
       <c r="G63" s="73" t="str">
-        <f t="shared" ref="G63" si="23">+IF(P63=0,"",P63)</f>
+        <f t="shared" ref="G63" si="31">+IF(P63=0,"",P63)</f>
         <v/>
       </c>
       <c r="M63" s="19"/>
@@ -5413,11 +5299,11 @@
         <v/>
       </c>
       <c r="O63" s="74" t="str">
-        <f t="shared" ref="O63" si="24">+IF(X63=0,"",X63)</f>
+        <f t="shared" ref="O63" si="32">+IF(X63=0,"",X63)</f>
         <v/>
       </c>
       <c r="P63" s="74" t="str">
-        <f t="shared" ref="P63" si="25">+IF(Y63=0,"",Y63)</f>
+        <f t="shared" ref="P63" si="33">+IF(Y63=0,"",Y63)</f>
         <v/>
       </c>
       <c r="Q63" s="73"/>
@@ -5568,15 +5454,15 @@
         <v/>
       </c>
       <c r="E73" s="74" t="str">
-        <f t="shared" ref="E73" si="26">+IF(N73=0,"",N73)</f>
+        <f t="shared" ref="E73" si="34">+IF(N73=0,"",N73)</f>
         <v/>
       </c>
       <c r="F73" s="74" t="str">
-        <f t="shared" ref="F73" si="27">+IF(O73=0,"",O73)</f>
+        <f t="shared" ref="F73" si="35">+IF(O73=0,"",O73)</f>
         <v/>
       </c>
       <c r="G73" s="73" t="str">
-        <f t="shared" ref="G73" si="28">+IF(P73=0,"",P73)</f>
+        <f t="shared" ref="G73" si="36">+IF(P73=0,"",P73)</f>
         <v/>
       </c>
       <c r="M73" s="19"/>
@@ -5585,11 +5471,11 @@
         <v/>
       </c>
       <c r="O73" s="74" t="str">
-        <f t="shared" ref="O73" si="29">+IF(X73=0,"",X73)</f>
+        <f t="shared" ref="O73" si="37">+IF(X73=0,"",X73)</f>
         <v/>
       </c>
       <c r="P73" s="74" t="str">
-        <f t="shared" ref="P73" si="30">+IF(Y73=0,"",Y73)</f>
+        <f t="shared" ref="P73" si="38">+IF(Y73=0,"",Y73)</f>
         <v/>
       </c>
       <c r="Q73" s="73"/>
@@ -5836,8 +5722,8 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6826,10 +6712,10 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A2:I33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+    <sheetView showGridLines="0" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6841,6 +6727,14 @@
     <col min="6" max="6" width="6.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="95"/>
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+    </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>140</v>
@@ -6879,69 +6773,51 @@
       <c r="B6" s="35">
         <v>0.01</v>
       </c>
-      <c r="C6" s="9">
-        <v>-1.357559</v>
-      </c>
+      <c r="C6" s="9"/>
       <c r="E6" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="47">
-        <v>744</v>
-      </c>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="35">
         <v>0.05</v>
       </c>
-      <c r="C7" s="9">
-        <v>-0.38607930000000001</v>
-      </c>
+      <c r="C7" s="9"/>
       <c r="E7" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="48">
-        <v>744</v>
-      </c>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="35">
         <v>0.1</v>
       </c>
-      <c r="C8" s="9">
-        <v>-0.26557120000000001</v>
-      </c>
+      <c r="C8" s="9"/>
       <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="35">
         <v>0.25</v>
       </c>
-      <c r="C9" s="9">
-        <v>-8.2062300000000005E-2</v>
-      </c>
+      <c r="C9" s="9"/>
       <c r="E9" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="28">
-        <v>0.22691549999999999</v>
-      </c>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" s="9"/>
       <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="28">
-        <v>1.390266</v>
-      </c>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="35">
         <v>0.5</v>
       </c>
-      <c r="C11" s="9">
-        <v>7.4287500000000006E-2</v>
-      </c>
+      <c r="C11" s="9"/>
       <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -6949,53 +6825,39 @@
       <c r="E12" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="28">
-        <v>1.932839</v>
-      </c>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="35">
         <v>0.75</v>
       </c>
-      <c r="C13" s="9">
-        <v>0.23517479999999999</v>
-      </c>
+      <c r="C13" s="9"/>
       <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="F13" s="28">
-        <v>8.7551120000000004</v>
-      </c>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="35">
         <v>0.9</v>
       </c>
-      <c r="C14" s="9">
-        <v>0.57731120000000002</v>
-      </c>
+      <c r="C14" s="9"/>
       <c r="E14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="49">
-        <v>102.45529999999999</v>
-      </c>
+      <c r="F14" s="49"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="35">
         <v>0.95</v>
       </c>
-      <c r="C15" s="9">
-        <v>1.1694340000000001</v>
-      </c>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="45">
         <v>0.99</v>
       </c>
-      <c r="C16" s="46">
-        <v>5.8520029999999998</v>
-      </c>
+      <c r="C16" s="46"/>
     </row>
     <row r="17" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -7036,38 +6898,28 @@
       <c r="B22" s="35">
         <v>0.01</v>
       </c>
-      <c r="C22" s="9">
-        <v>-2.9382799999999998</v>
-      </c>
+      <c r="C22" s="9"/>
       <c r="E22" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="47">
-        <v>912</v>
-      </c>
+      <c r="F22" s="47"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B23" s="35">
         <v>0.05</v>
       </c>
-      <c r="C23" s="9">
-        <v>-1.2431639999999999</v>
-      </c>
+      <c r="C23" s="9"/>
       <c r="E23" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="48">
-        <v>912</v>
-      </c>
+      <c r="F23" s="48"/>
       <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B24" s="35">
         <v>0.1</v>
       </c>
-      <c r="C24" s="9">
-        <v>-0.64895800000000003</v>
-      </c>
+      <c r="C24" s="9"/>
       <c r="F24" s="28"/>
       <c r="I24" s="35"/>
     </row>
@@ -7075,15 +6927,11 @@
       <c r="B25" s="35">
         <v>0.25</v>
       </c>
-      <c r="C25" s="9">
-        <v>-9.5295599999999994E-2</v>
-      </c>
+      <c r="C25" s="9"/>
       <c r="E25" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="28">
-        <v>0.3211851</v>
-      </c>
+      <c r="F25" s="28"/>
       <c r="I25" s="35"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -7091,18 +6939,14 @@
       <c r="E26" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="28">
-        <v>1.20275</v>
-      </c>
+      <c r="F26" s="28"/>
       <c r="I26" s="35"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" s="35">
         <v>0.5</v>
       </c>
-      <c r="C27" s="9">
-        <v>0.1865655</v>
-      </c>
+      <c r="C27" s="9"/>
       <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -7110,62 +6954,51 @@
       <c r="E28" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="28">
-        <v>1.446607</v>
-      </c>
+      <c r="F28" s="28"/>
       <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
         <v>0.75</v>
       </c>
-      <c r="C29" s="9">
-        <v>0.57733040000000002</v>
-      </c>
+      <c r="C29" s="9"/>
       <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="28">
-        <v>1.274227</v>
-      </c>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="35">
         <v>0.9</v>
       </c>
-      <c r="C30" s="9">
-        <v>1.4211590000000001</v>
-      </c>
+      <c r="C30" s="9"/>
       <c r="E30" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F30" s="49">
-        <v>9.5781530000000004</v>
-      </c>
+      <c r="F30" s="49"/>
       <c r="I30" s="35"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" s="35">
         <v>0.95</v>
       </c>
-      <c r="C31" s="9">
-        <v>2.3540019999999999</v>
-      </c>
+      <c r="C31" s="9"/>
       <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="45">
         <v>0.99</v>
       </c>
-      <c r="C32" s="46">
-        <v>5.2469239999999999</v>
-      </c>
+      <c r="C32" s="46"/>
       <c r="I32" s="35"/>
     </row>
     <row r="33" spans="9:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I33" s="35"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7779,10 +7612,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A2:D19"/>
+  <dimension ref="A2:D32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7798,7 +7631,7 @@
         <v>140</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -7818,16 +7651,10 @@
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
-        <v>3</v>
+        <v>316</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>6</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -7837,12 +7664,6 @@
       <c r="B7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
@@ -7851,12 +7672,6 @@
       <c r="B8" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>164</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
@@ -7865,12 +7680,6 @@
       <c r="B9" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>152</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
@@ -7879,12 +7688,6 @@
       <c r="B10" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
@@ -7893,12 +7696,6 @@
       <c r="B11" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>167</v>
-      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
@@ -7907,12 +7704,6 @@
       <c r="B12" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>169</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
@@ -7921,12 +7712,6 @@
       <c r="B13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
@@ -7935,12 +7720,6 @@
       <c r="B14" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>204</v>
-      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
@@ -7949,12 +7728,6 @@
       <c r="B15" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>220</v>
-      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
@@ -7963,42 +7736,128 @@
       <c r="B16" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="22" t="s">
         <v>170</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="C18" s="22" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D18" s="22" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B31" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:D4"/>
@@ -8012,7 +7871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed standard errors for unconstrained manual
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BCE360-DC10-4415-A416-BDF99D161169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7480AE1-8563-4E8B-8F90-81D2B1999E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="5" activeTab="8" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
@@ -1680,6 +1680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1719,6 +1720,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1734,25 +1750,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2354,14 +2354,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="127" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2463,14 +2463,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="126" t="s">
+      <c r="A9" s="127" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="126"/>
-      <c r="C9" s="126"/>
-      <c r="D9" s="126"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2695,52 +2695,52 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="145" t="s">
+      <c r="A9" s="143" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="145"/>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="145"/>
-      <c r="G9" s="145"/>
-      <c r="H9" s="145"/>
-      <c r="I9" s="145"/>
-      <c r="K9" s="146" t="s">
+      <c r="B9" s="143"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="143"/>
+      <c r="E9" s="143"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="143"/>
+      <c r="H9" s="143"/>
+      <c r="I9" s="143"/>
+      <c r="K9" s="144" t="s">
         <v>277</v>
       </c>
-      <c r="L9" s="146"/>
-      <c r="M9" s="146"/>
-      <c r="N9" s="146"/>
-      <c r="O9" s="146"/>
-      <c r="P9" s="146"/>
-      <c r="Q9" s="146"/>
-      <c r="R9" s="146"/>
-      <c r="S9" s="146"/>
+      <c r="L9" s="144"/>
+      <c r="M9" s="144"/>
+      <c r="N9" s="144"/>
+      <c r="O9" s="144"/>
+      <c r="P9" s="144"/>
+      <c r="Q9" s="144"/>
+      <c r="R9" s="144"/>
+      <c r="S9" s="144"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="141" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="144"/>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="144"/>
-      <c r="F11" s="144"/>
-      <c r="G11" s="144"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="144"/>
-      <c r="K11" s="144" t="s">
+      <c r="B11" s="141"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="K11" s="141" t="s">
         <v>278</v>
       </c>
-      <c r="L11" s="144"/>
-      <c r="M11" s="144"/>
-      <c r="N11" s="144"/>
-      <c r="O11" s="144"/>
-      <c r="P11" s="144"/>
-      <c r="Q11" s="144"/>
-      <c r="R11" s="144"/>
-      <c r="S11" s="144"/>
+      <c r="L11" s="141"/>
+      <c r="M11" s="141"/>
+      <c r="N11" s="141"/>
+      <c r="O11" s="141"/>
+      <c r="P11" s="141"/>
+      <c r="Q11" s="141"/>
+      <c r="R11" s="141"/>
+      <c r="S11" s="141"/>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3000,28 +3000,28 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="144" t="s">
+      <c r="A21" s="141" t="s">
         <v>279</v>
       </c>
-      <c r="B21" s="144"/>
-      <c r="C21" s="144"/>
-      <c r="D21" s="144"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="K21" s="147" t="s">
+      <c r="B21" s="141"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
+      <c r="K21" s="140" t="s">
         <v>279</v>
       </c>
-      <c r="L21" s="147"/>
-      <c r="M21" s="147"/>
-      <c r="N21" s="147"/>
-      <c r="O21" s="147"/>
-      <c r="P21" s="147"/>
-      <c r="Q21" s="147"/>
-      <c r="R21" s="147"/>
-      <c r="S21" s="147"/>
+      <c r="L21" s="140"/>
+      <c r="M21" s="140"/>
+      <c r="N21" s="140"/>
+      <c r="O21" s="140"/>
+      <c r="P21" s="140"/>
+      <c r="Q21" s="140"/>
+      <c r="R21" s="140"/>
+      <c r="S21" s="140"/>
     </row>
     <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3281,28 +3281,28 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A31" s="144" t="s">
+      <c r="A31" s="141" t="s">
         <v>280</v>
       </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="144"/>
-      <c r="D31" s="144"/>
-      <c r="E31" s="144"/>
-      <c r="F31" s="144"/>
-      <c r="G31" s="144"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="144"/>
-      <c r="K31" s="144" t="s">
+      <c r="B31" s="141"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="141"/>
+      <c r="G31" s="141"/>
+      <c r="H31" s="141"/>
+      <c r="I31" s="141"/>
+      <c r="K31" s="141" t="s">
         <v>280</v>
       </c>
-      <c r="L31" s="144"/>
-      <c r="M31" s="144"/>
-      <c r="N31" s="144"/>
-      <c r="O31" s="144"/>
-      <c r="P31" s="144"/>
-      <c r="Q31" s="144"/>
-      <c r="R31" s="144"/>
-      <c r="S31" s="144"/>
+      <c r="L31" s="141"/>
+      <c r="M31" s="141"/>
+      <c r="N31" s="141"/>
+      <c r="O31" s="141"/>
+      <c r="P31" s="141"/>
+      <c r="Q31" s="141"/>
+      <c r="R31" s="141"/>
+      <c r="S31" s="141"/>
     </row>
     <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3562,28 +3562,28 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A42" s="144" t="s">
+      <c r="A42" s="141" t="s">
         <v>281</v>
       </c>
-      <c r="B42" s="144"/>
-      <c r="C42" s="144"/>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144"/>
-      <c r="K42" s="144" t="s">
+      <c r="B42" s="141"/>
+      <c r="C42" s="141"/>
+      <c r="D42" s="141"/>
+      <c r="E42" s="141"/>
+      <c r="F42" s="141"/>
+      <c r="G42" s="141"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
+      <c r="K42" s="141" t="s">
         <v>281</v>
       </c>
-      <c r="L42" s="144"/>
-      <c r="M42" s="144"/>
-      <c r="N42" s="144"/>
-      <c r="O42" s="144"/>
-      <c r="P42" s="144"/>
-      <c r="Q42" s="144"/>
-      <c r="R42" s="144"/>
-      <c r="S42" s="144"/>
+      <c r="L42" s="141"/>
+      <c r="M42" s="141"/>
+      <c r="N42" s="141"/>
+      <c r="O42" s="141"/>
+      <c r="P42" s="141"/>
+      <c r="Q42" s="141"/>
+      <c r="R42" s="141"/>
+      <c r="S42" s="141"/>
     </row>
     <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3831,51 +3831,51 @@
       <c r="W50" s="84"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A53" s="148" t="s">
+      <c r="A53" s="142" t="s">
         <v>282</v>
       </c>
-      <c r="B53" s="148"/>
-      <c r="C53" s="148"/>
-      <c r="D53" s="148"/>
-      <c r="E53" s="148"/>
-      <c r="F53" s="148"/>
-      <c r="G53" s="148"/>
-      <c r="H53" s="148"/>
-      <c r="I53" s="148"/>
-      <c r="J53" s="148"/>
-      <c r="K53" s="148"/>
-      <c r="L53" s="148"/>
-      <c r="M53" s="148"/>
-      <c r="N53" s="148"/>
-      <c r="O53" s="148"/>
-      <c r="P53" s="148"/>
-      <c r="Q53" s="148"/>
-      <c r="R53" s="148"/>
-      <c r="S53" s="148"/>
+      <c r="B53" s="142"/>
+      <c r="C53" s="142"/>
+      <c r="D53" s="142"/>
+      <c r="E53" s="142"/>
+      <c r="F53" s="142"/>
+      <c r="G53" s="142"/>
+      <c r="H53" s="142"/>
+      <c r="I53" s="142"/>
+      <c r="J53" s="142"/>
+      <c r="K53" s="142"/>
+      <c r="L53" s="142"/>
+      <c r="M53" s="142"/>
+      <c r="N53" s="142"/>
+      <c r="O53" s="142"/>
+      <c r="P53" s="142"/>
+      <c r="Q53" s="142"/>
+      <c r="R53" s="142"/>
+      <c r="S53" s="142"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A55" s="144" t="s">
+      <c r="A55" s="141" t="s">
         <v>283</v>
       </c>
-      <c r="B55" s="144"/>
-      <c r="C55" s="144"/>
-      <c r="D55" s="144"/>
-      <c r="E55" s="144"/>
-      <c r="F55" s="144"/>
-      <c r="G55" s="144"/>
-      <c r="H55" s="144"/>
-      <c r="I55" s="144"/>
-      <c r="K55" s="144" t="s">
+      <c r="B55" s="141"/>
+      <c r="C55" s="141"/>
+      <c r="D55" s="141"/>
+      <c r="E55" s="141"/>
+      <c r="F55" s="141"/>
+      <c r="G55" s="141"/>
+      <c r="H55" s="141"/>
+      <c r="I55" s="141"/>
+      <c r="K55" s="141" t="s">
         <v>283</v>
       </c>
-      <c r="L55" s="144"/>
-      <c r="M55" s="144"/>
-      <c r="N55" s="144"/>
-      <c r="O55" s="144"/>
-      <c r="P55" s="144"/>
-      <c r="Q55" s="144"/>
-      <c r="R55" s="144"/>
-      <c r="S55" s="144"/>
+      <c r="L55" s="141"/>
+      <c r="M55" s="141"/>
+      <c r="N55" s="141"/>
+      <c r="O55" s="141"/>
+      <c r="P55" s="141"/>
+      <c r="Q55" s="141"/>
+      <c r="R55" s="141"/>
+      <c r="S55" s="141"/>
     </row>
     <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4026,28 +4026,28 @@
       <c r="Q63" s="68"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A65" s="144" t="s">
+      <c r="A65" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="B65" s="144"/>
-      <c r="C65" s="144"/>
-      <c r="D65" s="144"/>
-      <c r="E65" s="144"/>
-      <c r="F65" s="144"/>
-      <c r="G65" s="144"/>
-      <c r="H65" s="144"/>
-      <c r="I65" s="144"/>
-      <c r="K65" s="144" t="s">
+      <c r="B65" s="141"/>
+      <c r="C65" s="141"/>
+      <c r="D65" s="141"/>
+      <c r="E65" s="141"/>
+      <c r="F65" s="141"/>
+      <c r="G65" s="141"/>
+      <c r="H65" s="141"/>
+      <c r="I65" s="141"/>
+      <c r="K65" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="L65" s="144"/>
-      <c r="M65" s="144"/>
-      <c r="N65" s="144"/>
-      <c r="O65" s="144"/>
-      <c r="P65" s="144"/>
-      <c r="Q65" s="144"/>
-      <c r="R65" s="144"/>
-      <c r="S65" s="144"/>
+      <c r="L65" s="141"/>
+      <c r="M65" s="141"/>
+      <c r="N65" s="141"/>
+      <c r="O65" s="141"/>
+      <c r="P65" s="141"/>
+      <c r="Q65" s="141"/>
+      <c r="R65" s="141"/>
+      <c r="S65" s="141"/>
     </row>
     <row r="66" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4199,13 +4199,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K65:S65"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="K42:S42"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="K55:S55"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="K31:S31"/>
     <mergeCell ref="A9:I9"/>
@@ -4214,6 +4207,13 @@
     <mergeCell ref="K11:S11"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="K21:S21"/>
+    <mergeCell ref="K65:S65"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="K42:S42"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K55:S55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4257,31 +4257,31 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="147" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
-      <c r="E4" s="142" t="s">
+      <c r="C4" s="147"/>
+      <c r="D4" s="147"/>
+      <c r="E4" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="142"/>
-      <c r="G4" s="142"/>
-      <c r="H4" s="142"/>
-      <c r="I4" s="142"/>
-      <c r="J4" s="142"/>
-      <c r="K4" s="139" t="s">
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
+      <c r="H4" s="148"/>
+      <c r="I4" s="148"/>
+      <c r="J4" s="148"/>
+      <c r="K4" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
-      <c r="N4" s="139"/>
-      <c r="O4" s="140" t="s">
+      <c r="L4" s="145"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="140"/>
-      <c r="Q4" s="140"/>
-      <c r="R4" s="140"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B5" s="31" t="s">
@@ -5056,20 +5056,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="143"/>
-      <c r="C1" s="143"/>
-      <c r="D1" s="143"/>
-      <c r="E1" s="143"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="149"/>
+      <c r="E1" s="149"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="126" t="s">
+      <c r="G2" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -5384,11 +5384,11 @@
       <c r="B13" s="49">
         <v>62</v>
       </c>
-      <c r="G13" s="126" t="s">
+      <c r="G13" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="126"/>
-      <c r="I13" s="126"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
       <c r="M13" s="75"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -5403,13 +5403,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="143" t="s">
+      <c r="A15" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="143"/>
-      <c r="C15" s="143"/>
-      <c r="D15" s="143"/>
-      <c r="E15" s="143"/>
+      <c r="B15" s="149"/>
+      <c r="C15" s="149"/>
+      <c r="D15" s="149"/>
+      <c r="E15" s="149"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="10">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -5553,11 +5553,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="126" t="s">
+      <c r="G24" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
+      <c r="H24" s="127"/>
+      <c r="I24" s="127"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -5583,13 +5583,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="143" t="s">
+      <c r="A26" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="143"/>
-      <c r="C26" s="143"/>
-      <c r="D26" s="143"/>
-      <c r="E26" s="143"/>
+      <c r="B26" s="149"/>
+      <c r="C26" s="149"/>
+      <c r="D26" s="149"/>
+      <c r="E26" s="149"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="11">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -5766,20 +5766,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="143" t="s">
+      <c r="A37" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="143"/>
-      <c r="C37" s="143"/>
-      <c r="D37" s="143"/>
-      <c r="E37" s="143"/>
+      <c r="B37" s="149"/>
+      <c r="C37" s="149"/>
+      <c r="D37" s="149"/>
+      <c r="E37" s="149"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="126" t="s">
+      <c r="G38" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="126"/>
-      <c r="I38" s="126"/>
+      <c r="H38" s="127"/>
+      <c r="I38" s="127"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -6071,20 +6071,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="143" t="s">
+      <c r="A51" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="143"/>
-      <c r="C51" s="143"/>
-      <c r="D51" s="143"/>
-      <c r="E51" s="143"/>
+      <c r="B51" s="149"/>
+      <c r="C51" s="149"/>
+      <c r="D51" s="149"/>
+      <c r="E51" s="149"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="126" t="s">
+      <c r="G52" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="126"/>
-      <c r="I52" s="126"/>
+      <c r="H52" s="127"/>
+      <c r="I52" s="127"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -6430,20 +6430,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="143" t="s">
+      <c r="A3" s="149" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="143"/>
-      <c r="C3" s="143"/>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
+      <c r="B3" s="149"/>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="126" t="s">
+      <c r="G4" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="126"/>
-      <c r="I4" s="126"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -6760,10 +6760,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="25"/>
-      <c r="H10" s="149" t="s">
+      <c r="H10" s="150" t="s">
         <v>271</v>
       </c>
-      <c r="I10" s="149"/>
+      <c r="I10" s="150"/>
       <c r="L10" s="30"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -6774,8 +6774,8 @@
       <c r="F11" s="25">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="149"/>
-      <c r="I11" s="149"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="150"/>
       <c r="L11" s="30"/>
       <c r="N11" s="30"/>
     </row>
@@ -6792,8 +6792,8 @@
       <c r="F12" s="25">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="149"/>
-      <c r="I12" s="149"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="150"/>
       <c r="L12" s="30"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6809,8 +6809,8 @@
       <c r="F13" s="44">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="149"/>
-      <c r="I13" s="149"/>
+      <c r="H13" s="150"/>
+      <c r="I13" s="150"/>
       <c r="L13" s="30"/>
       <c r="N13" s="30"/>
     </row>
@@ -6978,8 +6978,8 @@
       <c r="E33" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="130"/>
-      <c r="I33" s="130"/>
+      <c r="H33" s="131"/>
+      <c r="I33" s="131"/>
       <c r="L33" s="30"/>
     </row>
     <row r="34" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7705,12 +7705,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="130"/>
-      <c r="B1" s="130"/>
-      <c r="C1" s="130"/>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
+      <c r="A1" s="131"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -8687,10 +8687,10 @@
       <c r="B3" s="57"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="131" t="s">
+      <c r="A4" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="131"/>
+      <c r="B4" s="132"/>
       <c r="C4" s="85"/>
       <c r="D4" s="85"/>
     </row>
@@ -9282,66 +9282,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="128" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
       <c r="G1" s="49"/>
-      <c r="H1" s="127" t="s">
+      <c r="H1" s="128" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="N1" s="127" t="s">
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="N1" s="128" t="s">
         <v>204</v>
       </c>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="T1" s="127" t="s">
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="T1" s="128" t="s">
         <v>205</v>
       </c>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="129" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
       <c r="G2" s="49"/>
-      <c r="H2" s="128" t="s">
+      <c r="H2" s="129" t="s">
         <v>206</v>
       </c>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="N2" s="128" t="s">
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="N2" s="129" t="s">
         <v>206</v>
       </c>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128"/>
-      <c r="T2" s="128" t="s">
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="129"/>
+      <c r="T2" s="129" t="s">
         <v>206</v>
       </c>
-      <c r="U2" s="129"/>
-      <c r="V2" s="129"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="129"/>
+      <c r="U2" s="130"/>
+      <c r="V2" s="130"/>
+      <c r="W2" s="130"/>
+      <c r="X2" s="130"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -10376,10 +10376,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="131" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="130"/>
+      <c r="C2" s="131"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -10914,13 +10914,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
+      <c r="B1" s="132"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
       <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -11034,12 +11034,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="132" t="s">
+      <c r="A10" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="132"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -11338,12 +11338,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="133" t="s">
+      <c r="A37" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="133"/>
-      <c r="C37" s="133"/>
-      <c r="D37" s="133"/>
+      <c r="B37" s="134"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="89"/>
@@ -11695,13 +11695,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="137" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="136"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="137"/>
+      <c r="D3" s="137"/>
+      <c r="E3" s="137"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -11939,13 +11939,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="137" t="s">
+      <c r="A21" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="137"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="138"/>
+      <c r="D21" s="138"/>
+      <c r="E21" s="138"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="45"/>
@@ -11973,13 +11973,13 @@
       <c r="E24" s="45"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="134" t="s">
+      <c r="A25" s="135" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="134"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="134"/>
-      <c r="E25" s="134"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="135"/>
+      <c r="D25" s="135"/>
+      <c r="E25" s="135"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="100"/>
@@ -12256,13 +12256,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="135" t="s">
+      <c r="A43" s="136" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="135"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="135"/>
-      <c r="E43" s="135"/>
+      <c r="B43" s="136"/>
+      <c r="C43" s="136"/>
+      <c r="D43" s="136"/>
+      <c r="E43" s="136"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -12630,36 +12630,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="138"/>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
-      <c r="X3" s="138"/>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="138"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="139"/>
+      <c r="L3" s="139"/>
+      <c r="M3" s="139"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
+      <c r="R3" s="139"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
+      <c r="Y3" s="139"/>
+      <c r="Z3" s="139"/>
+      <c r="AA3" s="139"/>
+      <c r="AB3" s="139"/>
       <c r="AC3" s="28"/>
     </row>
     <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13196,8 +13196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32157BE9-2307-4C04-9818-D75A80711DCD}">
   <dimension ref="B1:H24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:G24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13208,13 +13208,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B1" s="150" t="s">
+      <c r="B1" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="150" t="s">
+      <c r="C1" s="126" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="150" t="s">
+      <c r="D1" s="126" t="s">
         <v>79</v>
       </c>
       <c r="E1" s="80"/>
@@ -13223,15 +13223,15 @@
       <c r="H1" s="80"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B3" s="147" t="s">
+      <c r="B3" s="140" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
-      <c r="H3" s="147"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
+      <c r="F3" s="140"/>
+      <c r="G3" s="140"/>
+      <c r="H3" s="140"/>
     </row>
     <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13346,13 +13346,13 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="150" t="s">
+      <c r="B14" s="126" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="150" t="s">
+      <c r="C14" s="126" t="s">
         <v>204</v>
       </c>
-      <c r="D14" s="150" t="s">
+      <c r="D14" s="126" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="80"/>
@@ -13361,15 +13361,15 @@
       <c r="H14" s="80"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="140" t="s">
         <v>279</v>
       </c>
-      <c r="C16" s="147"/>
-      <c r="D16" s="147"/>
-      <c r="E16" s="147"/>
-      <c r="F16" s="147"/>
-      <c r="G16" s="147"/>
-      <c r="H16" s="147"/>
+      <c r="C16" s="140"/>
+      <c r="D16" s="140"/>
+      <c r="E16" s="140"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="140"/>
     </row>
     <row r="17" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -13407,10 +13407,18 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="D20" s="68"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="68"/>
+      <c r="D20" s="68">
+        <v>-3.1E-2</v>
+      </c>
+      <c r="E20" s="68">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="F20" s="68">
+        <v>-6.4699999999999994E-2</v>
+      </c>
+      <c r="G20" s="68">
+        <v>-7.0000000000000007E-2</v>
+      </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
@@ -13430,10 +13438,18 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="D22" s="68"/>
-      <c r="E22" s="68"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="68"/>
+      <c r="D22" s="68">
+        <v>-3.5900000000000001E-2</v>
+      </c>
+      <c r="E22" s="68">
+        <v>-7.4899999999999994E-2</v>
+      </c>
+      <c r="F22" s="68">
+        <v>-7.6899999999999996E-2</v>
+      </c>
+      <c r="G22" s="68">
+        <v>-7.4700000000000003E-2</v>
+      </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
@@ -13454,10 +13470,18 @@
     </row>
     <row r="24" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="19"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
+      <c r="D24" s="69">
+        <v>-3.09E-2</v>
+      </c>
+      <c r="E24" s="69">
+        <v>-6.9900000000000004E-2</v>
+      </c>
+      <c r="F24" s="69">
+        <v>-7.0199999999999999E-2</v>
+      </c>
+      <c r="G24" s="69">
+        <v>-5.5500000000000001E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Status before coding equation 6
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49CF557-88D8-4E18-B3C6-48B742A3B92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5DB120-F92B-44E4-A654-0371DC688AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="1" activeTab="5" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="2" activeTab="6" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -19,20 +19,21 @@
     <sheet name="dropped_occ" sheetId="13" state="hidden" r:id="rId4"/>
     <sheet name="summaries" sheetId="4" r:id="rId5"/>
     <sheet name="people_do_diff" sheetId="1" r:id="rId6"/>
-    <sheet name="step-up" sheetId="10" r:id="rId7"/>
-    <sheet name="indexes_make_sense" sheetId="6" r:id="rId8"/>
-    <sheet name="skill_correlation" sheetId="7" r:id="rId9"/>
-    <sheet name="theta_estimates" sheetId="2" state="hidden" r:id="rId10"/>
-    <sheet name="lab_abstract" sheetId="18" r:id="rId11"/>
-    <sheet name="OLS_thetas" sheetId="8" r:id="rId12"/>
-    <sheet name="sigma_estimates" sheetId="3" r:id="rId13"/>
-    <sheet name="pi_estimates" sheetId="16" r:id="rId14"/>
-    <sheet name="dlnA estimates" sheetId="17" r:id="rId15"/>
-    <sheet name="top_jobs_skill" sheetId="5" r:id="rId16"/>
-    <sheet name="index_composition" sheetId="14" r:id="rId17"/>
+    <sheet name="top_quadrant" sheetId="19" r:id="rId7"/>
+    <sheet name="step-up" sheetId="10" r:id="rId8"/>
+    <sheet name="indexes_make_sense" sheetId="6" r:id="rId9"/>
+    <sheet name="skill_correlation" sheetId="7" r:id="rId10"/>
+    <sheet name="theta_estimates" sheetId="2" state="hidden" r:id="rId11"/>
+    <sheet name="lab_abstract" sheetId="18" r:id="rId12"/>
+    <sheet name="OLS_thetas" sheetId="8" r:id="rId13"/>
+    <sheet name="sigma_estimates" sheetId="3" r:id="rId14"/>
+    <sheet name="pi_estimates" sheetId="16" r:id="rId15"/>
+    <sheet name="dlnA estimates" sheetId="17" r:id="rId16"/>
+    <sheet name="top_jobs_skill" sheetId="5" r:id="rId17"/>
+    <sheet name="index_composition" sheetId="14" r:id="rId18"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'step-up'!$E$9:$F$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'step-up'!$E$9:$F$32</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -135,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="330">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1139,6 +1140,27 @@
   </si>
   <si>
     <t>(0.009)</t>
+  </si>
+  <si>
+    <t>5213 Metal forming, welding and related trades</t>
+  </si>
+  <si>
+    <t>5221 Metal Machining, Fitting And Instrument Making Trades</t>
+  </si>
+  <si>
+    <t>5231 Vehicle trades</t>
+  </si>
+  <si>
+    <t>5421 printing trades</t>
+  </si>
+  <si>
+    <t>5492 Skill trades nec</t>
+  </si>
+  <si>
+    <t>6221 Hairdressers And Related Occupations</t>
+  </si>
+  <si>
+    <t>Occupation</t>
   </si>
 </sst>
 </file>
@@ -1676,6 +1698,39 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1696,6 +1751,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1724,9 +1788,6 @@
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1736,50 +1797,11 @@
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2382,14 +2404,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="118" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2491,14 +2513,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="103"/>
-      <c r="C9" s="103"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2610,6 +2632,824 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F3C55B-20D0-4D01-AB90-788A157F68F3}">
+  <dimension ref="A1:R22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="59">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B4" s="133" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="133"/>
+      <c r="D4" s="133"/>
+      <c r="E4" s="134" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="134"/>
+      <c r="G4" s="134"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
+      <c r="K4" s="131" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="131"/>
+      <c r="M4" s="131"/>
+      <c r="N4" s="131"/>
+      <c r="O4" s="132" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="132"/>
+      <c r="Q4" s="132"/>
+      <c r="R4" s="132"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B5" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="K5" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="R5" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.52429999999999999</v>
+      </c>
+      <c r="C7" s="18">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="18">
+        <v>0.50409999999999999</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.75739999999999996</v>
+      </c>
+      <c r="D8" s="18">
+        <v>1</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="18">
+        <v>-0.10829999999999999</v>
+      </c>
+      <c r="C9" s="18">
+        <v>-9.69E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>-2.7699999999999999E-2</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="18">
+        <v>-8.0999999999999996E-3</v>
+      </c>
+      <c r="C10" s="18">
+        <v>-8.8999999999999999E-3</v>
+      </c>
+      <c r="D10" s="18">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0.2596</v>
+      </c>
+      <c r="F10" s="18">
+        <v>1</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="18">
+        <v>-1.83E-2</v>
+      </c>
+      <c r="C11" s="18">
+        <v>-5.3600000000000002E-2</v>
+      </c>
+      <c r="D11" s="18">
+        <v>-4.8999999999999998E-3</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.29580000000000001</v>
+      </c>
+      <c r="F11" s="18">
+        <v>0.64780000000000004</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="18"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="18">
+        <v>-0.16220000000000001</v>
+      </c>
+      <c r="C12" s="18">
+        <v>-0.20030000000000001</v>
+      </c>
+      <c r="D12" s="18">
+        <v>-0.1011</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="F12" s="18">
+        <v>0.2651</v>
+      </c>
+      <c r="G12" s="18">
+        <v>0.27389999999999998</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="18">
+        <v>-0.12180000000000001</v>
+      </c>
+      <c r="C13" s="18">
+        <v>-0.14349999999999999</v>
+      </c>
+      <c r="D13" s="18">
+        <v>-4.7600000000000003E-2</v>
+      </c>
+      <c r="E13" s="18">
+        <v>0.37580000000000002</v>
+      </c>
+      <c r="F13" s="18">
+        <v>0.31369999999999998</v>
+      </c>
+      <c r="G13" s="18">
+        <v>0.33760000000000001</v>
+      </c>
+      <c r="H13" s="18">
+        <v>0.59350000000000003</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="18">
+        <v>2.93E-2</v>
+      </c>
+      <c r="C14" s="18">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="D14" s="18">
+        <v>7.3400000000000007E-2</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.31819999999999998</v>
+      </c>
+      <c r="F14" s="18">
+        <v>0.42980000000000002</v>
+      </c>
+      <c r="G14" s="18">
+        <v>0.40849999999999997</v>
+      </c>
+      <c r="H14" s="18">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="I14" s="18">
+        <v>0.47870000000000001</v>
+      </c>
+      <c r="J14" s="18">
+        <v>1</v>
+      </c>
+      <c r="K14" s="18"/>
+      <c r="L14" s="18"/>
+      <c r="M14" s="18"/>
+      <c r="N14" s="18"/>
+      <c r="O14" s="18"/>
+      <c r="P14" s="18"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="18">
+        <v>-0.1754</v>
+      </c>
+      <c r="C15" s="18">
+        <v>-0.1913</v>
+      </c>
+      <c r="D15" s="18">
+        <v>-0.1711</v>
+      </c>
+      <c r="E15" s="18">
+        <v>8.8499999999999995E-2</v>
+      </c>
+      <c r="F15" s="18">
+        <v>-1.03E-2</v>
+      </c>
+      <c r="G15" s="18">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="H15" s="18">
+        <v>0.21290000000000001</v>
+      </c>
+      <c r="I15" s="18">
+        <v>0.1653</v>
+      </c>
+      <c r="J15" s="18">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="K15" s="18">
+        <v>1</v>
+      </c>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="18">
+        <v>6.3E-2</v>
+      </c>
+      <c r="C16" s="18">
+        <v>3.8699999999999998E-2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.13289999999999999</v>
+      </c>
+      <c r="F16" s="18">
+        <v>-5.5999999999999999E-3</v>
+      </c>
+      <c r="G16" s="18">
+        <v>3.4799999999999998E-2</v>
+      </c>
+      <c r="H16" s="18">
+        <v>8.1600000000000006E-2</v>
+      </c>
+      <c r="I16" s="18">
+        <v>0.1512</v>
+      </c>
+      <c r="J16" s="18">
+        <v>8.6800000000000002E-2</v>
+      </c>
+      <c r="K16" s="18">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="L16" s="18">
+        <v>1</v>
+      </c>
+      <c r="M16" s="18"/>
+      <c r="N16" s="18"/>
+      <c r="O16" s="18"/>
+      <c r="P16" s="18"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="18"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="18">
+        <v>-3.5099999999999999E-2</v>
+      </c>
+      <c r="C17" s="18">
+        <v>-0.1091</v>
+      </c>
+      <c r="D17" s="18">
+        <v>-5.5199999999999999E-2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.27060000000000001</v>
+      </c>
+      <c r="F17" s="18">
+        <v>0.15260000000000001</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.20039999999999999</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0.29630000000000001</v>
+      </c>
+      <c r="I17" s="18">
+        <v>0.31830000000000003</v>
+      </c>
+      <c r="J17" s="18">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="K17" s="18">
+        <v>0.30869999999999997</v>
+      </c>
+      <c r="L17" s="18">
+        <v>0.22389999999999999</v>
+      </c>
+      <c r="M17" s="18">
+        <v>1</v>
+      </c>
+      <c r="N17" s="18"/>
+      <c r="O17" s="18"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="18"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="18">
+        <v>-6.2399999999999997E-2</v>
+      </c>
+      <c r="C18" s="18">
+        <v>-0.11509999999999999</v>
+      </c>
+      <c r="D18" s="18">
+        <v>-3.7199999999999997E-2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>0.2878</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.14480000000000001</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.21129999999999999</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0.36470000000000002</v>
+      </c>
+      <c r="I18" s="18">
+        <v>0.3967</v>
+      </c>
+      <c r="J18" s="18">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="K18" s="18">
+        <v>0.155</v>
+      </c>
+      <c r="L18" s="18">
+        <v>0.24640000000000001</v>
+      </c>
+      <c r="M18" s="18">
+        <v>0.34210000000000002</v>
+      </c>
+      <c r="N18" s="18">
+        <v>1</v>
+      </c>
+      <c r="O18" s="18"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="18"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="18">
+        <v>-0.13139999999999999</v>
+      </c>
+      <c r="C19" s="18">
+        <v>-0.22650000000000001</v>
+      </c>
+      <c r="D19" s="18">
+        <v>-0.14960000000000001</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0.30520000000000003</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0.51729999999999998</v>
+      </c>
+      <c r="I19" s="18">
+        <v>0.43730000000000002</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="K19" s="18">
+        <v>0.161</v>
+      </c>
+      <c r="L19" s="18">
+        <v>0.1009</v>
+      </c>
+      <c r="M19" s="18">
+        <v>0.29409999999999997</v>
+      </c>
+      <c r="N19" s="18">
+        <v>0.377</v>
+      </c>
+      <c r="O19" s="18">
+        <v>1</v>
+      </c>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="18">
+        <v>-5.2900000000000003E-2</v>
+      </c>
+      <c r="C20" s="18">
+        <v>-0.14449999999999999</v>
+      </c>
+      <c r="D20" s="18">
+        <v>-8.3400000000000002E-2</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.2676</v>
+      </c>
+      <c r="F20" s="18">
+        <v>0.27789999999999998</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0.34379999999999999</v>
+      </c>
+      <c r="H20" s="18">
+        <v>0.43959999999999999</v>
+      </c>
+      <c r="I20" s="18">
+        <v>0.41420000000000001</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0.36280000000000001</v>
+      </c>
+      <c r="K20" s="18">
+        <v>0.13109999999999999</v>
+      </c>
+      <c r="L20" s="18">
+        <v>9.8599999999999993E-2</v>
+      </c>
+      <c r="M20" s="18">
+        <v>0.2853</v>
+      </c>
+      <c r="N20" s="18">
+        <v>0.3533</v>
+      </c>
+      <c r="O20" s="18">
+        <v>0.66120000000000001</v>
+      </c>
+      <c r="P20" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="18">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="C21" s="18">
+        <v>-0.11020000000000001</v>
+      </c>
+      <c r="D21" s="18">
+        <v>-8.5199999999999998E-2</v>
+      </c>
+      <c r="E21" s="18">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="F21" s="18">
+        <v>0.1187</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0.15359999999999999</v>
+      </c>
+      <c r="H21" s="18">
+        <v>0.29730000000000001</v>
+      </c>
+      <c r="I21" s="18">
+        <v>0.24579999999999999</v>
+      </c>
+      <c r="J21" s="18">
+        <v>0.19950000000000001</v>
+      </c>
+      <c r="K21" s="18">
+        <v>8.4099999999999994E-2</v>
+      </c>
+      <c r="L21" s="18">
+        <v>5.96E-2</v>
+      </c>
+      <c r="M21" s="18">
+        <v>0.16930000000000001</v>
+      </c>
+      <c r="N21" s="18">
+        <v>0.21110000000000001</v>
+      </c>
+      <c r="O21" s="18">
+        <v>0.37980000000000003</v>
+      </c>
+      <c r="P21" s="18">
+        <v>0.34660000000000002</v>
+      </c>
+      <c r="Q21" s="18">
+        <v>1</v>
+      </c>
+      <c r="R21" s="18"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="18">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="C22" s="18">
+        <v>-0.1246</v>
+      </c>
+      <c r="D22" s="18">
+        <v>-6.25E-2</v>
+      </c>
+      <c r="E22" s="18">
+        <v>0.2135</v>
+      </c>
+      <c r="F22" s="18">
+        <v>0.24510000000000001</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0.30840000000000001</v>
+      </c>
+      <c r="H22" s="18">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0.45639999999999997</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0.35649999999999998</v>
+      </c>
+      <c r="K22" s="18">
+        <v>0.15709999999999999</v>
+      </c>
+      <c r="L22" s="18">
+        <v>0.14729999999999999</v>
+      </c>
+      <c r="M22" s="18">
+        <v>0.31590000000000001</v>
+      </c>
+      <c r="N22" s="18">
+        <v>0.39829999999999999</v>
+      </c>
+      <c r="O22" s="18">
+        <v>0.50249999999999995</v>
+      </c>
+      <c r="P22" s="18">
+        <v>0.52749999999999997</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>0.4093</v>
+      </c>
+      <c r="R22" s="18">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="O4:R4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:J4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B6:R22">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A63E760-C2E1-4C8F-8338-4A55E5F2D8F6}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -2627,20 +3467,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="135"/>
+      <c r="C1" s="135"/>
+      <c r="D1" s="135"/>
+      <c r="E1" s="135"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="103" t="s">
+      <c r="G2" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2955,11 +3795,11 @@
       <c r="B13" s="50">
         <v>62</v>
       </c>
-      <c r="G13" s="103" t="s">
+      <c r="G13" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="103"/>
-      <c r="I13" s="103"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
       <c r="M13" s="77"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2974,13 +3814,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="117"/>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="117"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="10">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -3124,11 +3964,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="103" t="s">
+      <c r="G24" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
+      <c r="H24" s="118"/>
+      <c r="I24" s="118"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -3154,13 +3994,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="117" t="s">
+      <c r="A26" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="117"/>
-      <c r="C26" s="117"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="117"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="135"/>
+      <c r="D26" s="135"/>
+      <c r="E26" s="135"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="11">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -3337,20 +4177,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="117"/>
-      <c r="C37" s="117"/>
-      <c r="D37" s="117"/>
-      <c r="E37" s="117"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="135"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="103" t="s">
+      <c r="G38" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="103"/>
-      <c r="I38" s="103"/>
+      <c r="H38" s="118"/>
+      <c r="I38" s="118"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3642,20 +4482,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="117" t="s">
+      <c r="A51" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="117"/>
-      <c r="C51" s="117"/>
-      <c r="D51" s="117"/>
-      <c r="E51" s="117"/>
+      <c r="B51" s="135"/>
+      <c r="C51" s="135"/>
+      <c r="D51" s="135"/>
+      <c r="E51" s="135"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="103" t="s">
+      <c r="G52" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="103"/>
-      <c r="I52" s="103"/>
+      <c r="H52" s="118"/>
+      <c r="I52" s="118"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3975,7 +4815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
   <dimension ref="A2:W73"/>
   <sheetViews>
@@ -4089,52 +4929,52 @@
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="137" t="s">
         <v>289</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
-      <c r="F9" s="120"/>
-      <c r="G9" s="120"/>
-      <c r="H9" s="120"/>
-      <c r="I9" s="120"/>
-      <c r="K9" s="121" t="s">
+      <c r="B9" s="137"/>
+      <c r="C9" s="137"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
+      <c r="K9" s="138" t="s">
         <v>290</v>
       </c>
-      <c r="L9" s="121"/>
-      <c r="M9" s="121"/>
-      <c r="N9" s="121"/>
-      <c r="O9" s="121"/>
-      <c r="P9" s="121"/>
-      <c r="Q9" s="121"/>
-      <c r="R9" s="121"/>
-      <c r="S9" s="121"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+      <c r="O9" s="138"/>
+      <c r="P9" s="138"/>
+      <c r="Q9" s="138"/>
+      <c r="R9" s="138"/>
+      <c r="S9" s="138"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="136" t="s">
         <v>291</v>
       </c>
-      <c r="B11" s="118"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="K11" s="118" t="s">
+      <c r="B11" s="136"/>
+      <c r="C11" s="136"/>
+      <c r="D11" s="136"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="136"/>
+      <c r="I11" s="136"/>
+      <c r="K11" s="136" t="s">
         <v>291</v>
       </c>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="118"/>
-      <c r="P11" s="118"/>
-      <c r="Q11" s="118"/>
-      <c r="R11" s="118"/>
-      <c r="S11" s="118"/>
+      <c r="L11" s="136"/>
+      <c r="M11" s="136"/>
+      <c r="N11" s="136"/>
+      <c r="O11" s="136"/>
+      <c r="P11" s="136"/>
+      <c r="Q11" s="136"/>
+      <c r="R11" s="136"/>
+      <c r="S11" s="136"/>
     </row>
     <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4394,28 +5234,28 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="136" t="s">
         <v>292</v>
       </c>
-      <c r="B21" s="118"/>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="K21" s="122" t="s">
+      <c r="B21" s="136"/>
+      <c r="C21" s="136"/>
+      <c r="D21" s="136"/>
+      <c r="E21" s="136"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="136"/>
+      <c r="H21" s="136"/>
+      <c r="I21" s="136"/>
+      <c r="K21" s="139" t="s">
         <v>292</v>
       </c>
-      <c r="L21" s="122"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="122"/>
-      <c r="O21" s="122"/>
-      <c r="P21" s="122"/>
-      <c r="Q21" s="122"/>
-      <c r="R21" s="122"/>
-      <c r="S21" s="122"/>
+      <c r="L21" s="139"/>
+      <c r="M21" s="139"/>
+      <c r="N21" s="139"/>
+      <c r="O21" s="139"/>
+      <c r="P21" s="139"/>
+      <c r="Q21" s="139"/>
+      <c r="R21" s="139"/>
+      <c r="S21" s="139"/>
     </row>
     <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4675,28 +5515,28 @@
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A31" s="118" t="s">
+      <c r="A31" s="136" t="s">
         <v>293</v>
       </c>
-      <c r="B31" s="118"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="118"/>
-      <c r="E31" s="118"/>
-      <c r="F31" s="118"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
-      <c r="I31" s="118"/>
-      <c r="K31" s="118" t="s">
+      <c r="B31" s="136"/>
+      <c r="C31" s="136"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="136"/>
+      <c r="I31" s="136"/>
+      <c r="K31" s="136" t="s">
         <v>293</v>
       </c>
-      <c r="L31" s="118"/>
-      <c r="M31" s="118"/>
-      <c r="N31" s="118"/>
-      <c r="O31" s="118"/>
-      <c r="P31" s="118"/>
-      <c r="Q31" s="118"/>
-      <c r="R31" s="118"/>
-      <c r="S31" s="118"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="136"/>
+      <c r="Q31" s="136"/>
+      <c r="R31" s="136"/>
+      <c r="S31" s="136"/>
     </row>
     <row r="32" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="33" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4956,28 +5796,28 @@
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A42" s="118" t="s">
+      <c r="A42" s="136" t="s">
         <v>294</v>
       </c>
-      <c r="B42" s="118"/>
-      <c r="C42" s="118"/>
-      <c r="D42" s="118"/>
-      <c r="E42" s="118"/>
-      <c r="F42" s="118"/>
-      <c r="G42" s="118"/>
-      <c r="H42" s="118"/>
-      <c r="I42" s="118"/>
-      <c r="K42" s="118" t="s">
+      <c r="B42" s="136"/>
+      <c r="C42" s="136"/>
+      <c r="D42" s="136"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="136"/>
+      <c r="G42" s="136"/>
+      <c r="H42" s="136"/>
+      <c r="I42" s="136"/>
+      <c r="K42" s="136" t="s">
         <v>294</v>
       </c>
-      <c r="L42" s="118"/>
-      <c r="M42" s="118"/>
-      <c r="N42" s="118"/>
-      <c r="O42" s="118"/>
-      <c r="P42" s="118"/>
-      <c r="Q42" s="118"/>
-      <c r="R42" s="118"/>
-      <c r="S42" s="118"/>
+      <c r="L42" s="136"/>
+      <c r="M42" s="136"/>
+      <c r="N42" s="136"/>
+      <c r="O42" s="136"/>
+      <c r="P42" s="136"/>
+      <c r="Q42" s="136"/>
+      <c r="R42" s="136"/>
+      <c r="S42" s="136"/>
     </row>
     <row r="43" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="44" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5225,51 +6065,51 @@
       <c r="W50" s="86"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A53" s="119" t="s">
+      <c r="A53" s="140" t="s">
         <v>295</v>
       </c>
-      <c r="B53" s="119"/>
-      <c r="C53" s="119"/>
-      <c r="D53" s="119"/>
-      <c r="E53" s="119"/>
-      <c r="F53" s="119"/>
-      <c r="G53" s="119"/>
-      <c r="H53" s="119"/>
-      <c r="I53" s="119"/>
-      <c r="J53" s="119"/>
-      <c r="K53" s="119"/>
-      <c r="L53" s="119"/>
-      <c r="M53" s="119"/>
-      <c r="N53" s="119"/>
-      <c r="O53" s="119"/>
-      <c r="P53" s="119"/>
-      <c r="Q53" s="119"/>
-      <c r="R53" s="119"/>
-      <c r="S53" s="119"/>
+      <c r="B53" s="140"/>
+      <c r="C53" s="140"/>
+      <c r="D53" s="140"/>
+      <c r="E53" s="140"/>
+      <c r="F53" s="140"/>
+      <c r="G53" s="140"/>
+      <c r="H53" s="140"/>
+      <c r="I53" s="140"/>
+      <c r="J53" s="140"/>
+      <c r="K53" s="140"/>
+      <c r="L53" s="140"/>
+      <c r="M53" s="140"/>
+      <c r="N53" s="140"/>
+      <c r="O53" s="140"/>
+      <c r="P53" s="140"/>
+      <c r="Q53" s="140"/>
+      <c r="R53" s="140"/>
+      <c r="S53" s="140"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A55" s="118" t="s">
+      <c r="A55" s="136" t="s">
         <v>296</v>
       </c>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
-      <c r="G55" s="118"/>
-      <c r="H55" s="118"/>
-      <c r="I55" s="118"/>
-      <c r="K55" s="118" t="s">
+      <c r="B55" s="136"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="136"/>
+      <c r="E55" s="136"/>
+      <c r="F55" s="136"/>
+      <c r="G55" s="136"/>
+      <c r="H55" s="136"/>
+      <c r="I55" s="136"/>
+      <c r="K55" s="136" t="s">
         <v>296</v>
       </c>
-      <c r="L55" s="118"/>
-      <c r="M55" s="118"/>
-      <c r="N55" s="118"/>
-      <c r="O55" s="118"/>
-      <c r="P55" s="118"/>
-      <c r="Q55" s="118"/>
-      <c r="R55" s="118"/>
-      <c r="S55" s="118"/>
+      <c r="L55" s="136"/>
+      <c r="M55" s="136"/>
+      <c r="N55" s="136"/>
+      <c r="O55" s="136"/>
+      <c r="P55" s="136"/>
+      <c r="Q55" s="136"/>
+      <c r="R55" s="136"/>
+      <c r="S55" s="136"/>
     </row>
     <row r="56" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="57" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5420,28 +6260,28 @@
       <c r="Q63" s="69"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A65" s="118" t="s">
+      <c r="A65" s="136" t="s">
         <v>297</v>
       </c>
-      <c r="B65" s="118"/>
-      <c r="C65" s="118"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="118"/>
-      <c r="F65" s="118"/>
-      <c r="G65" s="118"/>
-      <c r="H65" s="118"/>
-      <c r="I65" s="118"/>
-      <c r="K65" s="118" t="s">
+      <c r="B65" s="136"/>
+      <c r="C65" s="136"/>
+      <c r="D65" s="136"/>
+      <c r="E65" s="136"/>
+      <c r="F65" s="136"/>
+      <c r="G65" s="136"/>
+      <c r="H65" s="136"/>
+      <c r="I65" s="136"/>
+      <c r="K65" s="136" t="s">
         <v>297</v>
       </c>
-      <c r="L65" s="118"/>
-      <c r="M65" s="118"/>
-      <c r="N65" s="118"/>
-      <c r="O65" s="118"/>
-      <c r="P65" s="118"/>
-      <c r="Q65" s="118"/>
-      <c r="R65" s="118"/>
-      <c r="S65" s="118"/>
+      <c r="L65" s="136"/>
+      <c r="M65" s="136"/>
+      <c r="N65" s="136"/>
+      <c r="O65" s="136"/>
+      <c r="P65" s="136"/>
+      <c r="Q65" s="136"/>
+      <c r="R65" s="136"/>
+      <c r="S65" s="136"/>
     </row>
     <row r="66" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="67" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5593,6 +6433,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K65:S65"/>
+    <mergeCell ref="A65:I65"/>
+    <mergeCell ref="A42:I42"/>
+    <mergeCell ref="K42:S42"/>
+    <mergeCell ref="A53:S53"/>
+    <mergeCell ref="A55:I55"/>
+    <mergeCell ref="K55:S55"/>
     <mergeCell ref="A31:I31"/>
     <mergeCell ref="K31:S31"/>
     <mergeCell ref="A9:I9"/>
@@ -5601,20 +6448,13 @@
     <mergeCell ref="K11:S11"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="K21:S21"/>
-    <mergeCell ref="K65:S65"/>
-    <mergeCell ref="A65:I65"/>
-    <mergeCell ref="A42:I42"/>
-    <mergeCell ref="K42:S42"/>
-    <mergeCell ref="A53:S53"/>
-    <mergeCell ref="A55:I55"/>
-    <mergeCell ref="K55:S55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{621AD9AE-E34E-4A18-B651-4D2CF9D0D43B}">
   <sheetPr>
     <tabColor theme="7"/>
@@ -5640,20 +6480,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="117"/>
+      <c r="B3" s="135"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="103" t="s">
+      <c r="G4" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="103"/>
-      <c r="I4" s="103"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -5826,7 +6666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C324394-3725-49AA-88D9-CE062D28E523}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
@@ -5974,10 +6814,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="26"/>
-      <c r="H10" s="123" t="s">
+      <c r="H10" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="I10" s="123"/>
+      <c r="I10" s="141"/>
       <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5988,8 +6828,8 @@
       <c r="F11" s="26">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
       <c r="L11" s="31"/>
       <c r="N11" s="31"/>
     </row>
@@ -6006,8 +6846,8 @@
       <c r="F12" s="26">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
+      <c r="H12" s="141"/>
+      <c r="I12" s="141"/>
       <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6023,8 +6863,8 @@
       <c r="F13" s="45">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
+      <c r="H13" s="141"/>
+      <c r="I13" s="141"/>
       <c r="L13" s="31"/>
       <c r="N13" s="31"/>
     </row>
@@ -6192,8 +7032,8 @@
       <c r="E33" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="107"/>
-      <c r="I33" s="107"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
       <c r="L33" s="31"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6201,10 +7041,10 @@
         <v>281</v>
       </c>
       <c r="O34" s="75"/>
-      <c r="P34" s="107" t="s">
+      <c r="P34" s="122" t="s">
         <v>271</v>
       </c>
-      <c r="Q34" s="107"/>
+      <c r="Q34" s="122"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
@@ -6334,10 +7174,10 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="F40" s="26"/>
-      <c r="H40" s="123" t="s">
+      <c r="H40" s="141" t="s">
         <v>284</v>
       </c>
-      <c r="I40" s="123"/>
+      <c r="I40" s="141"/>
       <c r="K40" t="s">
         <v>279</v>
       </c>
@@ -6355,8 +7195,8 @@
       <c r="F41" s="26">
         <v>1.365048</v>
       </c>
-      <c r="H41" s="123"/>
-      <c r="I41" s="123"/>
+      <c r="H41" s="141"/>
+      <c r="I41" s="141"/>
       <c r="K41" t="s">
         <v>280</v>
       </c>
@@ -6369,8 +7209,8 @@
       <c r="F42" s="26">
         <v>-0.3439432</v>
       </c>
-      <c r="H42" s="123"/>
-      <c r="I42" s="123"/>
+      <c r="H42" s="141"/>
+      <c r="I42" s="141"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="31">
@@ -6385,8 +7225,8 @@
       <c r="F43" s="45">
         <v>13.51919</v>
       </c>
-      <c r="H43" s="123"/>
-      <c r="I43" s="123"/>
+      <c r="H43" s="141"/>
+      <c r="I43" s="141"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44" s="31">
@@ -6818,7 +7658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4C7DBF-8E9C-4E7A-AD2C-6A1AFD2D3CE0}">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
@@ -6836,12 +7676,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="107"/>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
+      <c r="A1" s="122"/>
+      <c r="B1" s="122"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
@@ -7112,7 +7952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ED2790-90CA-437E-8990-4813411B73C2}">
   <dimension ref="A1:K41"/>
   <sheetViews>
@@ -7716,7 +8556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1118EAC5-EE01-4F6F-831E-9781C531891C}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -7750,10 +8590,10 @@
       <c r="B3" s="58"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="123" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="108"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="87"/>
       <c r="D4" s="87"/>
     </row>
@@ -7976,7 +8816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65F0097E-5ADA-4F9F-8E43-EFEAF7A70026}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -8345,66 +9185,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="119" t="s">
         <v>207</v>
       </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
       <c r="G1" s="50"/>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="119" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="104"/>
-      <c r="J1" s="104"/>
-      <c r="K1" s="104"/>
-      <c r="L1" s="104"/>
-      <c r="N1" s="104" t="s">
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="N1" s="119" t="s">
         <v>204</v>
       </c>
-      <c r="O1" s="104"/>
-      <c r="P1" s="104"/>
-      <c r="Q1" s="104"/>
-      <c r="R1" s="104"/>
-      <c r="T1" s="104" t="s">
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="T1" s="119" t="s">
         <v>205</v>
       </c>
-      <c r="U1" s="104"/>
-      <c r="V1" s="104"/>
-      <c r="W1" s="104"/>
-      <c r="X1" s="104"/>
+      <c r="U1" s="119"/>
+      <c r="V1" s="119"/>
+      <c r="W1" s="119"/>
+      <c r="X1" s="119"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="105" t="s">
+      <c r="B2" s="120" t="s">
         <v>206</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
       <c r="G2" s="50"/>
-      <c r="H2" s="105" t="s">
+      <c r="H2" s="120" t="s">
         <v>206</v>
       </c>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="N2" s="105" t="s">
+      <c r="I2" s="120"/>
+      <c r="J2" s="120"/>
+      <c r="K2" s="120"/>
+      <c r="L2" s="120"/>
+      <c r="N2" s="120" t="s">
         <v>206</v>
       </c>
-      <c r="O2" s="105"/>
-      <c r="P2" s="105"/>
-      <c r="Q2" s="105"/>
-      <c r="R2" s="105"/>
-      <c r="T2" s="105" t="s">
+      <c r="O2" s="120"/>
+      <c r="P2" s="120"/>
+      <c r="Q2" s="120"/>
+      <c r="R2" s="120"/>
+      <c r="T2" s="120" t="s">
         <v>206</v>
       </c>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -9439,10 +10279,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="122" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="107"/>
+      <c r="C2" s="122"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -9977,13 +10817,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="108"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
       <c r="G1" s="28"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -10097,12 +10937,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="109"/>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
+      <c r="D10" s="124"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -10401,15 +11241,15 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="124" t="s">
+      <c r="A37" s="125" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="124"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="124"/>
+      <c r="B37" s="125"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="125"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="125"/>
+      <c r="A38" s="103"/>
       <c r="B38" s="12">
         <v>2001</v>
       </c>
@@ -10432,13 +11272,13 @@
       <c r="A40" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="B40" s="126">
+      <c r="B40" s="104">
         <v>0.47114489999999998</v>
       </c>
-      <c r="C40" s="126">
+      <c r="C40" s="104">
         <v>0.3135192</v>
       </c>
-      <c r="D40" s="126">
+      <c r="D40" s="104">
         <f>+C40-B40</f>
         <v>-0.15762569999999998</v>
       </c>
@@ -10447,13 +11287,13 @@
       <c r="A41" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="126">
+      <c r="B41" s="104">
         <v>0.24976689999999999</v>
       </c>
-      <c r="C41" s="126">
+      <c r="C41" s="104">
         <v>0.2400099</v>
       </c>
-      <c r="D41" s="126">
+      <c r="D41" s="104">
         <f t="shared" ref="D41:D42" si="2">+C41-B41</f>
         <v>-9.7569999999999879E-3</v>
       </c>
@@ -10462,13 +11302,13 @@
       <c r="A42" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="126">
+      <c r="B42" s="104">
         <v>0.27908830000000001</v>
       </c>
-      <c r="C42" s="126">
+      <c r="C42" s="104">
         <v>0.4464709</v>
       </c>
-      <c r="D42" s="126">
+      <c r="D42" s="104">
         <f t="shared" si="2"/>
         <v>0.16738259999999999</v>
       </c>
@@ -10488,7 +11328,7 @@
       <c r="D44" s="86"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A45" s="127" t="s">
+      <c r="A45" s="105" t="s">
         <v>3</v>
       </c>
       <c r="B45" s="86"/>
@@ -10496,7 +11336,7 @@
       <c r="D45" s="86"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A46" s="128" t="s">
+      <c r="A46" s="106" t="s">
         <v>81</v>
       </c>
       <c r="B46" s="86">
@@ -10505,13 +11345,13 @@
       <c r="C46" s="86">
         <v>0.56899999999999995</v>
       </c>
-      <c r="D46" s="126">
+      <c r="D46" s="104">
         <f>+C46-B46</f>
         <v>3.7999999999999923E-2</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" s="128" t="s">
+      <c r="A47" s="106" t="s">
         <v>9</v>
       </c>
       <c r="B47" s="86">
@@ -10520,13 +11360,13 @@
       <c r="C47" s="86">
         <v>0.51600000000000001</v>
       </c>
-      <c r="D47" s="126">
+      <c r="D47" s="104">
         <f t="shared" ref="D47:D48" si="3">+C47-B47</f>
         <v>2.1000000000000019E-2</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" s="128" t="s">
+      <c r="A48" s="106" t="s">
         <v>10</v>
       </c>
       <c r="B48" s="86">
@@ -10535,181 +11375,181 @@
       <c r="C48" s="86">
         <v>0.35599999999999998</v>
       </c>
-      <c r="D48" s="126">
+      <c r="D48" s="104">
         <f t="shared" si="3"/>
         <v>1.2999999999999956E-2</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" s="127" t="s">
+      <c r="A49" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="126"/>
-      <c r="C49" s="126"/>
-      <c r="D49" s="126"/>
+      <c r="B49" s="104"/>
+      <c r="C49" s="104"/>
+      <c r="D49" s="104"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="128" t="s">
+      <c r="A50" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="126">
+      <c r="B50" s="104">
         <v>0.58199999999999996</v>
       </c>
-      <c r="C50" s="126">
+      <c r="C50" s="104">
         <v>0.60799999999999998</v>
       </c>
-      <c r="D50" s="126">
+      <c r="D50" s="104">
         <f t="shared" ref="D50:D52" si="4">+C50-B50</f>
         <v>2.6000000000000023E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="128" t="s">
+      <c r="A51" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="126">
+      <c r="B51" s="104">
         <v>0.63</v>
       </c>
-      <c r="C51" s="126">
+      <c r="C51" s="104">
         <v>0.66600000000000004</v>
       </c>
-      <c r="D51" s="126">
+      <c r="D51" s="104">
         <f t="shared" si="4"/>
         <v>3.6000000000000032E-2</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="128" t="s">
+      <c r="A52" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B52" s="126">
+      <c r="B52" s="104">
         <v>0.72099999999999997</v>
       </c>
-      <c r="C52" s="126">
+      <c r="C52" s="104">
         <v>0.73499999999999999</v>
       </c>
-      <c r="D52" s="126">
+      <c r="D52" s="104">
         <f t="shared" si="4"/>
         <v>1.4000000000000012E-2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="126"/>
-      <c r="C53" s="126"/>
-      <c r="D53" s="126"/>
+      <c r="B53" s="104"/>
+      <c r="C53" s="104"/>
+      <c r="D53" s="104"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="128" t="s">
+      <c r="A54" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="B54" s="126">
+      <c r="B54" s="104">
         <v>0.61799999999999999</v>
       </c>
-      <c r="C54" s="126">
+      <c r="C54" s="104">
         <v>0.58399999999999996</v>
       </c>
-      <c r="D54" s="126">
+      <c r="D54" s="104">
         <f t="shared" ref="D54:D56" si="5">+C54-B54</f>
         <v>-3.400000000000003E-2</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="128" t="s">
+      <c r="A55" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="B55" s="126">
+      <c r="B55" s="104">
         <v>0.67</v>
       </c>
-      <c r="C55" s="126">
+      <c r="C55" s="104">
         <v>0.63400000000000001</v>
       </c>
-      <c r="D55" s="126">
+      <c r="D55" s="104">
         <f t="shared" si="5"/>
         <v>-3.6000000000000032E-2</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="128" t="s">
+      <c r="A56" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="126">
+      <c r="B56" s="104">
         <v>0.73799999999999999</v>
       </c>
-      <c r="C56" s="126">
+      <c r="C56" s="104">
         <v>0.69799999999999995</v>
       </c>
-      <c r="D56" s="126">
+      <c r="D56" s="104">
         <f t="shared" si="5"/>
         <v>-4.0000000000000036E-2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="127" t="s">
+      <c r="A57" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="126"/>
-      <c r="C57" s="126"/>
-      <c r="D57" s="126"/>
+      <c r="B57" s="104"/>
+      <c r="C57" s="104"/>
+      <c r="D57" s="104"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" s="128" t="s">
+      <c r="A58" s="106" t="s">
         <v>81</v>
       </c>
-      <c r="B58" s="126">
+      <c r="B58" s="104">
         <v>0.371</v>
       </c>
-      <c r="C58" s="126">
+      <c r="C58" s="104">
         <v>0.42799999999999999</v>
       </c>
-      <c r="D58" s="126">
+      <c r="D58" s="104">
         <f t="shared" ref="D58:D60" si="6">+C58-B58</f>
         <v>5.6999999999999995E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" s="128" t="s">
+      <c r="A59" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="126">
+      <c r="B59" s="104">
         <v>0.47</v>
       </c>
-      <c r="C59" s="126">
+      <c r="C59" s="104">
         <v>0.499</v>
       </c>
-      <c r="D59" s="126">
+      <c r="D59" s="104">
         <f t="shared" si="6"/>
         <v>2.9000000000000026E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="128" t="s">
+      <c r="A60" s="106" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="126">
+      <c r="B60" s="104">
         <v>0.58499999999999996</v>
       </c>
-      <c r="C60" s="126">
+      <c r="C60" s="104">
         <v>0.60399999999999998</v>
       </c>
-      <c r="D60" s="126">
+      <c r="D60" s="104">
         <f t="shared" si="6"/>
         <v>1.9000000000000017E-2</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="129" t="s">
+      <c r="A61" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="B61" s="130">
+      <c r="B61" s="108">
         <v>93</v>
       </c>
-      <c r="C61" s="130">
+      <c r="C61" s="108">
         <v>93</v>
       </c>
-      <c r="D61" s="130">
+      <c r="D61" s="108">
         <v>93</v>
       </c>
     </row>
@@ -10739,7 +11579,7 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="91" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -10758,13 +11598,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="110"/>
-      <c r="C3" s="110"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -11002,13 +11842,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="111" t="s">
+      <c r="A21" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="111"/>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="111"/>
+      <c r="B21" s="129"/>
+      <c r="C21" s="129"/>
+      <c r="D21" s="129"/>
+      <c r="E21" s="129"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="46"/>
@@ -11036,58 +11876,58 @@
       <c r="E24" s="46"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="132" t="s">
+      <c r="A25" s="126" t="s">
         <v>122</v>
       </c>
-      <c r="B25" s="132"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132"/>
-      <c r="E25" s="132"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="126"/>
+      <c r="D25" s="126"/>
+      <c r="E25" s="126"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="133"/>
-      <c r="B26" s="133"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
+      <c r="A26" s="110"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="110"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="134" t="str">
+      <c r="A27" s="111" t="str">
         <f>""</f>
         <v/>
       </c>
-      <c r="B27" s="134" t="str">
+      <c r="B27" s="111" t="str">
         <f>"(1)"</f>
         <v>(1)</v>
       </c>
-      <c r="C27" s="134" t="str">
+      <c r="C27" s="111" t="str">
         <f>"(2)"</f>
         <v>(2)</v>
       </c>
-      <c r="D27" s="134" t="str">
+      <c r="D27" s="111" t="str">
         <f>"(3)"</f>
         <v>(3)</v>
       </c>
-      <c r="E27" s="134" t="str">
+      <c r="E27" s="111" t="str">
         <f>"(4)"</f>
         <v>(4)</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="135" t="str">
+      <c r="A28" s="112" t="str">
         <f>""</f>
         <v/>
       </c>
-      <c r="B28" s="135" t="s">
+      <c r="B28" s="112" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="135" t="s">
+      <c r="C28" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="135" t="s">
+      <c r="D28" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="135" t="s">
+      <c r="E28" s="112" t="s">
         <v>6</v>
       </c>
     </row>
@@ -11102,16 +11942,16 @@
       <c r="A30" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="136" t="s">
+      <c r="B30" s="113" t="s">
         <v>310</v>
       </c>
-      <c r="C30" s="136" t="s">
+      <c r="C30" s="113" t="s">
         <v>311</v>
       </c>
-      <c r="D30" s="136" t="s">
+      <c r="D30" s="113" t="s">
         <v>311</v>
       </c>
-      <c r="E30" s="136" t="s">
+      <c r="E30" s="113" t="s">
         <v>312</v>
       </c>
     </row>
@@ -11120,40 +11960,40 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B31" s="136" t="s">
+      <c r="B31" s="113" t="s">
         <v>313</v>
       </c>
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="113" t="s">
         <v>314</v>
       </c>
-      <c r="D31" s="136" t="s">
+      <c r="D31" s="113" t="s">
         <v>313</v>
       </c>
-      <c r="E31" s="136" t="s">
+      <c r="E31" s="113" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="86"/>
-      <c r="B32" s="137"/>
-      <c r="C32" s="137"/>
-      <c r="D32" s="137"/>
-      <c r="E32" s="137"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="114"/>
+      <c r="E32" s="114"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="136" t="s">
+      <c r="B33" s="113" t="s">
         <v>315</v>
       </c>
-      <c r="C33" s="136" t="s">
+      <c r="C33" s="113" t="s">
         <v>316</v>
       </c>
-      <c r="D33" s="136" t="s">
+      <c r="D33" s="113" t="s">
         <v>317</v>
       </c>
-      <c r="E33" s="136" t="s">
+      <c r="E33" s="113" t="s">
         <v>305</v>
       </c>
     </row>
@@ -11162,41 +12002,41 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B34" s="136" t="s">
+      <c r="B34" s="113" t="s">
         <v>318</v>
       </c>
-      <c r="C34" s="136" t="s">
+      <c r="C34" s="113" t="s">
         <v>319</v>
       </c>
-      <c r="D34" s="136" t="s">
+      <c r="D34" s="113" t="s">
         <v>318</v>
       </c>
-      <c r="E34" s="136" t="s">
+      <c r="E34" s="113" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="86"/>
-      <c r="B35" s="136"/>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="136"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="86" t="str">
         <f>"College+"</f>
         <v>College+</v>
       </c>
-      <c r="B36" s="136" t="s">
+      <c r="B36" s="113" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="136" t="s">
+      <c r="C36" s="113" t="s">
         <v>321</v>
       </c>
-      <c r="D36" s="136" t="s">
+      <c r="D36" s="113" t="s">
         <v>131</v>
       </c>
-      <c r="E36" s="136" t="s">
+      <c r="E36" s="113" t="s">
         <v>306</v>
       </c>
     </row>
@@ -11205,16 +12045,16 @@
         <f>""</f>
         <v/>
       </c>
-      <c r="B37" s="136" t="s">
+      <c r="B37" s="113" t="s">
         <v>322</v>
       </c>
-      <c r="C37" s="136" t="s">
+      <c r="C37" s="113" t="s">
         <v>320</v>
       </c>
-      <c r="D37" s="136" t="s">
+      <c r="D37" s="113" t="s">
         <v>320</v>
       </c>
-      <c r="E37" s="136" t="s">
+      <c r="E37" s="113" t="s">
         <v>318</v>
       </c>
     </row>
@@ -11226,19 +12066,19 @@
       <c r="E38" s="86"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A39" s="138" t="s">
+      <c r="A39" s="115" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="138" t="s">
+      <c r="B39" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="138" t="s">
+      <c r="C39" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="138" t="s">
+      <c r="D39" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="138" t="s">
+      <c r="E39" s="115" t="s">
         <v>2</v>
       </c>
     </row>
@@ -11277,32 +12117,32 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="139" t="str">
+      <c r="A42" s="116" t="str">
         <f>"Observations"</f>
         <v>Observations</v>
       </c>
-      <c r="B42" s="140">
+      <c r="B42" s="117">
         <v>14376</v>
       </c>
-      <c r="C42" s="140">
+      <c r="C42" s="117">
         <v>14376</v>
       </c>
-      <c r="D42" s="140">
+      <c r="D42" s="117">
         <v>14376</v>
       </c>
-      <c r="E42" s="140">
+      <c r="E42" s="117">
         <v>14376</v>
       </c>
-      <c r="F42" s="131"/>
+      <c r="F42" s="109"/>
     </row>
     <row r="43" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="141" t="s">
+      <c r="A43" s="127" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="141"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="141"/>
-      <c r="E43" s="141"/>
+      <c r="B43" s="127"/>
+      <c r="C43" s="127"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="127"/>
     </row>
     <row r="45" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -11319,6 +12159,71 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D030FB25-C4A7-41B5-82CD-581347FF46BF}">
+  <dimension ref="A3:A13"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="53.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="37" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11EAE855-2047-4291-BF60-109D5E6A6769}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -11633,7 +12538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FC4A17-C099-4E4B-9183-D165FAAEB730}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
@@ -11670,36 +12575,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="130" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="112"/>
-      <c r="R3" s="112"/>
-      <c r="S3" s="112"/>
-      <c r="T3" s="112"/>
-      <c r="U3" s="112"/>
-      <c r="V3" s="112"/>
-      <c r="W3" s="112"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="112"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="130"/>
+      <c r="W3" s="130"/>
+      <c r="X3" s="130"/>
+      <c r="Y3" s="130"/>
+      <c r="Z3" s="130"/>
+      <c r="AA3" s="130"/>
+      <c r="AB3" s="130"/>
       <c r="AC3" s="29"/>
     </row>
     <row r="4" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -12230,822 +13135,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F3C55B-20D0-4D01-AB90-788A157F68F3}">
-  <dimension ref="A1:R22"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
-        <v>132</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2" s="59">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B4" s="115" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="116" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="114" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="114"/>
-      <c r="R4" s="114"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B5" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="M5" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="R5" s="33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="18">
-        <v>1</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="18">
-        <v>0.52429999999999999</v>
-      </c>
-      <c r="C7" s="18">
-        <v>1</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="18">
-        <v>0.50409999999999999</v>
-      </c>
-      <c r="C8" s="18">
-        <v>0.75739999999999996</v>
-      </c>
-      <c r="D8" s="18">
-        <v>1</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="18">
-        <v>-0.10829999999999999</v>
-      </c>
-      <c r="C9" s="18">
-        <v>-9.69E-2</v>
-      </c>
-      <c r="D9" s="18">
-        <v>-2.7699999999999999E-2</v>
-      </c>
-      <c r="E9" s="18">
-        <v>1</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A10" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="18">
-        <v>-8.0999999999999996E-3</v>
-      </c>
-      <c r="C10" s="18">
-        <v>-8.8999999999999999E-3</v>
-      </c>
-      <c r="D10" s="18">
-        <v>3.1399999999999997E-2</v>
-      </c>
-      <c r="E10" s="18">
-        <v>0.2596</v>
-      </c>
-      <c r="F10" s="18">
-        <v>1</v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="18">
-        <v>-1.83E-2</v>
-      </c>
-      <c r="C11" s="18">
-        <v>-5.3600000000000002E-2</v>
-      </c>
-      <c r="D11" s="18">
-        <v>-4.8999999999999998E-3</v>
-      </c>
-      <c r="E11" s="18">
-        <v>0.29580000000000001</v>
-      </c>
-      <c r="F11" s="18">
-        <v>0.64780000000000004</v>
-      </c>
-      <c r="G11" s="18">
-        <v>1</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A12" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="18">
-        <v>-0.16220000000000001</v>
-      </c>
-      <c r="C12" s="18">
-        <v>-0.20030000000000001</v>
-      </c>
-      <c r="D12" s="18">
-        <v>-0.1011</v>
-      </c>
-      <c r="E12" s="18">
-        <v>0.28599999999999998</v>
-      </c>
-      <c r="F12" s="18">
-        <v>0.2651</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0.27389999999999998</v>
-      </c>
-      <c r="H12" s="18">
-        <v>1</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="18">
-        <v>-0.12180000000000001</v>
-      </c>
-      <c r="C13" s="18">
-        <v>-0.14349999999999999</v>
-      </c>
-      <c r="D13" s="18">
-        <v>-4.7600000000000003E-2</v>
-      </c>
-      <c r="E13" s="18">
-        <v>0.37580000000000002</v>
-      </c>
-      <c r="F13" s="18">
-        <v>0.31369999999999998</v>
-      </c>
-      <c r="G13" s="18">
-        <v>0.33760000000000001</v>
-      </c>
-      <c r="H13" s="18">
-        <v>0.59350000000000003</v>
-      </c>
-      <c r="I13" s="18">
-        <v>1</v>
-      </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="18">
-        <v>2.93E-2</v>
-      </c>
-      <c r="C14" s="18">
-        <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="D14" s="18">
-        <v>7.3400000000000007E-2</v>
-      </c>
-      <c r="E14" s="18">
-        <v>0.31819999999999998</v>
-      </c>
-      <c r="F14" s="18">
-        <v>0.42980000000000002</v>
-      </c>
-      <c r="G14" s="18">
-        <v>0.40849999999999997</v>
-      </c>
-      <c r="H14" s="18">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="I14" s="18">
-        <v>0.47870000000000001</v>
-      </c>
-      <c r="J14" s="18">
-        <v>1</v>
-      </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="18"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B15" s="18">
-        <v>-0.1754</v>
-      </c>
-      <c r="C15" s="18">
-        <v>-0.1913</v>
-      </c>
-      <c r="D15" s="18">
-        <v>-0.1711</v>
-      </c>
-      <c r="E15" s="18">
-        <v>8.8499999999999995E-2</v>
-      </c>
-      <c r="F15" s="18">
-        <v>-1.03E-2</v>
-      </c>
-      <c r="G15" s="18">
-        <v>2.4799999999999999E-2</v>
-      </c>
-      <c r="H15" s="18">
-        <v>0.21290000000000001</v>
-      </c>
-      <c r="I15" s="18">
-        <v>0.1653</v>
-      </c>
-      <c r="J15" s="18">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="K15" s="18">
-        <v>1</v>
-      </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="18">
-        <v>6.3E-2</v>
-      </c>
-      <c r="C16" s="18">
-        <v>3.8699999999999998E-2</v>
-      </c>
-      <c r="D16" s="18">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="E16" s="18">
-        <v>0.13289999999999999</v>
-      </c>
-      <c r="F16" s="18">
-        <v>-5.5999999999999999E-3</v>
-      </c>
-      <c r="G16" s="18">
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="H16" s="18">
-        <v>8.1600000000000006E-2</v>
-      </c>
-      <c r="I16" s="18">
-        <v>0.1512</v>
-      </c>
-      <c r="J16" s="18">
-        <v>8.6800000000000002E-2</v>
-      </c>
-      <c r="K16" s="18">
-        <v>4.5699999999999998E-2</v>
-      </c>
-      <c r="L16" s="18">
-        <v>1</v>
-      </c>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A17" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="18">
-        <v>-3.5099999999999999E-2</v>
-      </c>
-      <c r="C17" s="18">
-        <v>-0.1091</v>
-      </c>
-      <c r="D17" s="18">
-        <v>-5.5199999999999999E-2</v>
-      </c>
-      <c r="E17" s="18">
-        <v>0.27060000000000001</v>
-      </c>
-      <c r="F17" s="18">
-        <v>0.15260000000000001</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0.20039999999999999</v>
-      </c>
-      <c r="H17" s="18">
-        <v>0.29630000000000001</v>
-      </c>
-      <c r="I17" s="18">
-        <v>0.31830000000000003</v>
-      </c>
-      <c r="J17" s="18">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0.30869999999999997</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0.22389999999999999</v>
-      </c>
-      <c r="M17" s="18">
-        <v>1</v>
-      </c>
-      <c r="N17" s="18"/>
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A18" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B18" s="18">
-        <v>-6.2399999999999997E-2</v>
-      </c>
-      <c r="C18" s="18">
-        <v>-0.11509999999999999</v>
-      </c>
-      <c r="D18" s="18">
-        <v>-3.7199999999999997E-2</v>
-      </c>
-      <c r="E18" s="18">
-        <v>0.2878</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0.14480000000000001</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0.21129999999999999</v>
-      </c>
-      <c r="H18" s="18">
-        <v>0.36470000000000002</v>
-      </c>
-      <c r="I18" s="18">
-        <v>0.3967</v>
-      </c>
-      <c r="J18" s="18">
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0.155</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0.24640000000000001</v>
-      </c>
-      <c r="M18" s="18">
-        <v>0.34210000000000002</v>
-      </c>
-      <c r="N18" s="18">
-        <v>1</v>
-      </c>
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="18">
-        <v>-0.13139999999999999</v>
-      </c>
-      <c r="C19" s="18">
-        <v>-0.22650000000000001</v>
-      </c>
-      <c r="D19" s="18">
-        <v>-0.14960000000000001</v>
-      </c>
-      <c r="E19" s="18">
-        <v>0.26150000000000001</v>
-      </c>
-      <c r="F19" s="18">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0.30520000000000003</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0.51729999999999998</v>
-      </c>
-      <c r="I19" s="18">
-        <v>0.43730000000000002</v>
-      </c>
-      <c r="J19" s="18">
-        <v>0.32490000000000002</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0.161</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0.1009</v>
-      </c>
-      <c r="M19" s="18">
-        <v>0.29409999999999997</v>
-      </c>
-      <c r="N19" s="18">
-        <v>0.377</v>
-      </c>
-      <c r="O19" s="18">
-        <v>1</v>
-      </c>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A20" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="18">
-        <v>-5.2900000000000003E-2</v>
-      </c>
-      <c r="C20" s="18">
-        <v>-0.14449999999999999</v>
-      </c>
-      <c r="D20" s="18">
-        <v>-8.3400000000000002E-2</v>
-      </c>
-      <c r="E20" s="18">
-        <v>0.2676</v>
-      </c>
-      <c r="F20" s="18">
-        <v>0.27789999999999998</v>
-      </c>
-      <c r="G20" s="18">
-        <v>0.34379999999999999</v>
-      </c>
-      <c r="H20" s="18">
-        <v>0.43959999999999999</v>
-      </c>
-      <c r="I20" s="18">
-        <v>0.41420000000000001</v>
-      </c>
-      <c r="J20" s="18">
-        <v>0.36280000000000001</v>
-      </c>
-      <c r="K20" s="18">
-        <v>0.13109999999999999</v>
-      </c>
-      <c r="L20" s="18">
-        <v>9.8599999999999993E-2</v>
-      </c>
-      <c r="M20" s="18">
-        <v>0.2853</v>
-      </c>
-      <c r="N20" s="18">
-        <v>0.3533</v>
-      </c>
-      <c r="O20" s="18">
-        <v>0.66120000000000001</v>
-      </c>
-      <c r="P20" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="18">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="C21" s="18">
-        <v>-0.11020000000000001</v>
-      </c>
-      <c r="D21" s="18">
-        <v>-8.5199999999999998E-2</v>
-      </c>
-      <c r="E21" s="18">
-        <v>7.0599999999999996E-2</v>
-      </c>
-      <c r="F21" s="18">
-        <v>0.1187</v>
-      </c>
-      <c r="G21" s="18">
-        <v>0.15359999999999999</v>
-      </c>
-      <c r="H21" s="18">
-        <v>0.29730000000000001</v>
-      </c>
-      <c r="I21" s="18">
-        <v>0.24579999999999999</v>
-      </c>
-      <c r="J21" s="18">
-        <v>0.19950000000000001</v>
-      </c>
-      <c r="K21" s="18">
-        <v>8.4099999999999994E-2</v>
-      </c>
-      <c r="L21" s="18">
-        <v>5.96E-2</v>
-      </c>
-      <c r="M21" s="18">
-        <v>0.16930000000000001</v>
-      </c>
-      <c r="N21" s="18">
-        <v>0.21110000000000001</v>
-      </c>
-      <c r="O21" s="18">
-        <v>0.37980000000000003</v>
-      </c>
-      <c r="P21" s="18">
-        <v>0.34660000000000002</v>
-      </c>
-      <c r="Q21" s="18">
-        <v>1</v>
-      </c>
-      <c r="R21" s="18"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A22" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="B22" s="18">
-        <v>1.2699999999999999E-2</v>
-      </c>
-      <c r="C22" s="18">
-        <v>-0.1246</v>
-      </c>
-      <c r="D22" s="18">
-        <v>-6.25E-2</v>
-      </c>
-      <c r="E22" s="18">
-        <v>0.2135</v>
-      </c>
-      <c r="F22" s="18">
-        <v>0.24510000000000001</v>
-      </c>
-      <c r="G22" s="18">
-        <v>0.30840000000000001</v>
-      </c>
-      <c r="H22" s="18">
-        <v>0.43159999999999998</v>
-      </c>
-      <c r="I22" s="18">
-        <v>0.45639999999999997</v>
-      </c>
-      <c r="J22" s="18">
-        <v>0.35649999999999998</v>
-      </c>
-      <c r="K22" s="18">
-        <v>0.15709999999999999</v>
-      </c>
-      <c r="L22" s="18">
-        <v>0.14729999999999999</v>
-      </c>
-      <c r="M22" s="18">
-        <v>0.31590000000000001</v>
-      </c>
-      <c r="N22" s="18">
-        <v>0.39829999999999999</v>
-      </c>
-      <c r="O22" s="18">
-        <v>0.50249999999999995</v>
-      </c>
-      <c r="P22" s="18">
-        <v>0.52749999999999997</v>
-      </c>
-      <c r="Q22" s="18">
-        <v>0.4093</v>
-      </c>
-      <c r="R22" s="18">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="O4:R4"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:J4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B6:R22">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Estimated the employment equation@
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_8_12.xlsx
+++ b/results/tables/final_tables_8_12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36A2CE7-421F-4088-B051-69B093979988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A356B3-734A-4F43-82A0-A221D1D0705B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9970" yWindow="21560" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-9970" yWindow="21560" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="8" activeTab="11" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="330">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -2636,7 +2636,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="L15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="L21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
@@ -4817,10 +4817,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CDE4BF-04E3-4DB6-8565-428D8409454E}">
-  <dimension ref="A2:W96"/>
+  <dimension ref="A2:W105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H86" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T93" sqref="T93"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H90" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6797,19 +6797,154 @@
         <v>0.581108921481442</v>
       </c>
     </row>
+    <row r="98" spans="13:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="99" spans="13:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M99" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N99" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O99" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="P99" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q99" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M100" t="s">
+        <v>81</v>
+      </c>
+      <c r="N100" s="9">
+        <v>0.55384109999999998</v>
+      </c>
+      <c r="O100" s="9">
+        <v>0.58211440000000003</v>
+      </c>
+      <c r="P100" s="9">
+        <v>0.59987069999999998</v>
+      </c>
+      <c r="Q100" s="9">
+        <v>0.43165809999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M101" t="s">
+        <v>9</v>
+      </c>
+      <c r="N101" s="9">
+        <v>0.51524199999999998</v>
+      </c>
+      <c r="O101" s="9">
+        <v>0.64602979999999999</v>
+      </c>
+      <c r="P101" s="9">
+        <v>0.65346740000000003</v>
+      </c>
+      <c r="Q101" s="9">
+        <v>0.52963939999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="M102" t="s">
+        <v>10</v>
+      </c>
+      <c r="N102" s="9">
+        <v>0.35336450000000003</v>
+      </c>
+      <c r="O102" s="9">
+        <v>0.74509349999999996</v>
+      </c>
+      <c r="P102" s="9">
+        <v>0.725553</v>
+      </c>
+      <c r="Q102" s="9">
+        <v>0.64033879999999999</v>
+      </c>
+    </row>
+    <row r="103" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="N103">
+        <f>+N100*N91</f>
+        <v>0.55384109999999998</v>
+      </c>
+      <c r="O103">
+        <f t="shared" ref="O103:Q105" si="57">+O100*O91</f>
+        <v>0.65815331564818547</v>
+      </c>
+      <c r="P103">
+        <f t="shared" si="57"/>
+        <v>0.68193287803987679</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="57"/>
+        <v>0.58640291835306013</v>
+      </c>
+      <c r="R103">
+        <f>+SUM(N103:Q103)</f>
+        <v>2.4803302120411224</v>
+      </c>
+    </row>
+    <row r="104" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="N104">
+        <f>+N101*N93</f>
+        <v>0.51524199999999998</v>
+      </c>
+      <c r="O104">
+        <f t="shared" ref="O104:Q104" si="58">+O101*O93</f>
+        <v>0.70182866334936722</v>
+      </c>
+      <c r="P104">
+        <f t="shared" si="58"/>
+        <v>0.71893860049834568</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="58"/>
+        <v>0.68694825467742315</v>
+      </c>
+      <c r="R104">
+        <f>+SUM(N104:Q104)</f>
+        <v>2.6229575185251361</v>
+      </c>
+    </row>
+    <row r="105" spans="13:18" x14ac:dyDescent="0.35">
+      <c r="N105">
+        <f>+N102*N95</f>
+        <v>0.35336450000000003</v>
+      </c>
+      <c r="O105">
+        <f t="shared" ref="O105:Q105" si="59">+O102*O95</f>
+        <v>0.740290480616972</v>
+      </c>
+      <c r="P105">
+        <f t="shared" si="59"/>
+        <v>0.72684011758390232</v>
+      </c>
+      <c r="Q105">
+        <f t="shared" si="59"/>
+        <v>0.74735216045734643</v>
+      </c>
+      <c r="R105">
+        <f t="shared" ref="R104:R105" si="60">+SUM(N105:Q105)</f>
+        <v>2.5678472586582206</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K55:S55"/>
-    <mergeCell ref="K88:S88"/>
-    <mergeCell ref="K76:S76"/>
-    <mergeCell ref="A31:I31"/>
-    <mergeCell ref="K31:S31"/>
     <mergeCell ref="A9:I9"/>
     <mergeCell ref="K9:S9"/>
     <mergeCell ref="A11:I11"/>
     <mergeCell ref="K11:S11"/>
     <mergeCell ref="A21:I21"/>
     <mergeCell ref="K21:S21"/>
+    <mergeCell ref="K55:S55"/>
+    <mergeCell ref="K88:S88"/>
+    <mergeCell ref="K76:S76"/>
+    <mergeCell ref="A31:I31"/>
+    <mergeCell ref="K31:S31"/>
     <mergeCell ref="K65:S65"/>
     <mergeCell ref="A65:I65"/>
     <mergeCell ref="A42:I42"/>
@@ -6829,7 +6964,7 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -11174,8 +11309,8 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:D61"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>